<commit_message>
fixed minor tpyo in HUE
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -488,9 +488,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -512,11 +509,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -534,96 +534,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1022,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1701,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1731,11 +1641,11 @@
       <c r="J1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="6" t="s">
         <v>56</v>
       </c>
@@ -2593,26 +2503,26 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="lessThan">
       <formula>$H3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I16">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
       <formula>$H4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2624,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2651,11 +2561,11 @@
       <c r="J1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="6" t="s">
         <v>56</v>
       </c>
@@ -2805,31 +2715,31 @@
       </c>
       <c r="I4" s="8">
         <f>VLOOKUP(MAX(M4:O4),vorlesung!A5:B34,2,TRUE)</f>
-        <v>42668</v>
+        <v>42669</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P4" t="str">
         <f>VLOOKUP(M4,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch2, Zahldarstellung</v>
+        <v>Ch 3, Animation von Programmen</v>
       </c>
       <c r="Q4" t="str">
         <f>VLOOKUP(N4,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 3, Animation von Programmen</v>
+        <v>Ch 4: Namenkonvention für Funktionsnamen</v>
       </c>
       <c r="R4" t="str">
         <f>VLOOKUP(O4,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 4: Namenkonvention für Funktionsnamen</v>
+        <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -2862,24 +2772,24 @@
       </c>
       <c r="I5" s="8">
         <f>VLOOKUP(MAX(M5:O5),vorlesung!A6:B35,2,TRUE)</f>
-        <v>42676</v>
+        <v>42682</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P5" t="str">
         <f>VLOOKUP(M5,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 4: Pass-by-assignment</v>
+        <v>Ch 5, Slicing, Länge</v>
       </c>
       <c r="Q5" t="str">
         <f>VLOOKUP(N5,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 5, Slicing, Länge</v>
+        <v>Ch 5: dicts, Operationen darauf</v>
       </c>
       <c r="R5" t="e">
         <f>VLOOKUP(O5,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -2916,31 +2826,31 @@
       </c>
       <c r="I6" s="8">
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A7:B36,2,TRUE)</f>
-        <v>42689</v>
+        <v>42690</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P6" t="str">
         <f>VLOOKUP(M6,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 5: dicts, Operationen darauf</v>
+        <v>Ch 6: Eindeutigkeit von else</v>
       </c>
       <c r="Q6" t="str">
         <f>VLOOKUP(N6,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 6: Eindeutigkeit von else</v>
+        <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
       <c r="R6" t="str">
         <f>VLOOKUP(O6,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 6: Schleifenvariable nach Schleifenende</v>
+        <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -2979,18 +2889,18 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P7" t="str">
         <f>VLOOKUP(M7,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 6: Mischen mit Slicing</v>
+        <v>Ch 7: globale Variabeln; Scopes</v>
       </c>
       <c r="Q7" t="str">
         <f>VLOOKUP(N7,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 7: globale Variabeln; Scopes</v>
+        <v>Ch 8: Daten und Funktionen</v>
       </c>
       <c r="R7" t="e">
         <f>VLOOKUP(O7,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3027,31 +2937,31 @@
       </c>
       <c r="I8" s="8">
         <f>VLOOKUP(MAX(M8:O8),vorlesung!A9:B38,2,TRUE)</f>
-        <v>42697</v>
+        <v>42703</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P8" t="str">
         <f>VLOOKUP(M8,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 8: Daten und Funktionen</v>
+        <v>Ch 8: Aufruf, Kurzschreibweise</v>
       </c>
       <c r="Q8" t="str">
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 8: Aufruf, Kurzschreibweise</v>
+        <v>Ch 8: Stack, Code</v>
       </c>
       <c r="R8" t="str">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 8: Stack, Code</v>
+        <v xml:space="preserve">Ch 9: Klassifkation, Gemeinsamkeiten </v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -3084,24 +2994,24 @@
       </c>
       <c r="I9" s="8">
         <f>VLOOKUP(MAX(M9:O9),vorlesung!A10:B39,2,TRUE)</f>
-        <v>42704</v>
+        <v>42710</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v xml:space="preserve">Ch 9: Klassifkation, Gemeinsamkeiten </v>
+        <v>Ch 9: Vernschaulichung von isinstance</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 9: Vernschaulichung von isinstance</v>
+        <v>Ende Kapitel 9</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3138,31 +3048,31 @@
       </c>
       <c r="I10" s="8">
         <f>VLOOKUP(MAX(M10:O10),vorlesung!A11:B40,2,TRUE)</f>
-        <v>42717</v>
+        <v>42724</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P10" t="str">
         <f>VLOOKUP(M10,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ende Kapitel 9</v>
+        <v>Ch 10, Geschachtelte try</v>
       </c>
       <c r="Q10" t="str">
         <f>VLOOKUP(N10,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 10, Geschachtelte try</v>
+        <v>Ch 11, LEGB</v>
       </c>
       <c r="R10" t="str">
         <f>VLOOKUP(O10,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 11, LEGB</v>
+        <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -3195,24 +3105,24 @@
       </c>
       <c r="I11" s="8">
         <f>VLOOKUP(MAX(M11:O11),vorlesung!A12:B41,2,TRUE)</f>
-        <v>42725</v>
+        <v>42745</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P11" t="str">
         <f>VLOOKUP(M11,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 11: Eingerahmte Ausgabe</v>
+        <v xml:space="preserve">Ch 12: MRO (vor Linearisierung) </v>
       </c>
       <c r="Q11" t="str">
         <f>VLOOKUP(N11,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v xml:space="preserve">Ch 12: MRO (vor Linearisierung) </v>
+        <v>Ch 12: Dependency injection</v>
       </c>
       <c r="R11" t="e">
         <f>VLOOKUP(O11,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3249,24 +3159,24 @@
       </c>
       <c r="I12" s="8">
         <f>VLOOKUP(MAX(M12:O12),vorlesung!A13:B42,2,TRUE)</f>
-        <v>42746</v>
+        <v>42752</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P12" t="str">
         <f>VLOOKUP(M12,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 12: Dependency injection</v>
+        <v>Cg 14: Virtualenv</v>
       </c>
       <c r="Q12" t="str">
         <f>VLOOKUP(N12,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Cg 14: Virtualenv</v>
+        <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
       <c r="R12" t="e">
         <f>VLOOKUP(O12,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3303,24 +3213,24 @@
       </c>
       <c r="I13" s="8">
         <f>VLOOKUP(MAX(M13:O13),vorlesung!A14:B43,2,TRUE)</f>
-        <v>42753</v>
+        <v>42759</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P13" t="str">
         <f>VLOOKUP(M13,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 14: Compiler vs. Interpreter</v>
+        <v>Ch 16, Kommentare</v>
       </c>
       <c r="Q13" t="str">
         <f>VLOOKUP(N13,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 16, Kommentare</v>
+        <v>Ch 16: Klassische for, Multiplikation</v>
       </c>
       <c r="R13" t="e">
         <f>VLOOKUP(O13,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3357,24 +3267,24 @@
       </c>
       <c r="I14" s="8">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A15:B44,2,TRUE)</f>
-        <v>42760</v>
+        <v>42766</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N14">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P14" t="str">
         <f>VLOOKUP(M14,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 16: Klassische for, Multiplikation</v>
+        <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
       <c r="Q14" t="str">
         <f>VLOOKUP(N14,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 17: Zuweisungskompatibilität</v>
+        <v>Ch 17: interfaces</v>
       </c>
       <c r="R14" t="e">
         <f>VLOOKUP(O14,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3417,18 +3327,15 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15">
-        <v>29</v>
-      </c>
-      <c r="N15">
         <v>30</v>
       </c>
       <c r="P15" t="str">
         <f>VLOOKUP(M15,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 17: interfaces</v>
-      </c>
-      <c r="Q15" t="str">
+        <v>Ch 18 Ende!</v>
+      </c>
+      <c r="Q15" t="e">
         <f>VLOOKUP(N15,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 18 Ende!</v>
+        <v>#N/A</v>
       </c>
       <c r="R15" t="e">
         <f>VLOOKUP(O15,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3452,26 +3359,26 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I15">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>$G4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3493,88 +3400,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>4</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>8</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="22">
         <v>2</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="21">
+      <c r="J3" s="20">
         <f>SUMPRODUCT(D3:G3,D4:G4)</f>
         <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>14</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>28</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>13</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <f>SUM(D7:D14)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="10"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3586,25 +3493,25 @@
       <c r="C6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <v>0</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>14</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>13</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <v>0</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3618,23 +3525,23 @@
       <c r="C7" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="23">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="22">
         <f>SUMPRODUCT(D$3:G$3,D7:G7)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$6:M$6)/3</f>
         <v>39.333333333333336</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3646,23 +3553,23 @@
       <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="23">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="22">
         <f t="shared" ref="H8:H14" si="0">SUMPRODUCT(D$3:G$3,D8:G8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$6:M$6)/3</f>
         <v>39.333333333333336</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3674,23 +3581,23 @@
       <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="23">
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$6:M$6)/3</f>
         <v>39.333333333333336</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -3702,25 +3609,25 @@
       <c r="C10" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>1</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="23">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$15:M$15)/4</f>
         <v>30.5</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -3732,23 +3639,23 @@
       <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="23">
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$15:M$15)/4/2</f>
         <v>15.25</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -3760,23 +3667,23 @@
       <c r="C12" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="23">
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$15:M$15)/4/2</f>
         <v>15.25</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -3788,23 +3695,23 @@
       <c r="C13" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="23">
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$15:M$15)/4</f>
         <v>30.5</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3816,51 +3723,51 @@
       <c r="C14" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="23">
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="23">
         <f>SUMPRODUCT(D$3:G$3,J$15:M$15)/4</f>
         <v>30.5</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <f>SUM(I7:I14)</f>
         <v>240</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="10">
         <v>14</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="10">
         <v>14</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <v>0</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="10">
         <v>26</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="10" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H7:H14">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$I7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>$I7</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
tutorien und korrigieren geteilt; vorberitung erhoeht
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -357,13 +357,19 @@
   </si>
   <si>
     <t>Wie oft im Semester?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl: </t>
+  </si>
+  <si>
+    <t>Korrigieren, ein Tutorium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +399,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -414,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -599,11 +612,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -642,9 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -672,11 +724,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -864,6 +930,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1861,11 +1967,11 @@
       <c r="J1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
@@ -2781,11 +2887,11 @@
       <c r="J1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
@@ -3608,10 +3714,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S22"/>
+  <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3623,89 +3729,95 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="D2" s="38" t="s">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="D2" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="D3" s="22">
         <v>4</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="36">
         <v>1</v>
       </c>
       <c r="F3" s="22">
         <v>8</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="36">
         <v>2</v>
       </c>
       <c r="H3" s="22">
         <v>2</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="36">
         <v>1</v>
       </c>
       <c r="J3" s="22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3" s="22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L3" s="22">
+        <v>4</v>
+      </c>
+      <c r="M3" s="22">
         <v>2</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="20"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="D4" s="21">
         <v>14</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="35">
         <v>14</v>
       </c>
       <c r="F4" s="21">
-        <v>14</v>
-      </c>
-      <c r="G4" s="36">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="G4" s="35">
+        <v>13</v>
       </c>
       <c r="H4" s="21">
         <v>14</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="35">
         <v>14</v>
       </c>
       <c r="J4" s="21">
@@ -3717,38 +3829,42 @@
       <c r="L4" s="21">
         <v>14</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="21">
+        <v>14</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="T4" s="9"/>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D5" s="21">
         <v>1</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="35">
         <v>2</v>
       </c>
       <c r="F5" s="21">
         <v>1</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>2</v>
       </c>
       <c r="H5" s="21">
         <v>1</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="35">
         <v>1</v>
       </c>
       <c r="J5" s="21">
+        <f>SUM(C6:C8)</f>
         <v>9</v>
       </c>
       <c r="K5" s="21">
@@ -3756,18 +3872,23 @@
         <v>16</v>
       </c>
       <c r="L5" s="21">
+        <f>SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="21">
+        <f>SUM(C6:C8)</f>
+        <v>9</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T5" s="9"/>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -3778,44 +3899,47 @@
         <f>COUNTIF(C$13:C$21,$B6)</f>
         <v>3</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>0</v>
       </c>
-      <c r="E6" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="28">
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27">
         <v>1</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="27">
         <v>0</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <v>1</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="27">
         <v>1</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <v>1</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="34">
         <v>2</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
+        <v>0</v>
+      </c>
+      <c r="M6" s="27">
         <v>1</v>
       </c>
-      <c r="M6" s="1">
-        <f>SUMPRODUCT(D6:L6,D$10:L$10,D$11:L$11)</f>
-        <v>264.83333333333331</v>
-      </c>
-      <c r="O6" s="9"/>
+      <c r="N6" s="1">
+        <f>SUMPRODUCT(D6:M6,D$10:M$10,D$11:M$11)</f>
+        <v>174.66666666666666</v>
+      </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T6" s="9"/>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>80</v>
       </c>
@@ -3823,44 +3947,47 @@
         <f>COUNTIF(C$13:C$21,$B7)</f>
         <v>4</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>1</v>
       </c>
-      <c r="E7" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="28">
+      <c r="E7" s="27">
+        <v>1</v>
+      </c>
+      <c r="F7" s="27">
         <v>0</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="27">
         <v>1</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="27">
         <v>0</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="27">
         <v>1</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="27">
         <v>2</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
+        <v>2</v>
+      </c>
+      <c r="M7" s="27">
         <v>1</v>
       </c>
-      <c r="M7" s="1">
-        <f t="shared" ref="M7:M8" si="0">SUMPRODUCT(D7:L7,D$10:L$10,D$11:L$11)</f>
-        <v>235.9</v>
-      </c>
-      <c r="O7" s="9"/>
+      <c r="N7" s="1">
+        <f>SUMPRODUCT(D7:M7,D$10:M$10,D$11:M$11)</f>
+        <v>254</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-    </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T7" s="9"/>
+    </row>
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>91</v>
       </c>
@@ -3868,192 +3995,208 @@
         <f>COUNTIF(C$13:C$21,$B8)</f>
         <v>2</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <f>D7*0.5</f>
         <v>0.5</v>
       </c>
-      <c r="E8" s="28">
-        <f t="shared" ref="E8:K8" si="1">E7*0.5</f>
-        <v>0.25</v>
-      </c>
-      <c r="F8" s="28">
-        <f t="shared" si="1"/>
+      <c r="E8" s="27">
+        <f t="shared" ref="E8:K8" si="0">E7*0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="28">
-        <f t="shared" si="1"/>
+      <c r="G8" s="27">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H8" s="28">
-        <f t="shared" si="1"/>
+      <c r="H8" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="28">
-        <f t="shared" si="1"/>
+      <c r="I8" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="27">
         <v>1</v>
       </c>
-      <c r="K8" s="28">
-        <f t="shared" si="1"/>
+      <c r="K8" s="27">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <v>1</v>
       </c>
-      <c r="M8" s="1">
-        <f t="shared" si="0"/>
-        <v>138.94999999999999</v>
-      </c>
-      <c r="O8" s="9"/>
+      <c r="M8" s="27">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <f>SUMPRODUCT(D8:M8,D$10:M$10,D$11:M$11)</f>
+        <v>162</v>
+      </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="T8" s="9"/>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="28">
+      <c r="C9" s="45"/>
+      <c r="D9" s="46">
         <f>SUMPRODUCT($C6:$C8,D6:D8)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="28">
-        <f t="shared" ref="E9:L9" si="2">SUMPRODUCT($C6:$C8,E6:E8)</f>
-        <v>4</v>
-      </c>
-      <c r="F9" s="28">
-        <f t="shared" si="2"/>
+      <c r="E9" s="46">
+        <f t="shared" ref="E9:M9" si="1">SUMPRODUCT($C6:$C8,E6:E8)</f>
+        <v>5</v>
+      </c>
+      <c r="F9" s="46">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G9" s="28">
-        <f t="shared" si="2"/>
+      <c r="G9" s="46">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H9" s="28">
-        <f t="shared" si="2"/>
+      <c r="H9" s="46">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I9" s="28">
-        <f t="shared" si="2"/>
+      <c r="I9" s="46">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J9" s="28">
-        <f t="shared" si="2"/>
+      <c r="J9" s="46">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K9" s="28">
-        <f t="shared" si="2"/>
+      <c r="K9" s="46">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L9" s="28">
-        <f t="shared" si="2"/>
+      <c r="L9" s="46">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M9" s="46">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="M9" s="1">
-        <f>SUMPRODUCT(M6:M8,C6:C8)</f>
-        <v>2016</v>
-      </c>
-      <c r="O9" s="9"/>
+      <c r="N9" s="1">
+        <f>SUMPRODUCT(N6:N8,C6:C8)</f>
+        <v>1864</v>
+      </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" s="20" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T9" s="9"/>
+    </row>
+    <row r="10" spans="1:20" s="20" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <f>1/D9</f>
         <v>0.2</v>
       </c>
-      <c r="E10" s="29">
-        <f t="shared" ref="E10:L10" si="3">1/E9</f>
-        <v>0.25</v>
-      </c>
-      <c r="F10" s="29">
-        <f t="shared" si="3"/>
+      <c r="E10" s="28">
+        <f t="shared" ref="E10:M10" si="2">1/E9</f>
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="28">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G10" s="29">
-        <f t="shared" si="3"/>
+      <c r="G10" s="28">
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="H10" s="29">
-        <f t="shared" si="3"/>
+      <c r="H10" s="28">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I10" s="29">
-        <f t="shared" si="3"/>
+      <c r="I10" s="28">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J10" s="29">
-        <f t="shared" si="3"/>
+      <c r="J10" s="28">
+        <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="K10" s="29">
-        <f t="shared" si="3"/>
+      <c r="K10" s="28">
+        <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="L10" s="29">
-        <f t="shared" si="3"/>
+      <c r="L10" s="28">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="28">
+        <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <f>D3*D4*D5</f>
         <v>56</v>
       </c>
-      <c r="E11" s="28">
-        <f t="shared" ref="E11:L11" si="4">E3*E4*E5</f>
+      <c r="E11" s="27">
+        <f t="shared" ref="E11:M11" si="3">E3*E4*E5</f>
         <v>28</v>
       </c>
-      <c r="F11" s="28">
-        <f t="shared" si="4"/>
-        <v>112</v>
-      </c>
-      <c r="G11" s="28">
-        <f t="shared" si="4"/>
-        <v>56</v>
-      </c>
-      <c r="H11" s="28">
-        <f t="shared" si="4"/>
+      <c r="F11" s="27">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="G11" s="27">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="I11" s="28">
-        <f t="shared" si="4"/>
+      <c r="I11" s="27">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J11" s="28">
-        <f t="shared" si="4"/>
-        <v>126</v>
-      </c>
-      <c r="K11" s="28">
-        <f t="shared" si="4"/>
-        <v>1344</v>
-      </c>
-      <c r="L11" s="28">
-        <f t="shared" si="4"/>
+      <c r="J11" s="27">
+        <f t="shared" si="3"/>
+        <v>378</v>
+      </c>
+      <c r="K11" s="27">
+        <f t="shared" si="3"/>
+        <v>448</v>
+      </c>
+      <c r="L11" s="27">
+        <f t="shared" si="3"/>
+        <v>504</v>
+      </c>
+      <c r="M11" s="27">
+        <f t="shared" si="3"/>
         <v>252</v>
       </c>
-      <c r="M11" s="1">
-        <f>SUM(D11:L11)</f>
-        <v>2016</v>
-      </c>
-      <c r="O11" s="9"/>
+      <c r="N11" s="1">
+        <f>SUM(D11:M11)</f>
+        <v>1864</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-    </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T11" s="9"/>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -4063,19 +4206,22 @@
       <c r="C12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="O12" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S12" s="10"/>
+      <c r="T12" s="9"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -4088,37 +4234,43 @@
       <c r="D13" s="11">
         <v>0</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12">
         <v>0</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30">
+      <c r="I13" s="29"/>
+      <c r="J13" s="29">
         <v>14</v>
       </c>
-      <c r="K13" s="30">
+      <c r="K13" s="29">
+        <f>VLOOKUP($C13,$B$6:$L$9,10,FALSE)*K$4</f>
+        <v>28</v>
+      </c>
+      <c r="L13" s="44">
+        <f>VLOOKUP($C13,$B$6:$L$9,11,FALSE)*L$4</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="13">
+        <f>VLOOKUP($C13,$B$6:$M$9,12,FALSE)*M$4</f>
         <v>14</v>
       </c>
-      <c r="L13" s="13">
-        <v>14</v>
-      </c>
-      <c r="M13" s="22">
-        <f>SUMPRODUCT(D$3:L$3,D13:L13)</f>
+      <c r="N13" s="22">
+        <f>SUMPRODUCT(D$3:M$3,D13:M13)</f>
         <v>126</v>
       </c>
-      <c r="N13" s="23">
-        <f>VLOOKUP(C13,B$6:M$8,12,FALSE)</f>
-        <v>264.83333333333331</v>
-      </c>
-      <c r="O13" s="10"/>
+      <c r="O13" s="23">
+        <f>VLOOKUP(C13,B$6:N$8,13,FALSE)</f>
+        <v>174.66666666666666</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -4131,41 +4283,47 @@
       <c r="D14" s="14">
         <v>0</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="15">
-        <v>1</v>
-      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="15">
         <v>0</v>
       </c>
       <c r="H14" s="15">
         <v>1</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31">
+      <c r="I14" s="30">
+        <v>1</v>
+      </c>
+      <c r="J14" s="30">
         <v>14</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="30">
+        <f t="shared" ref="K14:L21" si="4">VLOOKUP($C14,$B$6:$L$9,10,FALSE)*K$4</f>
+        <v>28</v>
+      </c>
+      <c r="L14" s="41">
+        <f t="shared" ref="L14:L21" si="5">VLOOKUP($C14,$B$6:$L$9,11,FALSE)*L$4</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="16">
+        <f t="shared" ref="M14:M21" si="6">VLOOKUP($C14,$B$6:$M$9,12,FALSE)*M$4</f>
         <v>14</v>
       </c>
-      <c r="L14" s="16">
-        <v>14</v>
-      </c>
-      <c r="M14" s="22">
-        <f t="shared" ref="M14:M21" si="5">SUMPRODUCT(D$3:L$3,D14:L14)</f>
-        <v>136</v>
-      </c>
-      <c r="N14" s="23">
-        <f t="shared" ref="N14:N21" si="6">VLOOKUP(C14,B$6:M$8,12,FALSE)</f>
-        <v>264.83333333333331</v>
-      </c>
-      <c r="O14" s="10"/>
+      <c r="N14" s="22">
+        <f t="shared" ref="N14:N21" si="7">SUMPRODUCT(D$3:M$3,D14:M14)</f>
+        <v>129</v>
+      </c>
+      <c r="O14" s="23">
+        <f t="shared" ref="O14:O21" si="8">VLOOKUP(C14,B$6:N$8,13,FALSE)</f>
+        <v>174.66666666666666</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -4175,40 +4333,46 @@
       <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="24">
         <v>0</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26">
+      <c r="E15" s="33"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25">
         <v>0</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34">
+      <c r="H15" s="25"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33">
         <v>14</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="33">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="L15" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="26">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="L15" s="27">
-        <v>14</v>
-      </c>
-      <c r="M15" s="22">
-        <f t="shared" si="5"/>
+      <c r="N15" s="22">
+        <f t="shared" si="7"/>
         <v>126</v>
       </c>
-      <c r="N15" s="23">
-        <f t="shared" si="6"/>
-        <v>264.83333333333331</v>
-      </c>
-      <c r="O15" s="10"/>
+      <c r="O15" s="23">
+        <f>VLOOKUP(C15,B$6:N$8,13,FALSE)</f>
+        <v>174.66666666666666</v>
+      </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -4221,7 +4385,7 @@
       <c r="D16" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="15">
         <v>0</v>
       </c>
@@ -4229,33 +4393,39 @@
       <c r="H16" s="15">
         <v>0</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="30">
         <v>0</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="30">
+        <v>14</v>
+      </c>
+      <c r="K16" s="30">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="K16" s="31">
+      <c r="L16" s="41">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="L16" s="16">
+      <c r="M16" s="16">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="M16" s="22">
-        <f t="shared" si="5"/>
-        <v>228</v>
-      </c>
-      <c r="N16" s="23">
-        <f t="shared" si="6"/>
-        <v>235.9</v>
-      </c>
-      <c r="O16" s="10"/>
+      <c r="N16" s="22">
+        <f t="shared" si="7"/>
+        <v>242</v>
+      </c>
+      <c r="O16" s="23">
+        <f t="shared" si="8"/>
+        <v>254</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -4266,7 +4436,7 @@
         <v>91</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="31"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="15">
         <v>0</v>
       </c>
@@ -4274,33 +4444,39 @@
       <c r="H17" s="15">
         <v>0</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="30">
         <v>0</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="30">
         <v>14</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="30">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="41">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="M17" s="22">
-        <f t="shared" si="5"/>
-        <v>126</v>
-      </c>
-      <c r="N17" s="23">
+      <c r="M17" s="16">
         <f t="shared" si="6"/>
-        <v>138.94999999999999</v>
-      </c>
-      <c r="O17" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="N17" s="22">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="O17" s="23">
+        <f t="shared" si="8"/>
+        <v>162</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -4311,7 +4487,7 @@
         <v>91</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="31"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="15">
         <v>0</v>
       </c>
@@ -4319,33 +4495,39 @@
       <c r="H18" s="15">
         <v>0</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="30">
         <v>0</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="30">
         <v>14</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="30">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="41">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="M18" s="22">
-        <f t="shared" si="5"/>
-        <v>126</v>
-      </c>
-      <c r="N18" s="23">
+      <c r="M18" s="16">
         <f t="shared" si="6"/>
-        <v>138.94999999999999</v>
-      </c>
-      <c r="O18" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="22">
+        <f t="shared" si="7"/>
+        <v>154</v>
+      </c>
+      <c r="O18" s="23">
+        <f t="shared" si="8"/>
+        <v>162</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -4356,41 +4538,47 @@
         <v>80</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33">
+      <c r="E19" s="30"/>
+      <c r="F19" s="32">
         <v>0</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15">
         <v>0</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="30">
         <v>0</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="30">
+        <v>14</v>
+      </c>
+      <c r="K19" s="30">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="K19" s="31">
+      <c r="L19" s="41">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="L19" s="16">
+      <c r="M19" s="16">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="M19" s="22">
-        <f t="shared" si="5"/>
-        <v>224</v>
-      </c>
-      <c r="N19" s="23">
-        <f t="shared" si="6"/>
-        <v>235.9</v>
-      </c>
-      <c r="O19" s="10"/>
+      <c r="N19" s="22">
+        <f t="shared" si="7"/>
+        <v>238</v>
+      </c>
+      <c r="O19" s="23">
+        <f t="shared" si="8"/>
+        <v>254</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -4401,41 +4589,47 @@
         <v>80</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="33">
+      <c r="E20" s="30"/>
+      <c r="F20" s="32">
         <v>0</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15">
         <v>0</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="30">
         <v>0</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="30">
+        <v>14</v>
+      </c>
+      <c r="K20" s="30">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="K20" s="31">
+      <c r="L20" s="41">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="L20" s="16">
+      <c r="M20" s="16">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="M20" s="22">
-        <f t="shared" si="5"/>
-        <v>224</v>
-      </c>
-      <c r="N20" s="23">
-        <f t="shared" si="6"/>
-        <v>235.9</v>
-      </c>
-      <c r="O20" s="10"/>
+      <c r="N20" s="22">
+        <f t="shared" si="7"/>
+        <v>238</v>
+      </c>
+      <c r="O20" s="23">
+        <f t="shared" si="8"/>
+        <v>254</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
-    </row>
-    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -4446,7 +4640,7 @@
         <v>80</v>
       </c>
       <c r="D21" s="17"/>
-      <c r="E21" s="32"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="18">
         <v>0</v>
       </c>
@@ -4454,50 +4648,111 @@
       <c r="H21" s="18">
         <v>0</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="31">
         <v>0</v>
       </c>
-      <c r="J21" s="32">
+      <c r="J21" s="31">
+        <v>14</v>
+      </c>
+      <c r="K21" s="31">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="K21" s="32">
+      <c r="L21" s="43">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="L21" s="19">
+      <c r="M21" s="19">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="M21" s="22">
-        <f t="shared" si="5"/>
-        <v>224</v>
-      </c>
-      <c r="N21" s="23">
-        <f t="shared" si="6"/>
-        <v>235.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="N21" s="22">
+        <f t="shared" si="7"/>
+        <v>238</v>
+      </c>
+      <c r="O21" s="23">
+        <f t="shared" si="8"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D22" s="40">
+        <f>D3*SUM(D13:D21)</f>
+        <v>4</v>
+      </c>
+      <c r="E22" s="40">
+        <f t="shared" ref="E22:M22" si="9">E3*SUM(E13:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="40">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="I22" s="40">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="40">
+        <f t="shared" si="9"/>
+        <v>378</v>
+      </c>
+      <c r="K22" s="40">
+        <f t="shared" si="9"/>
+        <v>448</v>
+      </c>
+      <c r="L22" s="40">
+        <f t="shared" si="9"/>
+        <v>560</v>
+      </c>
+      <c r="M22" s="40">
+        <f t="shared" si="9"/>
+        <v>252</v>
+      </c>
+      <c r="N22" s="22">
+        <f>SUM(N13:N21)</f>
+        <v>1645</v>
+      </c>
+      <c r="O22" s="22">
+        <f>SUM(O13:O21)</f>
+        <v>1864</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
-      <formula>$N13</formula>
+  <conditionalFormatting sqref="N13:N21">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>$O13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
-      <formula>$N13</formula>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>$O13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M21">
+  <conditionalFormatting sqref="N14:N22">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>$O14</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+      <formula>$O14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
-      <formula>$N14</formula>
+      <formula>$O22</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
-      <formula>$N14</formula>
+      <formula>$O22</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added AS as Drafter for first PUE
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -724,9 +724,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -738,31 +735,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -930,46 +910,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1258,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1937,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1967,11 +1907,11 @@
       <c r="J1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
@@ -2062,6 +2002,9 @@
       <c r="I3" s="8" t="e">
         <f>VLOOKUP(MAX(M3:O3),vorlesung!A$4:B$33,2,TRUE)</f>
         <v>#N/A</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -2829,26 +2772,26 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="lessThan">
       <formula>$H3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I16">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>$H4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2860,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2887,11 +2830,11 @@
       <c r="J1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
@@ -3593,7 +3536,7 @@
       </c>
       <c r="I14" s="8">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A15:B44,2,TRUE)</f>
-        <v>42766</v>
+        <v>42760</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -3601,16 +3544,13 @@
       <c r="M14">
         <v>28</v>
       </c>
-      <c r="N14">
-        <v>29</v>
-      </c>
       <c r="P14" t="str">
         <f>VLOOKUP(M14,vorlesung!$A$4:$H$33,8,FALSE)</f>
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="Q14" t="e">
         <f>VLOOKUP(N14,vorlesung!$A$4:$H$33,8,FALSE)</f>
-        <v>Ch 17: interfaces</v>
+        <v>#N/A</v>
       </c>
       <c r="R14" t="e">
         <f>VLOOKUP(O14,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -3685,26 +3625,26 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
       <formula>$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I15">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>$G4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3716,7 +3656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -4043,47 +3983,47 @@
       <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="46">
+      <c r="C9" s="44"/>
+      <c r="D9" s="45">
         <f>SUMPRODUCT($C6:$C8,D6:D8)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <f t="shared" ref="E9:M9" si="1">SUMPRODUCT($C6:$C8,E6:E8)</f>
         <v>5</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="45">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J9" s="46">
+      <c r="J9" s="45">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K9" s="46">
+      <c r="K9" s="45">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L9" s="46">
+      <c r="L9" s="45">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M9" s="46">
+      <c r="M9" s="45">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -4248,7 +4188,7 @@
         <f>VLOOKUP($C13,$B$6:$L$9,10,FALSE)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="43">
         <f>VLOOKUP($C13,$B$6:$L$9,11,FALSE)*L$4</f>
         <v>0</v>
       </c>
@@ -4298,10 +4238,10 @@
         <v>14</v>
       </c>
       <c r="K14" s="30">
-        <f t="shared" ref="K14:L21" si="4">VLOOKUP($C14,$B$6:$L$9,10,FALSE)*K$4</f>
+        <f t="shared" ref="K14:K21" si="4">VLOOKUP($C14,$B$6:$L$9,10,FALSE)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="40">
         <f t="shared" ref="L14:L21" si="5">VLOOKUP($C14,$B$6:$L$9,11,FALSE)*L$4</f>
         <v>0</v>
       </c>
@@ -4350,7 +4290,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="41">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -4403,7 +4343,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="40">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
@@ -4454,7 +4394,7 @@
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="40">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
@@ -4505,7 +4445,7 @@
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="40">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
@@ -4556,7 +4496,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="L19" s="41">
+      <c r="L19" s="40">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
@@ -4607,7 +4547,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="L20" s="41">
+      <c r="L20" s="40">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
@@ -4658,7 +4598,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="L21" s="43">
+      <c r="L21" s="42">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
@@ -4676,43 +4616,43 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D22" s="40">
+      <c r="D22" s="39">
         <f>D3*SUM(D13:D21)</f>
         <v>4</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="39">
         <f t="shared" ref="E22:M22" si="9">E3*SUM(E13:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="39">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="39">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="39">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="39">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="39">
         <f t="shared" si="9"/>
         <v>378</v>
       </c>
-      <c r="K22" s="40">
+      <c r="K22" s="39">
         <f t="shared" si="9"/>
         <v>448</v>
       </c>
-      <c r="L22" s="40">
+      <c r="L22" s="39">
         <f t="shared" si="9"/>
         <v>560</v>
       </c>
-      <c r="M22" s="40">
+      <c r="M22" s="39">
         <f t="shared" si="9"/>
         <v>252</v>
       </c>
@@ -4732,26 +4672,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N13:N21">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>$O13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
       <formula>$O13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14:N22">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>$O14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>$O14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>$O22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$O22</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Initialen eintragen, nicht namen
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/gp1-jupyter/meetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="38100" windowHeight="22860" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -363,15 +363,6 @@
   </si>
   <si>
     <t>Korrigieren, ein Tutorium</t>
-  </si>
-  <si>
-    <t>Setzer</t>
-  </si>
-  <si>
-    <t>Parruca</t>
-  </si>
-  <si>
-    <t>Feldmann</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2033,8 +2024,8 @@
         <v>75</v>
       </c>
       <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
-        <v>111</v>
+      <c r="L3" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="P3" t="e">
         <f>VLOOKUP(M3,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -2089,7 +2080,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -2146,7 +2137,7 @@
         <v>42665</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -2203,7 +2194,7 @@
         <v>42668</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -2261,7 +2252,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -2322,7 +2313,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M8">
         <v>9</v>
@@ -2380,7 +2371,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M9">
         <v>11</v>
@@ -2441,7 +2432,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M10">
         <v>14</v>
@@ -2499,7 +2490,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M11">
         <v>16</v>
@@ -2560,7 +2551,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M12">
         <v>19</v>
@@ -2618,7 +2609,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M13">
         <v>21</v>
@@ -2679,7 +2670,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M14">
         <v>24</v>
@@ -2737,7 +2728,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M15">
         <v>26</v>
@@ -2798,7 +2789,7 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M16">
         <v>29</v>
@@ -2855,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J15" sqref="J9:J15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2979,7 +2970,7 @@
         <v>42665</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3041,7 +3032,7 @@
         <v>42669</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -3100,7 +3091,7 @@
         <v>42682</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -3156,7 +3147,7 @@
         <v>42690</v>
       </c>
       <c r="J6" s="47" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3215,7 +3206,7 @@
         <v>42693</v>
       </c>
       <c r="J7" s="47" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -3271,7 +3262,7 @@
         <v>42703</v>
       </c>
       <c r="J8" s="47" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -3330,7 +3321,7 @@
         <v>42710</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -3386,7 +3377,7 @@
         <v>42724</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -3445,7 +3436,7 @@
         <v>42745</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -3501,7 +3492,7 @@
         <v>42752</v>
       </c>
       <c r="J12" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -3557,7 +3548,7 @@
         <v>42759</v>
       </c>
       <c r="J13" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -3613,7 +3604,7 @@
         <v>42760</v>
       </c>
       <c r="J14" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -3666,7 +3657,7 @@
         <v>42767</v>
       </c>
       <c r="J15" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -3734,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
automatic bookkeeping on preparing and reviewing homework assignments
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="38100" windowHeight="22860" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2846,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3725,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4241,15 +4241,29 @@
         <v>73</v>
       </c>
       <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="12"/>
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="29">
+        <f>COUNTIF(PUE!K$3:L$16,$B13)</f>
+        <v>6</v>
+      </c>
+      <c r="F13" s="12">
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B13)</f>
+        <v>5</v>
+      </c>
       <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="29"/>
+        <f>COUNTIF(HUE!K$3:$L16,Tutoren!$B13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <f>F13</f>
+        <v>5</v>
+      </c>
+      <c r="I13" s="29">
+        <f>H13</f>
+        <v>5</v>
+      </c>
       <c r="J13" s="29">
         <v>14</v>
       </c>
@@ -4267,7 +4281,7 @@
       </c>
       <c r="N13" s="22">
         <f>SUMPRODUCT(D$3:M$3,D13:M13)</f>
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="O13" s="23">
         <f>VLOOKUP(C13,B$6:N$8,13,FALSE)</f>
@@ -4290,40 +4304,50 @@
         <v>73</v>
       </c>
       <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="15"/>
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B14)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B14)</f>
+        <v>4</v>
+      </c>
+      <c r="F14" s="15">
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B14)</f>
+        <v>4</v>
+      </c>
       <c r="G14" s="15">
+        <f>COUNTIF(HUE!K$3:$L17,Tutoren!$B14)</f>
         <v>0</v>
       </c>
       <c r="H14" s="15">
-        <v>1</v>
+        <f t="shared" ref="H14:H21" si="4">F14</f>
+        <v>4</v>
       </c>
       <c r="I14" s="30">
-        <v>1</v>
+        <f t="shared" ref="I14:I21" si="5">H14</f>
+        <v>4</v>
       </c>
       <c r="J14" s="30">
         <v>14</v>
       </c>
       <c r="K14" s="30">
-        <f t="shared" ref="K14:K21" si="4">VLOOKUP($C14,$B$6:$L$9,10,FALSE)*K$4</f>
+        <f t="shared" ref="K14:K21" si="6">VLOOKUP($C14,$B$6:$L$9,10,FALSE)*K$4</f>
         <v>28</v>
       </c>
       <c r="L14" s="40">
-        <f t="shared" ref="L14:L21" si="5">VLOOKUP($C14,$B$6:$L$9,11,FALSE)*L$4</f>
+        <f t="shared" ref="L14:L21" si="7">VLOOKUP($C14,$B$6:$L$9,11,FALSE)*L$4</f>
         <v>0</v>
       </c>
       <c r="M14" s="16">
-        <f t="shared" ref="M14:M21" si="6">VLOOKUP($C14,$B$6:$M$9,12,FALSE)*M$4</f>
+        <f t="shared" ref="M14:M21" si="8">VLOOKUP($C14,$B$6:$M$9,12,FALSE)*M$4</f>
         <v>14</v>
       </c>
       <c r="N14" s="22">
-        <f t="shared" ref="N14:N21" si="7">SUMPRODUCT(D$3:M$3,D14:M14)</f>
-        <v>129</v>
+        <f t="shared" ref="N14:N21" si="9">SUMPRODUCT(D$3:M$3,D14:M14)</f>
+        <v>178</v>
       </c>
       <c r="O14" s="23">
-        <f t="shared" ref="O14:O21" si="8">VLOOKUP(C14,B$6:N$8,13,FALSE)</f>
+        <f t="shared" ref="O14:O21" si="10">VLOOKUP(C14,B$6:N$8,13,FALSE)</f>
         <v>174.66666666666666</v>
       </c>
       <c r="P14" s="10"/>
@@ -4343,33 +4367,47 @@
         <v>73</v>
       </c>
       <c r="D15" s="24">
-        <v>0</v>
-      </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="25"/>
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <f>COUNTIF(PUE!K$3:L$16,$B15)</f>
+        <v>4</v>
+      </c>
+      <c r="F15" s="25">
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B15)</f>
+        <v>4</v>
+      </c>
       <c r="G15" s="25">
-        <v>0</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="33"/>
+        <f>COUNTIF(HUE!K$3:$L18,Tutoren!$B15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="25">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="I15" s="33">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="J15" s="33">
         <v>14</v>
       </c>
       <c r="K15" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L15" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M15" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="N15" s="22">
-        <f t="shared" si="7"/>
-        <v>126</v>
+        <f t="shared" si="9"/>
+        <v>174</v>
       </c>
       <c r="O15" s="23">
         <f>VLOOKUP(C15,B$6:N$8,13,FALSE)</f>
@@ -4392,40 +4430,50 @@
         <v>80</v>
       </c>
       <c r="D16" s="14">
-        <v>1</v>
-      </c>
-      <c r="E16" s="30"/>
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B16)</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="15">
-        <v>0</v>
-      </c>
-      <c r="G16" s="15"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <f>COUNTIF(HUE!K$3:$L19,Tutoren!$B16)</f>
+        <v>0</v>
+      </c>
       <c r="H16" s="15">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I16" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J16" s="30">
         <v>14</v>
       </c>
       <c r="K16" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L16" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="M16" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="N16" s="22">
-        <f t="shared" si="7"/>
-        <v>242</v>
+        <f t="shared" si="9"/>
+        <v>238</v>
       </c>
       <c r="O16" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>254</v>
       </c>
       <c r="P16" s="10"/>
@@ -4444,39 +4492,51 @@
       <c r="C17" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="30"/>
+      <c r="D17" s="14">
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B17)</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="15">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B17)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <f>COUNTIF(HUE!K$3:$L20,Tutoren!$B17)</f>
+        <v>0</v>
+      </c>
       <c r="H17" s="15">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I17" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J17" s="30">
         <v>14</v>
       </c>
       <c r="K17" s="30">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="L17" s="40">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="M17" s="16">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
+      <c r="L17" s="40">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="M17" s="16">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
       <c r="N17" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>154</v>
       </c>
       <c r="O17" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>162</v>
       </c>
       <c r="P17" s="10"/>
@@ -4495,39 +4555,51 @@
       <c r="C18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="14">
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B18)</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="15">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B18)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <f>COUNTIF(HUE!K$3:$L21,Tutoren!$B18)</f>
+        <v>0</v>
+      </c>
       <c r="H18" s="15">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J18" s="30">
         <v>14</v>
       </c>
       <c r="K18" s="30">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="L18" s="40">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="M18" s="16">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
+      <c r="L18" s="40">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="M18" s="16">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
       <c r="N18" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>154</v>
       </c>
       <c r="O18" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>162</v>
       </c>
       <c r="P18" s="10"/>
@@ -4546,39 +4618,51 @@
       <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="14">
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B19)</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="32">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B19)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <f>COUNTIF(HUE!K$3:$L22,Tutoren!$B19)</f>
+        <v>0</v>
+      </c>
       <c r="H19" s="15">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I19" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J19" s="30">
         <v>14</v>
       </c>
       <c r="K19" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L19" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="M19" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="N19" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>238</v>
       </c>
       <c r="O19" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>254</v>
       </c>
       <c r="P19" s="10"/>
@@ -4597,39 +4681,51 @@
       <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="30"/>
+      <c r="D20" s="14">
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="30">
+        <f>COUNTIF(PUE!K$3:L$16,$B20)</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="32">
-        <v>0</v>
-      </c>
-      <c r="G20" s="15"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B20)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="15">
+        <f>COUNTIF(HUE!K$3:$L23,Tutoren!$B20)</f>
+        <v>0</v>
+      </c>
       <c r="H20" s="15">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I20" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J20" s="30">
         <v>14</v>
       </c>
       <c r="K20" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L20" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="M20" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="N20" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>238</v>
       </c>
       <c r="O20" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>254</v>
       </c>
       <c r="P20" s="10"/>
@@ -4648,39 +4744,51 @@
       <c r="C21" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="31"/>
+      <c r="D21" s="17">
+        <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B21)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="31">
+        <f>COUNTIF(PUE!K$3:L$16,$B21)</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="18">
-        <v>0</v>
-      </c>
-      <c r="G21" s="18"/>
+        <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B21)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="18">
+        <f>COUNTIF(HUE!K$3:$L24,Tutoren!$B21)</f>
+        <v>0</v>
+      </c>
       <c r="H21" s="18">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I21" s="31">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J21" s="31">
         <v>14</v>
       </c>
       <c r="K21" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L21" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="M21" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="N21" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>238</v>
       </c>
       <c r="O21" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>254</v>
       </c>
     </row>
@@ -4690,44 +4798,44 @@
         <v>4</v>
       </c>
       <c r="E22" s="39">
-        <f t="shared" ref="E22:M22" si="9">E3*SUM(E13:E21)</f>
-        <v>0</v>
+        <f t="shared" ref="E22:M22" si="11">E3*SUM(E13:E21)</f>
+        <v>14</v>
       </c>
       <c r="F22" s="39">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>104</v>
       </c>
       <c r="G22" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H22" s="39">
-        <f t="shared" si="9"/>
-        <v>2</v>
+        <f t="shared" si="11"/>
+        <v>26</v>
       </c>
       <c r="I22" s="39">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <f t="shared" si="11"/>
+        <v>13</v>
       </c>
       <c r="J22" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>378</v>
       </c>
       <c r="K22" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>448</v>
       </c>
       <c r="L22" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>560</v>
       </c>
       <c r="M22" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>252</v>
       </c>
       <c r="N22" s="22">
         <f>SUM(N13:N21)</f>
-        <v>1645</v>
+        <v>1799</v>
       </c>
       <c r="O22" s="22">
         <f>SUM(O13:O21)</f>

</xml_diff>

<commit_message>
Reviewterminen von WiMis eingetragen
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -363,15 +363,6 @@
   </si>
   <si>
     <t>Korrigieren, ein Tutorium</t>
-  </si>
-  <si>
-    <t>Setzer</t>
-  </si>
-  <si>
-    <t>Parruca</t>
-  </si>
-  <si>
-    <t>Feldmann</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,7 +2025,7 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="P3" t="e">
         <f>VLOOKUP(M3,vorlesung!$A$4:$H$33,8,FALSE)</f>
@@ -2089,7 +2080,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -2146,7 +2137,7 @@
         <v>42665</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -2203,7 +2194,7 @@
         <v>42668</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -2261,7 +2252,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -2322,7 +2313,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="M8">
         <v>9</v>
@@ -2380,7 +2371,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M9">
         <v>11</v>
@@ -2441,7 +2432,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M10">
         <v>14</v>
@@ -2499,7 +2490,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M11">
         <v>16</v>
@@ -2560,7 +2551,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="47" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="M12">
         <v>19</v>
@@ -2618,7 +2609,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M13">
         <v>21</v>
@@ -2679,7 +2670,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M14">
         <v>24</v>
@@ -2737,7 +2728,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="47" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="M15">
         <v>26</v>
@@ -2797,8 +2788,8 @@
         <v>42767</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>111</v>
+      <c r="L16" s="47" t="s">
+        <v>75</v>
       </c>
       <c r="M16">
         <v>29</v>
@@ -2855,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J15" sqref="J9:J15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2979,10 +2970,14 @@
         <v>42665</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="M3">
         <v>1</v>
       </c>
@@ -3041,10 +3036,14 @@
         <v>42669</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="M4">
         <v>4</v>
       </c>
@@ -3100,10 +3099,14 @@
         <v>42682</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="M5">
         <v>7</v>
       </c>
@@ -3156,10 +3159,14 @@
         <v>42690</v>
       </c>
       <c r="J6" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="M6">
         <v>9</v>
       </c>
@@ -3215,10 +3222,14 @@
         <v>42693</v>
       </c>
       <c r="J7" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="M7">
         <v>12</v>
       </c>
@@ -3271,10 +3282,14 @@
         <v>42703</v>
       </c>
       <c r="J8" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="M8">
         <v>14</v>
       </c>
@@ -3330,10 +3345,14 @@
         <v>42710</v>
       </c>
       <c r="J9" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="M9">
         <v>17</v>
       </c>
@@ -3386,10 +3405,14 @@
         <v>42724</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="M10">
         <v>19</v>
       </c>
@@ -3445,10 +3468,14 @@
         <v>42745</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="M11">
         <v>22</v>
       </c>
@@ -3501,10 +3528,14 @@
         <v>42752</v>
       </c>
       <c r="J12" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="M12">
         <v>24</v>
       </c>
@@ -3557,10 +3588,14 @@
         <v>42759</v>
       </c>
       <c r="J13" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="M13">
         <v>26</v>
       </c>
@@ -3613,10 +3648,14 @@
         <v>42760</v>
       </c>
       <c r="J14" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="M14">
         <v>28</v>
       </c>
@@ -3666,10 +3705,14 @@
         <v>42767</v>
       </c>
       <c r="J15" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="M15">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
1. PUE Review und 1. PUE für Paul Börding hinzugefügt.
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/gp1-jupyter/meetings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="16440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -17,11 +12,8 @@
     <sheet name="HUE" sheetId="5" r:id="rId3"/>
     <sheet name="Tutoren" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="111">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -757,7 +749,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -1205,7 +1197,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1217,19 +1209,19 @@
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="6" max="6" width="23.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1277,7 +1269,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1296,7 +1288,7 @@
         <v>Ch 1, Versionsverwaltung</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1315,7 +1307,7 @@
         <v>Ch2, Zahldarstellung</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1334,7 +1326,7 @@
         <v>Ch 3, Animation von Programmen</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1353,7 +1345,7 @@
         <v>Ch 4: Namenkonvention für Funktionsnamen</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1372,7 +1364,7 @@
         <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1391,7 +1383,7 @@
         <v>Ch 5, Slicing, Länge</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1410,7 +1402,7 @@
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1429,7 +1421,7 @@
         <v>Ch 6: Eindeutigkeit von else</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1448,7 +1440,7 @@
         <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1467,7 +1459,7 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1489,7 +1481,7 @@
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1511,7 +1503,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1533,7 +1525,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1555,7 +1547,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1577,7 +1569,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1599,7 +1591,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1621,7 +1613,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1643,7 +1635,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1665,7 +1657,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1687,7 +1679,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1709,7 +1701,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1731,7 +1723,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1753,7 +1745,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1775,7 +1767,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1797,7 +1789,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1819,7 +1811,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1841,7 +1833,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1863,7 +1855,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1894,23 +1886,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.125" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" customWidth="1"/>
-    <col min="16" max="16" width="30.33203125" customWidth="1"/>
-    <col min="17" max="17" width="33.1640625" customWidth="1"/>
+    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="15" max="15" width="4.625" customWidth="1"/>
+    <col min="16" max="16" width="30.375" customWidth="1"/>
+    <col min="17" max="17" width="33.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
@@ -1936,7 +1928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1986,7 +1978,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2043,7 +2035,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2101,7 +2093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2158,7 +2150,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2193,6 +2185,9 @@
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A$4:B$33,2,TRUE)</f>
         <v>42668</v>
       </c>
+      <c r="K6" t="s">
+        <v>88</v>
+      </c>
       <c r="L6" s="2" t="s">
         <v>71</v>
       </c>
@@ -2215,7 +2210,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2250,6 +2245,9 @@
         <f>VLOOKUP(MAX(M7:O7),vorlesung!A$4:B$33,2,TRUE)</f>
         <v>42682</v>
       </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
         <v>71</v>
@@ -2276,7 +2274,7 @@
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2395,7 +2393,7 @@
         <v>Ch 8: Daten und Funktionen</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2453,7 +2451,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2514,7 +2512,7 @@
         <v>Ende Kapitel 9</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2572,7 +2570,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2633,7 +2631,7 @@
         <v>Ch 12: Dependency injection</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2752,7 +2750,7 @@
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2846,23 +2844,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="K3" sqref="K3:L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.125" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" customWidth="1"/>
-    <col min="16" max="16" width="30.33203125" customWidth="1"/>
-    <col min="17" max="17" width="33.1640625" customWidth="1"/>
+    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="15" max="15" width="4.625" customWidth="1"/>
+    <col min="16" max="16" width="30.375" customWidth="1"/>
+    <col min="17" max="17" width="33.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
@@ -2885,7 +2883,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
@@ -2938,7 +2936,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3003,7 +3001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3066,7 +3064,7 @@
         <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3126,7 +3124,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3189,7 +3187,7 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3249,7 +3247,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3312,7 +3310,7 @@
         <v xml:space="preserve">Ch 9: Klassifkation, Gemeinsamkeiten </v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3372,7 +3370,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3435,7 +3433,7 @@
         <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3495,7 +3493,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3555,7 +3553,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3615,7 +3613,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3672,7 +3670,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3729,7 +3727,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -3781,20 +3779,20 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D2" s="37" t="s">
         <v>105</v>
       </c>
@@ -3826,7 +3824,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D3" s="22">
         <v>4</v>
       </c>
@@ -3862,7 +3860,7 @@
       </c>
       <c r="P3" s="20"/>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D4" s="21">
         <v>14</v>
       </c>
@@ -3902,7 +3900,7 @@
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>99</v>
       </c>
@@ -3949,7 +3947,7 @@
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -4000,7 +3998,7 @@
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>80</v>
       </c>
@@ -4048,7 +4046,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>91</v>
       </c>
@@ -4103,7 +4101,7 @@
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
         <v>100</v>
       </c>
@@ -4158,7 +4156,7 @@
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
     </row>
-    <row r="10" spans="1:20" s="20" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="20" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>102</v>
       </c>
@@ -4203,7 +4201,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>101</v>
       </c>
@@ -4257,7 +4255,7 @@
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
     </row>
-    <row r="12" spans="1:20" s="1" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="1" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -4282,7 +4280,7 @@
       <c r="S12" s="10"/>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -4345,7 +4343,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -4408,7 +4406,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -4471,7 +4469,7 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -4534,7 +4532,7 @@
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -4597,7 +4595,7 @@
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -4660,7 +4658,7 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -4723,7 +4721,7 @@
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -4735,11 +4733,11 @@
       </c>
       <c r="D20" s="14">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="30">
         <f>COUNTIF(PUE!K$3:L$16,$B20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="32">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B20)</f>
@@ -4774,7 +4772,7 @@
       </c>
       <c r="N20" s="22">
         <f t="shared" si="9"/>
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="O20" s="23">
         <f t="shared" si="10"/>
@@ -4786,7 +4784,7 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -4844,14 +4842,14 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D22" s="39">
         <f>D3*SUM(D13:D21)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E22" s="39">
         <f t="shared" ref="E22:M22" si="11">E3*SUM(E13:E21)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F22" s="39">
         <f t="shared" si="11"/>
@@ -4887,7 +4885,7 @@
       </c>
       <c r="N22" s="22">
         <f>SUM(N13:N21)</f>
-        <v>1851</v>
+        <v>1856</v>
       </c>
       <c r="O22" s="22">
         <f>SUM(O13:O21)</f>

</xml_diff>

<commit_message>
WiMi Reviewterminen modifiziert nach Absprache mit AS
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\gp1-jupyter\meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/gp1-jupyter/meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="658" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="658" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,14 @@
     <sheet name="HUE" sheetId="3" r:id="rId3"/>
     <sheet name="Tutoren" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -365,7 +371,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -666,9 +672,6 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -742,9 +745,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -1307,67 +1313,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5"/>
-    <col min="2" max="2" width="11.125" style="2"/>
-    <col min="3" max="5" width="10.625"/>
-    <col min="6" max="6" width="23.875" style="3"/>
-    <col min="7" max="1025" width="10.625"/>
+    <col min="2" max="2" width="9" style="1"/>
+    <col min="6" max="6" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>42661</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:C33" si="0">WEEKNUM(B4,2)-1</f>
         <v>42</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="str">
@@ -1375,18 +1378,18 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>42662</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="str">
@@ -1394,18 +1397,18 @@
         <v>Ch 1, Versionsverwaltung</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>42665</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="str">
@@ -1413,18 +1416,18 @@
         <v>Ch2, Zahldarstellung</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>42665</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H7" t="str">
@@ -1432,18 +1435,18 @@
         <v>Ch 3, Animation von Programmen</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>42668</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="str">
@@ -1451,18 +1454,18 @@
         <v>Ch 4: Namenkonvention für Funktionsnamen</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>42669</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="str">
@@ -1470,18 +1473,18 @@
         <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>42676</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10" t="str">
@@ -1489,18 +1492,18 @@
         <v>Ch 5, Slicing, Länge</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>42682</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H11" t="str">
@@ -1508,18 +1511,18 @@
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>42683</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H12" t="str">
@@ -1527,18 +1530,18 @@
         <v>Ch 6: Eindeutigkeit von else</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>42689</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="str">
@@ -1546,18 +1549,18 @@
         <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>42690</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H14" t="str">
@@ -1565,421 +1568,421 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>42693</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
         <v>Ch 7: globale Variabeln; Scopes</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="1">
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>42693</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
         <v>Ch 8: Daten und Funktionen</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="1">
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>42696</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
         <v>Ch 8: Aufruf, Kurzschreibweise</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="1">
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>42697</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
         <v>Ch 8: Stack, Code</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="1">
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>42703</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Ch 9: Klassifkation, Gemeinsamkeiten </v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="1">
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>42704</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
         <v>Ch 9: Vernschaulichung von isinstance</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="1">
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>42710</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
         <v>Ende Kapitel 9</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21" s="1">
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>42711</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
         <v>Ch 10, Geschachtelte try</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22" s="1">
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>42717</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
         <v>Ch 11, LEGB</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="1">
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>42724</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
         <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="1">
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>42725</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Ch 12: MRO (vor Linearisierung) </v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="1">
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>42745</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
         <v>Ch 12: Dependency injection</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="1">
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>42746</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
         <v>Cg 14: Virtualenv</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O27" s="1">
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>42752</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
         <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
-      <c r="O28" s="2">
+      <c r="O28" s="1">
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>42753</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
         <v>Ch 16, Kommentare</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O29" s="1">
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>42759</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>36</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
         <v>Ch 16: Klassische for, Multiplikation</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="1">
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>42760</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
-      <c r="O31" s="2">
+      <c r="O31" s="1">
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>42766</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
         <v>Ch 17: interfaces</v>
       </c>
-      <c r="O32" s="2">
+      <c r="O32" s="1">
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>42767</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
         <v>Ch 18 Ende!</v>
       </c>
-      <c r="O33" s="2">
+      <c r="O33" s="1">
         <v>42774</v>
       </c>
     </row>
@@ -1993,139 +1996,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25"/>
-    <col min="2" max="2" width="9.625"/>
-    <col min="3" max="12" width="10.625"/>
-    <col min="13" max="13" width="6.125"/>
-    <col min="14" max="14" width="6.75"/>
-    <col min="15" max="15" width="4.75"/>
-    <col min="16" max="16" width="31.125"/>
-    <col min="17" max="17" width="33.875"/>
-    <col min="18" max="1025" width="10.625"/>
+    <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>43</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C16" si="0">D3-10</f>
         <v>42644</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D16" si="1">E3-5</f>
         <v>42654</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E16" si="2">F3-3</f>
         <v>42659</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f t="shared" ref="F3:F16" si="3">G3-2</f>
         <v>42662</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>42664</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f t="shared" ref="H3:H11" si="4">G3+7</f>
         <v>42671</v>
       </c>
-      <c r="I3" s="8" t="e">
+      <c r="I3" s="7" t="e">
         <f>VLOOKUP(MAX(M3:O3),vorlesung!A$4:B$33,2,1)</f>
         <v>#N/A</v>
       </c>
       <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>61</v>
       </c>
       <c r="P3" t="e">
@@ -2140,47 +2138,47 @@
         <f>VLOOKUP(O3,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>44</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>42651</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
         <v>42661</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f t="shared" si="2"/>
         <v>42666</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f t="shared" si="3"/>
         <v>42669</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f t="shared" ref="G4:G12" si="5">G3+7</f>
         <v>42671</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f t="shared" si="4"/>
         <v>42678</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <f>VLOOKUP(MAX(M4:O4),vorlesung!A$4:B$33,2,1)</f>
         <v>42661</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M4">
@@ -2202,42 +2200,42 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>45</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>42658</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>42668</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>42673</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f t="shared" si="3"/>
         <v>42676</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f t="shared" si="5"/>
         <v>42678</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f t="shared" si="4"/>
         <v>42685</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>VLOOKUP(MAX(M5:O5),vorlesung!A$4:B$33,2,1)</f>
         <v>42665</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M5">
@@ -2259,38 +2257,38 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>46</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>42675</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>42680</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f t="shared" si="3"/>
         <v>42683</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f t="shared" si="5"/>
         <v>42685</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" si="4"/>
         <v>42692</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A$4:B$33,2,1)</f>
         <v>42668</v>
       </c>
@@ -2300,7 +2298,7 @@
       <c r="K6" t="s">
         <v>65</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M6">
@@ -2322,46 +2320,46 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>47</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>42682</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>42687</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="3"/>
         <v>42690</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f t="shared" si="5"/>
         <v>42692</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="4"/>
         <v>42699</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <f>VLOOKUP(MAX(M7:O7),vorlesung!A$4:B$33,2,1)</f>
         <v>42682</v>
       </c>
       <c r="J7" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M7">
@@ -2386,43 +2384,43 @@
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>48</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>42679</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>42689</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>42694</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f t="shared" si="3"/>
         <v>42697</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f t="shared" si="5"/>
         <v>42699</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="4"/>
         <v>42706</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <f>VLOOKUP(MAX(M8:O8),vorlesung!A$4:B$33,2,1)</f>
         <v>42689</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M8">
@@ -2444,45 +2442,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>49</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>42686</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>42696</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>42701</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f t="shared" si="3"/>
         <v>42704</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f t="shared" si="5"/>
         <v>42706</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="4"/>
         <v>42713</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <f>VLOOKUP(MAX(M9:O9),vorlesung!A$4:B$33,2,1)</f>
         <v>42693</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M9">
@@ -2507,45 +2505,45 @@
         <v>Ch 8: Daten und Funktionen</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>42693</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>42703</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>42708</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <f t="shared" si="3"/>
         <v>42711</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f t="shared" si="5"/>
         <v>42713</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="4"/>
         <v>42720</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f>VLOOKUP(MAX(M10:O10),vorlesung!A$4:B$33,2,1)</f>
         <v>42697</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M10">
@@ -2567,45 +2565,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>51</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>42700</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>42710</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>42715</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <f t="shared" si="3"/>
         <v>42718</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <f t="shared" si="5"/>
         <v>42720</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f t="shared" si="4"/>
         <v>42727</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <f>VLOOKUP(MAX(M11:O11),vorlesung!A$4:B$33,2,1)</f>
         <v>42710</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M11">
@@ -2630,48 +2628,48 @@
         <v>Ende Kapitel 9</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>42707</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>42717</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>42722</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <f t="shared" si="3"/>
         <v>42725</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <f t="shared" si="5"/>
         <v>42727</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f>G12+21</f>
         <v>42748</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <f>VLOOKUP(MAX(M12:O12),vorlesung!A$4:B$33,2,1)</f>
         <v>42717</v>
       </c>
       <c r="J12" t="s">
         <v>107</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M12">
@@ -2693,46 +2691,46 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>42728</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>42738</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>42743</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f t="shared" si="3"/>
         <v>42746</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <f>G12+21</f>
         <v>42748</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <f>G13+7</f>
         <v>42755</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <f>VLOOKUP(MAX(M13:O13),vorlesung!A$4:B$33,2,1)</f>
         <v>42745</v>
       </c>
       <c r="J13" t="s">
         <v>107</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M13">
@@ -2757,48 +2755,48 @@
         <v>Ch 12: Dependency injection</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>42735</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>42745</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f t="shared" si="2"/>
         <v>42750</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f t="shared" si="3"/>
         <v>42753</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <f>G13+7</f>
         <v>42755</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <f>G14+7</f>
         <v>42762</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A$4:B$33,2,1)</f>
         <v>42752</v>
       </c>
       <c r="J14" t="s">
         <v>107</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M14">
@@ -2820,45 +2818,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>42742</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>42752</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f t="shared" si="2"/>
         <v>42757</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f t="shared" si="3"/>
         <v>42760</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <f>G14+7</f>
         <v>42762</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <f>G15+7</f>
         <v>42769</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <f>VLOOKUP(MAX(M15:O15),vorlesung!A$4:B$33,2,1)</f>
         <v>42760</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M15">
@@ -2883,45 +2881,45 @@
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>42749</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>42759</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>42764</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <f t="shared" si="3"/>
         <v>42767</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <f>G15+7</f>
         <v>42769</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <f>G16+7</f>
         <v>42776</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <f>VLOOKUP(MAX(M16:O16),vorlesung!A$4:B$33,2,1)</f>
         <v>42767</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="1" t="s">
         <v>60</v>
       </c>
       <c r="M16">
@@ -2980,137 +2978,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25"/>
-    <col min="2" max="2" width="9.625"/>
-    <col min="3" max="12" width="10.625"/>
-    <col min="13" max="13" width="6.125"/>
-    <col min="14" max="14" width="6.75"/>
-    <col min="15" max="15" width="4.75"/>
-    <col min="16" max="16" width="31.125"/>
-    <col min="17" max="17" width="33.875"/>
-    <col min="18" max="1025" width="10.625"/>
+    <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C15" si="0">D3-10</f>
         <v>42651</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D15" si="1">E3-5</f>
         <v>42661</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E15" si="2">F3-3</f>
         <v>42666</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f t="shared" ref="F3:F15" si="3">G3-2</f>
         <v>42669</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>42671</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f t="shared" ref="H3:H10" si="4">G3+9</f>
         <v>42680</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <f>VLOOKUP(MAX(M3:O3),vorlesung!A4:B33,2,1)</f>
         <v>42665</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -3137,45 +3129,45 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>42658</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
         <v>42668</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f t="shared" si="2"/>
         <v>42673</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f t="shared" si="3"/>
         <v>42676</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f t="shared" ref="G4:G11" si="5">G3+7</f>
         <v>42678</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f t="shared" si="4"/>
         <v>42687</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <f>VLOOKUP(MAX(M4:O4),vorlesung!A5:B34,2,1)</f>
         <v>42669</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M4">
@@ -3200,45 +3192,45 @@
         <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>42675</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>42680</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f t="shared" si="3"/>
         <v>42683</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f t="shared" si="5"/>
         <v>42685</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f t="shared" si="4"/>
         <v>42694</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>VLOOKUP(MAX(M5:O5),vorlesung!A6:B35,2,1)</f>
         <v>42682</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M5">
@@ -3260,45 +3252,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>42682</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>42687</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f t="shared" si="3"/>
         <v>42690</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f t="shared" si="5"/>
         <v>42692</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" si="4"/>
         <v>42701</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A7:B36,2,1)</f>
         <v>42690</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M6">
@@ -3323,45 +3315,45 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>42679</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>42689</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>42694</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="3"/>
         <v>42697</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f t="shared" si="5"/>
         <v>42699</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="4"/>
         <v>42708</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <f>VLOOKUP(MAX(M7:O7),vorlesung!A8:B37,2,1)</f>
         <v>42693</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M7">
@@ -3383,46 +3375,46 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>42686</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>42696</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>42701</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f t="shared" si="3"/>
         <v>42704</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f t="shared" si="5"/>
         <v>42706</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="4"/>
         <v>42715</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <f>VLOOKUP(MAX(M8:O8),vorlesung!A9:B38,2,1)</f>
         <v>42703</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="L8" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="M8">
         <v>14</v>
@@ -3446,45 +3438,45 @@
         <v xml:space="preserve">Ch 9: Klassifkation, Gemeinsamkeiten </v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>42693</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>42703</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>42708</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f t="shared" si="3"/>
         <v>42711</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f t="shared" si="5"/>
         <v>42713</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="4"/>
         <v>42722</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <f>VLOOKUP(MAX(M9:O9),vorlesung!A10:B39,2,1)</f>
         <v>42710</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M9">
@@ -3506,45 +3498,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>42700</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>42710</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>42715</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <f t="shared" si="3"/>
         <v>42718</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f t="shared" si="5"/>
         <v>42720</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="4"/>
         <v>42729</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f>VLOOKUP(MAX(M10:O10),vorlesung!A11:B40,2,1)</f>
         <v>42724</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M10">
@@ -3569,45 +3561,45 @@
         <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>42707</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>42717</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>42722</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <f t="shared" si="3"/>
         <v>42725</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <f t="shared" si="5"/>
         <v>42727</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f>G11+23</f>
         <v>42750</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <f>VLOOKUP(MAX(M11:O11),vorlesung!A12:B41,2,1)</f>
         <v>42745</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="7" t="s">
         <v>60</v>
       </c>
       <c r="M11">
@@ -3629,46 +3621,46 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>42728</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>42738</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>42743</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <f t="shared" si="3"/>
         <v>42746</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <f>G11+21</f>
         <v>42748</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f>G12+9</f>
         <v>42757</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <f>VLOOKUP(MAX(M12:O12),vorlesung!A13:B42,2,1)</f>
         <v>42752</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="M12">
         <v>24</v>
@@ -3689,45 +3681,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>42735</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>42745</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>42750</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f t="shared" si="3"/>
         <v>42753</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <f>G12+7</f>
         <v>42755</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <f>G13+9</f>
         <v>42764</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <f>VLOOKUP(MAX(M13:O13),vorlesung!A14:B43,2,1)</f>
         <v>42759</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>61</v>
       </c>
       <c r="M13">
@@ -3749,45 +3741,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>42742</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>42752</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f t="shared" si="2"/>
         <v>42757</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f t="shared" si="3"/>
         <v>42760</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <f>G13+7</f>
         <v>42762</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <f>G14+9</f>
         <v>42771</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A15:B44,2,1)</f>
         <v>42760</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>61</v>
       </c>
       <c r="M14">
@@ -3806,45 +3798,45 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>42749</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>42759</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f t="shared" si="2"/>
         <v>42764</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f t="shared" si="3"/>
         <v>42767</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <f>G14+7</f>
         <v>42769</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <f>G15+9</f>
         <v>42778</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <f>VLOOKUP(MAX(M15:O15),vorlesung!A16:B45,2,1)</f>
         <v>42767</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>61</v>
       </c>
       <c r="M15">
@@ -3900,521 +3892,509 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.75"/>
-    <col min="2" max="2" width="15.25"/>
-    <col min="3" max="3" width="10.625"/>
-    <col min="4" max="5" width="11.25"/>
-    <col min="6" max="6" width="11.875"/>
-    <col min="7" max="7" width="11.25"/>
-    <col min="8" max="10" width="11.875"/>
-    <col min="11" max="13" width="11.25"/>
-    <col min="14" max="14" width="11.875"/>
-    <col min="15" max="1025" width="10.625"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="D2" s="9" t="s">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="D2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="11">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="10">
         <v>4</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>1</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>8</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>2</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>2</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>1</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>3</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>2</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>4</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>2</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="14">
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="13">
         <v>14</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>14</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>13</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>13</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>14</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <v>14</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>14</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>14</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="13">
         <v>14</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="13">
         <v>14</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-    </row>
-    <row r="5" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+    </row>
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>2</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>1</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>1</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <f>SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <f>SUMPRODUCT(K6:K8,C6:C8)</f>
         <v>16</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <f>SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f>COUNTIF(C$13:C$21,$B6)</f>
         <v>3</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>0</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>1</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="16">
         <v>0</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="16">
         <v>1</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <v>1</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="16">
         <v>1</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="17">
         <v>2</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <v>0</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <v>1</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <f>SUMPRODUCT(D6:M6,D$10:M$10,D$11:M$11)</f>
         <v>174.66666666666666</v>
       </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f>COUNTIF(C$13:C$21,$B7)</f>
         <v>4</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>1</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>0</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <v>1</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>0</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="16">
         <v>0</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="16">
         <v>1</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="16">
         <v>2</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>2</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>1</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <f>SUMPRODUCT(D7:M7,D$10:M$10,D$11:M$11)</f>
         <v>254</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>COUNTIF(C$13:C$21,$B8)</f>
         <v>2</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <f t="shared" ref="D8:I8" si="0">D7*0.5</f>
         <v>0.5</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>1</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <f>K7*0.5</f>
         <v>1</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>1</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>1</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <f>SUMPRODUCT(D8:M8,D$10:M$10,D$11:M$11)</f>
         <v>162</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+    </row>
+    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19">
         <f t="shared" ref="D9:M9" si="1">SUMPRODUCT($C6:$C8,D6:D8)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="19">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="19">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="19">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="19">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="19">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <f>SUMPRODUCT(N6:N8,C6:C8)</f>
         <v>1864</v>
       </c>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-    </row>
-    <row r="10" spans="1:20" s="13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+    </row>
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <f t="shared" ref="D10:M10" si="2">1/D9</f>
         <v>0.2</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="20">
         <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="20">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="20">
         <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <f t="shared" ref="D11:M11" si="3">D3*D4*D5</f>
         <v>56</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="16">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="16">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="16">
         <f t="shared" si="3"/>
         <v>378</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="16">
         <f t="shared" si="3"/>
         <v>448</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="16">
         <f t="shared" si="3"/>
         <v>504</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="16">
         <f t="shared" si="3"/>
         <v>252</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <f>SUM(D11:M11)</f>
         <v>1864</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+    </row>
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="15"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -4424,60 +4404,60 @@
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="23">
         <f>COUNTIF(PUE!K$3:L$16,$B13)</f>
         <v>6</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="24">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B13)</f>
         <v>5</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="24">
         <f>COUNTIF(HUE!K$3:$L16,Tutoren!$B13)</f>
         <v>8</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="24">
         <f t="shared" ref="H13:H21" si="4">F13</f>
         <v>5</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <f t="shared" ref="I13:I21" si="5">H13</f>
         <v>5</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="23">
         <v>14</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="23">
         <f t="shared" ref="K13:K21" si="6">VLOOKUP($C13,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="25">
         <f t="shared" ref="L13:L21" si="7">VLOOKUP($C13,$B$6:$L$9,11,0)*L$4</f>
         <v>0</v>
       </c>
-      <c r="M13" s="27">
+      <c r="M13" s="26">
         <f t="shared" ref="M13:M21" si="8">VLOOKUP($C13,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="10">
         <f t="shared" ref="N13:N21" si="9">SUMPRODUCT(D$3:M$3,D13:M13)</f>
         <v>203</v>
       </c>
-      <c r="O13" s="28">
+      <c r="O13" s="27">
         <f t="shared" ref="O13:O21" si="10">VLOOKUP(C13,B$6:N$8,13,0)</f>
         <v>174.66666666666666</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -4487,60 +4467,60 @@
       <c r="C14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B14)</f>
         <v>1</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B14)</f>
         <v>4</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="30">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B14)</f>
         <v>4</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="30">
         <f>COUNTIF(HUE!K$3:$L17,Tutoren!$B14)</f>
         <v>9</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="30">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="29">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="29">
         <v>14</v>
       </c>
-      <c r="K14" s="30">
+      <c r="K14" s="29">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L14" s="32">
+      <c r="L14" s="31">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="10">
         <f t="shared" si="9"/>
         <v>196</v>
       </c>
-      <c r="O14" s="28">
+      <c r="O14" s="27">
         <f t="shared" si="10"/>
         <v>174.66666666666666</v>
       </c>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -4550,60 +4530,60 @@
       <c r="C15" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="33">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="34">
         <f>COUNTIF(PUE!K$3:L$16,$B15)</f>
         <v>4</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="35">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B15)</f>
         <v>4</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="35">
         <f>COUNTIF(HUE!K$3:$L18,Tutoren!$B15)</f>
         <v>9</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="35">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="34">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="J15" s="35">
+      <c r="J15" s="34">
         <v>14</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="34">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L15" s="37">
+      <c r="L15" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M15" s="38">
+      <c r="M15" s="37">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="10">
         <f t="shared" si="9"/>
         <v>192</v>
       </c>
-      <c r="O15" s="28">
+      <c r="O15" s="27">
         <f t="shared" si="10"/>
         <v>174.66666666666666</v>
       </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -4613,60 +4593,60 @@
       <c r="C16" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B16)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="30">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="30">
         <f>COUNTIF(HUE!K$3:$L19,Tutoren!$B16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="30">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="29">
         <v>14</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="29">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L16" s="32">
+      <c r="L16" s="31">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <f t="shared" si="9"/>
         <v>238</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="27">
         <f t="shared" si="10"/>
         <v>254</v>
       </c>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -4676,60 +4656,60 @@
       <c r="C17" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B17)</f>
         <v>1</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B17)</f>
         <v>4</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="30">
         <f>COUNTIF(HUE!K$3:$L20,Tutoren!$B17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="30">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I17" s="30">
+      <c r="I17" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J17" s="29">
         <v>14</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="29">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="L17" s="32">
+      <c r="L17" s="31">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <f t="shared" si="9"/>
         <v>162</v>
       </c>
-      <c r="O17" s="28">
+      <c r="O17" s="27">
         <f t="shared" si="10"/>
         <v>162</v>
       </c>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -4739,60 +4719,60 @@
       <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B18)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="30">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B18)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="30">
         <f>COUNTIF(HUE!K$3:$L21,Tutoren!$B18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="30">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J18" s="30">
+      <c r="J18" s="29">
         <v>14</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="29">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="L18" s="32">
+      <c r="L18" s="31">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="M18" s="33">
+      <c r="M18" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <f t="shared" si="9"/>
         <v>154</v>
       </c>
-      <c r="O18" s="28">
+      <c r="O18" s="27">
         <f t="shared" si="10"/>
         <v>162</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -4802,60 +4782,60 @@
       <c r="C19" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B19)</f>
         <v>3</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B19)</f>
         <v>4</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="38">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B19)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="30">
         <f>COUNTIF(HUE!K$3:$L22,Tutoren!$B19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="30">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I19" s="30">
+      <c r="I19" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="29">
         <v>14</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="29">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L19" s="32">
+      <c r="L19" s="31">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="M19" s="33">
+      <c r="M19" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="10">
         <f t="shared" si="9"/>
         <v>254</v>
       </c>
-      <c r="O19" s="28">
+      <c r="O19" s="27">
         <f t="shared" si="10"/>
         <v>254</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -4865,60 +4845,60 @@
       <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B20)</f>
         <v>1</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <f>COUNTIF(PUE!K$3:L$16,$B20)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="38">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B20)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="30">
         <f>COUNTIF(HUE!K$3:$L23,Tutoren!$B20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="30">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="29">
         <v>14</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="29">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L20" s="32">
+      <c r="L20" s="31">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="32">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <f t="shared" si="9"/>
         <v>243</v>
       </c>
-      <c r="O20" s="28">
+      <c r="O20" s="27">
         <f t="shared" si="10"/>
         <v>254</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -4928,108 +4908,108 @@
       <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="39">
         <f>COUNTIF(PUE!J$3:J$16,Tutoren!$B21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="40">
         <f>COUNTIF(PUE!K$3:L$16,$B21)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="41">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B21)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="42">
+      <c r="G21" s="41">
         <f>COUNTIF(HUE!K$3:$L24,Tutoren!$B21)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="41">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I21" s="41">
+      <c r="I21" s="40">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J21" s="40">
         <v>14</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="40">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L21" s="43">
+      <c r="L21" s="42">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="M21" s="44">
+      <c r="M21" s="43">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="10">
         <f t="shared" si="9"/>
         <v>238</v>
       </c>
-      <c r="O21" s="28">
+      <c r="O21" s="27">
         <f t="shared" si="10"/>
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D22" s="45">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D22" s="44">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>24</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="44">
         <f t="shared" si="11"/>
         <v>23</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="44">
         <f t="shared" si="11"/>
         <v>104</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="44">
         <f t="shared" si="11"/>
         <v>52</v>
       </c>
-      <c r="H22" s="45">
+      <c r="H22" s="44">
         <f t="shared" si="11"/>
         <v>26</v>
       </c>
-      <c r="I22" s="45">
+      <c r="I22" s="44">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="J22" s="45">
+      <c r="J22" s="44">
         <f t="shared" si="11"/>
         <v>378</v>
       </c>
-      <c r="K22" s="45">
+      <c r="K22" s="44">
         <f t="shared" si="11"/>
         <v>448</v>
       </c>
-      <c r="L22" s="45">
+      <c r="L22" s="44">
         <f t="shared" si="11"/>
         <v>560</v>
       </c>
-      <c r="M22" s="45">
+      <c r="M22" s="44">
         <f t="shared" si="11"/>
         <v>252</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="10">
         <f>SUM(N13:N21)</f>
         <v>1880</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="10">
         <f>SUM(O13:O21)</f>
         <v>1864</v>
       </c>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N13:N21">

</xml_diff>

<commit_message>
Review-Verteilung Heimübungsblätter geändert, so dass nun SHKs berücksichtigt
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="658" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="658" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" state="visible" r:id="rId2"/>
@@ -95,7 +95,7 @@
     <t>Ch 8: Stack, Code</t>
   </si>
   <si>
-    <t>Ch 9: Klassifkation, Gemeinsamkeiten </t>
+    <t>Ch 9: Klassifkation, Gemeinsamkeiten</t>
   </si>
   <si>
     <t>Ch 9: Vernschaulichung von isinstance</t>
@@ -113,7 +113,7 @@
     <t>Ch 11: Eingerahmte Ausgabe</t>
   </si>
   <si>
-    <t>Ch 12: MRO (vor Linearisierung) </t>
+    <t>Ch 12: MRO (vor Linearisierung)</t>
   </si>
   <si>
     <t>Ch 12: Dependency injection</t>
@@ -149,7 +149,7 @@
     <t>Termine</t>
   </si>
   <si>
-    <t>Wer? </t>
+    <t>Wer?</t>
   </si>
   <si>
     <t>Bezug auf Vorlesungen</t>
@@ -179,13 +179,13 @@
     <t>Fertig</t>
   </si>
   <si>
-    <t>Vorlesungen </t>
+    <t>Vorlesungen</t>
   </si>
   <si>
     <t>Entwurf</t>
   </si>
   <si>
-    <t>Review 1 </t>
+    <t>Review 1</t>
   </si>
   <si>
     <t>Review 2 (WIMi)</t>
@@ -209,10 +209,10 @@
     <t>DP</t>
   </si>
   <si>
-    <t>Anmelden, Markup </t>
-  </si>
-  <si>
-    <t>Terminal, Programme ausführen </t>
+    <t>Anmelden, Markup</t>
+  </si>
+  <si>
+    <t>Terminal, Programme ausführen</t>
   </si>
   <si>
     <t>JR</t>
@@ -236,6 +236,15 @@
     <t>Review 2</t>
   </si>
   <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
     <t>#PUE entwerfen</t>
   </si>
   <si>
@@ -275,7 +284,7 @@
     <t>Anzahl</t>
   </si>
   <si>
-    <t>Wieviele Betroffen? </t>
+    <t>Wieviele Betroffen?</t>
   </si>
   <si>
     <t>Gewichte</t>
@@ -308,7 +317,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Anzahl: </t>
+    <t>Anzahl:</t>
   </si>
   <si>
     <t>Erreichte Leistung</t>
@@ -329,18 +338,12 @@
     <t>Jonas Harbig</t>
   </si>
   <si>
-    <t>JH</t>
-  </si>
-  <si>
     <t>Jost Rossel</t>
   </si>
   <si>
     <t>Mo Thiele</t>
   </si>
   <si>
-    <t>MT</t>
-  </si>
-  <si>
     <t>Thomas Kellner</t>
   </si>
   <si>
@@ -348,9 +351,6 @@
   </si>
   <si>
     <t>Patrick Steffens</t>
-  </si>
-  <si>
-    <t>PS</t>
   </si>
 </sst>
 </file>
@@ -622,16 +622,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -795,175 +795,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <sz val="12"/>
@@ -1120,15 +952,13 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="K3:K15 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9"/>
   </cols>
   <sheetData>
@@ -1136,35 +966,34 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
       <c r="F1" s="0"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" s="1" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1172,14 +1001,14 @@
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="3" t="n">
         <v>42661</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">WEEKNUM(B4,2)-1</f>
         <v>41</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="0" t="str">
@@ -1191,14 +1020,14 @@
       <c r="A5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="3" t="n">
         <v>42662</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">WEEKNUM(B5,2)-1</f>
         <v>41</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="0" t="str">
@@ -1210,14 +1039,14 @@
       <c r="A6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="3" t="n">
         <v>42665</v>
       </c>
       <c r="C6" s="4" t="n">
         <f aca="false">WEEKNUM(B6,2)-1</f>
         <v>41</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="0" t="str">
@@ -1229,14 +1058,14 @@
       <c r="A7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="3" t="n">
         <v>42665</v>
       </c>
       <c r="C7" s="4" t="n">
         <f aca="false">WEEKNUM(B7,2)-1</f>
         <v>41</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="0" t="str">
@@ -1248,14 +1077,14 @@
       <c r="A8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="3" t="n">
         <v>42668</v>
       </c>
       <c r="C8" s="4" t="n">
         <f aca="false">WEEKNUM(B8,2)-1</f>
         <v>42</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="0" t="str">
@@ -1267,14 +1096,14 @@
       <c r="A9" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="3" t="n">
         <v>42669</v>
       </c>
       <c r="C9" s="4" t="n">
         <f aca="false">WEEKNUM(B9,2)-1</f>
         <v>42</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="0" t="str">
@@ -1286,14 +1115,14 @@
       <c r="A10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="3" t="n">
         <v>42676</v>
       </c>
       <c r="C10" s="4" t="n">
         <f aca="false">WEEKNUM(B10,2)-1</f>
         <v>43</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="0" t="str">
@@ -1305,14 +1134,14 @@
       <c r="A11" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="3" t="n">
         <v>42682</v>
       </c>
       <c r="C11" s="4" t="n">
         <f aca="false">WEEKNUM(B11,2)-1</f>
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="0" t="str">
@@ -1324,14 +1153,14 @@
       <c r="A12" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="3" t="n">
         <v>42683</v>
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">WEEKNUM(B12,2)-1</f>
         <v>44</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H12" s="0" t="str">
@@ -1343,14 +1172,14 @@
       <c r="A13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="3" t="n">
         <v>42689</v>
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">WEEKNUM(B13,2)-1</f>
         <v>45</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="0" t="str">
@@ -1362,14 +1191,14 @@
       <c r="A14" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="3" t="n">
         <v>42690</v>
       </c>
       <c r="C14" s="4" t="n">
         <f aca="false">WEEKNUM(B14,2)-1</f>
         <v>45</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="0" t="str">
@@ -1381,21 +1210,21 @@
       <c r="A15" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="3" t="n">
         <v>42693</v>
       </c>
       <c r="C15" s="4" t="n">
         <f aca="false">WEEKNUM(B15,2)-1</f>
         <v>45</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">F15</f>
         <v>Ch 7: globale Variabeln; Scopes</v>
       </c>
-      <c r="O15" s="1" t="n">
+      <c r="O15" s="3" t="n">
         <v>42696</v>
       </c>
     </row>
@@ -1403,21 +1232,21 @@
       <c r="A16" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="3" t="n">
         <v>42693</v>
       </c>
       <c r="C16" s="4" t="n">
         <f aca="false">WEEKNUM(B16,2)-1</f>
         <v>45</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">F16</f>
         <v>Ch 8: Daten und Funktionen</v>
       </c>
-      <c r="O16" s="1" t="n">
+      <c r="O16" s="3" t="n">
         <v>42697</v>
       </c>
     </row>
@@ -1425,21 +1254,21 @@
       <c r="A17" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="3" t="n">
         <v>42696</v>
       </c>
       <c r="C17" s="4" t="n">
         <f aca="false">WEEKNUM(B17,2)-1</f>
         <v>46</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">F17</f>
         <v>Ch 8: Aufruf, Kurzschreibweise</v>
       </c>
-      <c r="O17" s="1" t="n">
+      <c r="O17" s="3" t="n">
         <v>42703</v>
       </c>
     </row>
@@ -1447,21 +1276,21 @@
       <c r="A18" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="3" t="n">
         <v>42697</v>
       </c>
       <c r="C18" s="4" t="n">
         <f aca="false">WEEKNUM(B18,2)-1</f>
         <v>46</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">F18</f>
         <v>Ch 8: Stack, Code</v>
       </c>
-      <c r="O18" s="1" t="n">
+      <c r="O18" s="3" t="n">
         <v>42704</v>
       </c>
     </row>
@@ -1469,21 +1298,21 @@
       <c r="A19" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="3" t="n">
         <v>42703</v>
       </c>
       <c r="C19" s="4" t="n">
         <f aca="false">WEEKNUM(B19,2)-1</f>
         <v>47</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="0" t="str">
         <f aca="false">F19</f>
-        <v>Ch 9: Klassifkation, Gemeinsamkeiten </v>
-      </c>
-      <c r="O19" s="1" t="n">
+        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
+      </c>
+      <c r="O19" s="3" t="n">
         <v>42710</v>
       </c>
     </row>
@@ -1491,21 +1320,21 @@
       <c r="A20" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="3" t="n">
         <v>42704</v>
       </c>
       <c r="C20" s="4" t="n">
         <f aca="false">WEEKNUM(B20,2)-1</f>
         <v>47</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">F20</f>
         <v>Ch 9: Vernschaulichung von isinstance</v>
       </c>
-      <c r="O20" s="1" t="n">
+      <c r="O20" s="3" t="n">
         <v>42711</v>
       </c>
     </row>
@@ -1513,21 +1342,21 @@
       <c r="A21" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="3" t="n">
         <v>42710</v>
       </c>
       <c r="C21" s="4" t="n">
         <f aca="false">WEEKNUM(B21,2)-1</f>
         <v>48</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">F21</f>
         <v>Ende Kapitel 9</v>
       </c>
-      <c r="O21" s="1" t="n">
+      <c r="O21" s="3" t="n">
         <v>42717</v>
       </c>
     </row>
@@ -1535,21 +1364,21 @@
       <c r="A22" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="3" t="n">
         <v>42711</v>
       </c>
       <c r="C22" s="4" t="n">
         <f aca="false">WEEKNUM(B22,2)-1</f>
         <v>48</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">F22</f>
         <v>Ch 10, Geschachtelte try</v>
       </c>
-      <c r="O22" s="1" t="n">
+      <c r="O22" s="3" t="n">
         <v>42724</v>
       </c>
     </row>
@@ -1557,21 +1386,21 @@
       <c r="A23" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="3" t="n">
         <v>42717</v>
       </c>
       <c r="C23" s="4" t="n">
         <f aca="false">WEEKNUM(B23,2)-1</f>
         <v>49</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="0" t="str">
         <f aca="false">F23</f>
         <v>Ch 11, LEGB</v>
       </c>
-      <c r="O23" s="1" t="n">
+      <c r="O23" s="3" t="n">
         <v>42725</v>
       </c>
     </row>
@@ -1579,21 +1408,21 @@
       <c r="A24" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="3" t="n">
         <v>42724</v>
       </c>
       <c r="C24" s="4" t="n">
         <f aca="false">WEEKNUM(B24,2)-1</f>
         <v>50</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H24" s="0" t="str">
         <f aca="false">F24</f>
         <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
-      <c r="O24" s="1" t="n">
+      <c r="O24" s="3" t="n">
         <v>42745</v>
       </c>
     </row>
@@ -1601,21 +1430,21 @@
       <c r="A25" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="3" t="n">
         <v>42725</v>
       </c>
       <c r="C25" s="4" t="n">
         <f aca="false">WEEKNUM(B25,2)-1</f>
         <v>50</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H25" s="0" t="str">
         <f aca="false">F25</f>
-        <v>Ch 12: MRO (vor Linearisierung) </v>
-      </c>
-      <c r="O25" s="1" t="n">
+        <v>Ch 12: MRO (vor Linearisierung)</v>
+      </c>
+      <c r="O25" s="3" t="n">
         <v>42746</v>
       </c>
     </row>
@@ -1623,21 +1452,21 @@
       <c r="A26" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="3" t="n">
         <v>42745</v>
       </c>
       <c r="C26" s="4" t="n">
         <f aca="false">WEEKNUM(B26,2)-1</f>
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H26" s="0" t="str">
         <f aca="false">F26</f>
         <v>Ch 12: Dependency injection</v>
       </c>
-      <c r="O26" s="1" t="n">
+      <c r="O26" s="3" t="n">
         <v>42752</v>
       </c>
     </row>
@@ -1645,21 +1474,21 @@
       <c r="A27" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="3" t="n">
         <v>42746</v>
       </c>
       <c r="C27" s="4" t="n">
         <f aca="false">WEEKNUM(B27,2)-1</f>
         <v>1</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H27" s="0" t="str">
         <f aca="false">F27</f>
         <v>Cg 14: Virtualenv</v>
       </c>
-      <c r="O27" s="1" t="n">
+      <c r="O27" s="3" t="n">
         <v>42753</v>
       </c>
     </row>
@@ -1667,21 +1496,21 @@
       <c r="A28" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="3" t="n">
         <v>42752</v>
       </c>
       <c r="C28" s="4" t="n">
         <f aca="false">WEEKNUM(B28,2)-1</f>
         <v>2</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H28" s="0" t="str">
         <f aca="false">F28</f>
         <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
-      <c r="O28" s="1" t="n">
+      <c r="O28" s="3" t="n">
         <v>42759</v>
       </c>
     </row>
@@ -1689,21 +1518,21 @@
       <c r="A29" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="3" t="n">
         <v>42753</v>
       </c>
       <c r="C29" s="4" t="n">
         <f aca="false">WEEKNUM(B29,2)-1</f>
         <v>2</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H29" s="0" t="str">
         <f aca="false">F29</f>
         <v>Ch 16, Kommentare</v>
       </c>
-      <c r="O29" s="1" t="n">
+      <c r="O29" s="3" t="n">
         <v>42760</v>
       </c>
     </row>
@@ -1711,21 +1540,21 @@
       <c r="A30" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="3" t="n">
         <v>42759</v>
       </c>
       <c r="C30" s="4" t="n">
         <f aca="false">WEEKNUM(B30,2)-1</f>
         <v>3</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H30" s="0" t="str">
         <f aca="false">F30</f>
         <v>Ch 16: Klassische for, Multiplikation</v>
       </c>
-      <c r="O30" s="1" t="n">
+      <c r="O30" s="3" t="n">
         <v>42766</v>
       </c>
     </row>
@@ -1733,21 +1562,21 @@
       <c r="A31" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="3" t="n">
         <v>42760</v>
       </c>
       <c r="C31" s="4" t="n">
         <f aca="false">WEEKNUM(B31,2)-1</f>
         <v>3</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H31" s="0" t="str">
         <f aca="false">F31</f>
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
-      <c r="O31" s="1" t="n">
+      <c r="O31" s="3" t="n">
         <v>42767</v>
       </c>
     </row>
@@ -1755,21 +1584,21 @@
       <c r="A32" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="3" t="n">
         <v>42766</v>
       </c>
       <c r="C32" s="4" t="n">
         <f aca="false">WEEKNUM(B32,2)-1</f>
         <v>4</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H32" s="0" t="str">
         <f aca="false">F32</f>
         <v>Ch 17: interfaces</v>
       </c>
-      <c r="O32" s="1" t="n">
+      <c r="O32" s="3" t="n">
         <v>42773</v>
       </c>
     </row>
@@ -1777,21 +1606,21 @@
       <c r="A33" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="3" t="n">
         <v>42767</v>
       </c>
       <c r="C33" s="4" t="n">
         <f aca="false">WEEKNUM(B33,2)-1</f>
         <v>4</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H33" s="0" t="str">
         <f aca="false">F33</f>
         <v>Ch 18 Ende!</v>
       </c>
-      <c r="O33" s="1" t="n">
+      <c r="O33" s="3" t="n">
         <v>42774</v>
       </c>
     </row>
@@ -1813,8 +1642,8 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="1" sqref="K3:K15 L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1853,53 +1682,53 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="2" t="s">
+    <row r="2" s="1" customFormat="true" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1910,19 +1739,19 @@
       <c r="B3" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="3" t="n">
         <f aca="false">D3-10</f>
         <v>42644</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="3" t="n">
         <f aca="false">E3-5</f>
         <v>42654</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <f aca="false">F3-3</f>
         <v>42659</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="3" t="n">
         <f aca="false">G3-2</f>
         <v>42662</v>
       </c>
@@ -1958,7 +1787,7 @@
         <f aca="false">VLOOKUP(O3,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1969,23 +1798,23 @@
       <c r="B4" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="3" t="n">
         <f aca="false">D4-10</f>
         <v>42651</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <f aca="false">E4-5</f>
         <v>42661</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="3" t="n">
         <f aca="false">F4-3</f>
         <v>42666</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="3" t="n">
         <f aca="false">G4-2</f>
         <v>42669</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="3" t="n">
         <f aca="false">G3+7</f>
         <v>42671</v>
       </c>
@@ -1997,8 +1826,8 @@
         <f aca="false">VLOOKUP(MAX(M4:O4),vorlesung!A$4:B$33,2,1)</f>
         <v>42661</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M4" s="0" t="n">
@@ -2008,17 +1837,13 @@
         <f aca="false">VLOOKUP(M4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
-      <c r="Q4" s="0" t="inlineStr">
+      <c r="Q4" s="0" t="e">
         <f aca="false">VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R4" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="R4" s="0" t="e">
         <f aca="false">VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="T4" s="0" t="s">
         <v>64</v>
@@ -2031,23 +1856,23 @@
       <c r="B5" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="3" t="n">
         <f aca="false">D5-10</f>
         <v>42658</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="3" t="n">
         <f aca="false">E5-5</f>
         <v>42668</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="3" t="n">
         <f aca="false">F5-3</f>
         <v>42673</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="3" t="n">
         <f aca="false">G5-2</f>
         <v>42676</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="3" t="n">
         <f aca="false">G4+7</f>
         <v>42678</v>
       </c>
@@ -2059,7 +1884,7 @@
         <f aca="false">VLOOKUP(MAX(M5:O5),vorlesung!A$4:B$33,2,1)</f>
         <v>42665</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M5" s="0" t="n">
@@ -2076,11 +1901,9 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch2, Zahldarstellung</v>
       </c>
-      <c r="R5" s="0" t="inlineStr">
+      <c r="R5" s="0" t="e">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,23 +1913,23 @@
       <c r="B6" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="3" t="n">
         <f aca="false">D6-10</f>
         <v>42665</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="3" t="n">
         <f aca="false">E6-5</f>
         <v>42675</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="3" t="n">
         <f aca="false">F6-3</f>
         <v>42680</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="3" t="n">
         <f aca="false">G6-2</f>
         <v>42683</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="3" t="n">
         <f aca="false">G5+7</f>
         <v>42685</v>
       </c>
@@ -2124,7 +1947,7 @@
       <c r="K6" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M6" s="0" t="n">
@@ -2141,11 +1964,9 @@
         <f aca="false">VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 4: Namenkonvention für Funktionsnamen</v>
       </c>
-      <c r="R6" s="0" t="inlineStr">
+      <c r="R6" s="0" t="e">
         <f aca="false">VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,23 +1976,23 @@
       <c r="B7" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="3" t="n">
         <f aca="false">D7-10</f>
         <v>42672</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <f aca="false">E7-5</f>
         <v>42682</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="3" t="n">
         <f aca="false">F7-3</f>
         <v>42687</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="3" t="n">
         <f aca="false">G7-2</f>
         <v>42690</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="3" t="n">
         <f aca="false">G6+7</f>
         <v>42692</v>
       </c>
@@ -2186,8 +2007,8 @@
       <c r="J7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M7" s="0" t="n">
@@ -2219,23 +2040,23 @@
       <c r="B8" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="3" t="n">
         <f aca="false">D8-10</f>
         <v>42679</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="3" t="n">
         <f aca="false">E8-5</f>
         <v>42689</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="3" t="n">
         <f aca="false">F8-3</f>
         <v>42694</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="3" t="n">
         <f aca="false">G8-2</f>
         <v>42697</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="3" t="n">
         <f aca="false">G7+7</f>
         <v>42699</v>
       </c>
@@ -2247,8 +2068,8 @@
         <f aca="false">VLOOKUP(MAX(M8:O8),vorlesung!A$4:B$33,2,1)</f>
         <v>42689</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
         <v>67</v>
       </c>
       <c r="M8" s="0" t="n">
@@ -2265,11 +2086,9 @@
         <f aca="false">VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
-      <c r="R8" s="0" t="inlineStr">
+      <c r="R8" s="0" t="e">
         <f aca="false">VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,23 +2098,23 @@
       <c r="B9" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="3" t="n">
         <f aca="false">D9-10</f>
         <v>42686</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <f aca="false">E9-5</f>
         <v>42696</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="3" t="n">
         <f aca="false">F9-3</f>
         <v>42701</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="3" t="n">
         <f aca="false">G9-2</f>
         <v>42704</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="3" t="n">
         <f aca="false">G8+7</f>
         <v>42706</v>
       </c>
@@ -2307,7 +2126,7 @@
         <f aca="false">VLOOKUP(MAX(M9:O9),vorlesung!A$4:B$33,2,1)</f>
         <v>42693</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="L9" s="8" t="s">
@@ -2342,23 +2161,23 @@
       <c r="B10" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="3" t="n">
         <f aca="false">D10-10</f>
         <v>42693</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="3" t="n">
         <f aca="false">E10-5</f>
         <v>42703</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="3" t="n">
         <f aca="false">F10-3</f>
         <v>42708</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="3" t="n">
         <f aca="false">G10-2</f>
         <v>42711</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="3" t="n">
         <f aca="false">G9+7</f>
         <v>42713</v>
       </c>
@@ -2370,7 +2189,7 @@
         <f aca="false">VLOOKUP(MAX(M10:O10),vorlesung!A$4:B$33,2,1)</f>
         <v>42697</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="3" t="s">
         <v>65</v>
       </c>
       <c r="L10" s="8" t="s">
@@ -2390,11 +2209,9 @@
         <f aca="false">VLOOKUP(N10,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 8: Stack, Code</v>
       </c>
-      <c r="R10" s="0" t="inlineStr">
+      <c r="R10" s="0" t="e">
         <f aca="false">VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,23 +2221,23 @@
       <c r="B11" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="3" t="n">
         <f aca="false">D11-10</f>
         <v>42700</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="3" t="n">
         <f aca="false">E11-5</f>
         <v>42710</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <f aca="false">F11-3</f>
         <v>42715</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="3" t="n">
         <f aca="false">G11-2</f>
         <v>42718</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="3" t="n">
         <f aca="false">G10+7</f>
         <v>42720</v>
       </c>
@@ -2432,7 +2249,7 @@
         <f aca="false">VLOOKUP(MAX(M11:O11),vorlesung!A$4:B$33,2,1)</f>
         <v>42710</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="3" t="s">
         <v>65</v>
       </c>
       <c r="L11" s="8" t="s">
@@ -2449,7 +2266,7 @@
       </c>
       <c r="P11" s="0" t="str">
         <f aca="false">VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Klassifkation, Gemeinsamkeiten </v>
+        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
       </c>
       <c r="Q11" s="0" t="str">
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
@@ -2467,23 +2284,23 @@
       <c r="B12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="3" t="n">
         <f aca="false">D12-10</f>
         <v>42707</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="3" t="n">
         <f aca="false">E12-5</f>
         <v>42717</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="3" t="n">
         <f aca="false">F12-3</f>
         <v>42722</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="3" t="n">
         <f aca="false">G12-2</f>
         <v>42725</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">G11+7</f>
         <v>42727</v>
       </c>
@@ -2498,7 +2315,7 @@
       <c r="J12" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="3" t="s">
         <v>65</v>
       </c>
       <c r="L12" s="8" t="s">
@@ -2518,11 +2335,9 @@
         <f aca="false">VLOOKUP(N12,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 11, LEGB</v>
       </c>
-      <c r="R12" s="0" t="inlineStr">
+      <c r="R12" s="0" t="e">
         <f aca="false">VLOOKUP(O12,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,23 +2347,23 @@
       <c r="B13" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="3" t="n">
         <f aca="false">D13-10</f>
         <v>42728</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="3" t="n">
         <f aca="false">E13-5</f>
         <v>42738</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <f aca="false">F13-3</f>
         <v>42743</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="3" t="n">
         <f aca="false">G13-2</f>
         <v>42746</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="3" t="n">
         <f aca="false">G12+21</f>
         <v>42748</v>
       </c>
@@ -2563,7 +2378,7 @@
       <c r="J13" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="8" t="s">
         <v>60</v>
       </c>
@@ -2582,7 +2397,7 @@
       </c>
       <c r="Q13" s="0" t="str">
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: MRO (vor Linearisierung) </v>
+        <v>Ch 12: MRO (vor Linearisierung)</v>
       </c>
       <c r="R13" s="0" t="str">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
@@ -2596,23 +2411,23 @@
       <c r="B14" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="3" t="n">
         <f aca="false">D14-10</f>
         <v>42735</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="3" t="n">
         <f aca="false">E14-5</f>
         <v>42745</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="3" t="n">
         <f aca="false">F14-3</f>
         <v>42750</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="3" t="n">
         <f aca="false">G14-2</f>
         <v>42753</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">G13+7</f>
         <v>42755</v>
       </c>
@@ -2627,7 +2442,7 @@
       <c r="J14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L14" s="8" t="s">
@@ -2647,11 +2462,9 @@
         <f aca="false">VLOOKUP(N14,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
-      <c r="R14" s="0" t="inlineStr">
+      <c r="R14" s="0" t="e">
         <f aca="false">VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,23 +2474,23 @@
       <c r="B15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="3" t="n">
         <f aca="false">D15-10</f>
         <v>42742</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="3" t="n">
         <f aca="false">E15-5</f>
         <v>42752</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <f aca="false">F15-3</f>
         <v>42757</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="3" t="n">
         <f aca="false">G15-2</f>
         <v>42760</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="3" t="n">
         <f aca="false">G14+7</f>
         <v>42762</v>
       </c>
@@ -2689,7 +2502,7 @@
         <f aca="false">VLOOKUP(MAX(M15:O15),vorlesung!A$4:B$33,2,1)</f>
         <v>42760</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L15" s="8" t="s">
@@ -2724,23 +2537,23 @@
       <c r="B16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="3" t="n">
         <f aca="false">D16-10</f>
         <v>42749</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="3" t="n">
         <f aca="false">E16-5</f>
         <v>42759</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="3" t="n">
         <f aca="false">F16-3</f>
         <v>42764</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="3" t="n">
         <f aca="false">G16-2</f>
         <v>42767</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="3" t="n">
         <f aca="false">G15+7</f>
         <v>42769</v>
       </c>
@@ -2752,10 +2565,10 @@
         <f aca="false">VLOOKUP(MAX(M16:O16),vorlesung!A$4:B$33,2,1)</f>
         <v>42767</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="M16" s="0" t="n">
@@ -2772,11 +2585,9 @@
         <f aca="false">VLOOKUP(N16,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 18 Ende!</v>
       </c>
-      <c r="R16" s="0" t="inlineStr">
+      <c r="R16" s="0" t="e">
         <f aca="false">VLOOKUP(O16,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -2822,10 +2633,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2859,76 +2670,76 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="2" t="s">
+    <row r="2" s="1" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="3" t="n">
         <f aca="false">D3-10</f>
         <v>42651</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="3" t="n">
         <f aca="false">E3-5</f>
         <v>42661</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <f aca="false">F3-3</f>
         <v>42666</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="3" t="n">
         <f aca="false">G3-2</f>
         <v>42669</v>
       </c>
@@ -2950,7 +2761,7 @@
         <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>1</v>
@@ -2977,27 +2788,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="3" t="n">
         <f aca="false">D4-10</f>
         <v>42658</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <f aca="false">E4-5</f>
         <v>42668</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="3" t="n">
         <f aca="false">F4-3</f>
         <v>42673</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="3" t="n">
         <f aca="false">G4-2</f>
         <v>42676</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="3" t="n">
         <f aca="false">G3+7</f>
         <v>42678</v>
       </c>
@@ -3016,7 +2827,7 @@
         <v>60</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>4</v>
@@ -3040,27 +2851,27 @@
         <v>Ch 4: Pass-by-assignment</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="3" t="n">
         <f aca="false">D5-10</f>
         <v>42665</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="3" t="n">
         <f aca="false">E5-5</f>
         <v>42675</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="3" t="n">
         <f aca="false">F5-3</f>
         <v>42680</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="3" t="n">
         <f aca="false">G5-2</f>
         <v>42683</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="3" t="n">
         <f aca="false">G4+7</f>
         <v>42685</v>
       </c>
@@ -3079,7 +2890,7 @@
         <v>60</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>7</v>
@@ -3095,34 +2906,32 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
-      <c r="R5" s="0" t="inlineStr">
+      <c r="R5" s="0" t="e">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="3" t="n">
         <f aca="false">D6-10</f>
         <v>42672</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="3" t="n">
         <f aca="false">E6-5</f>
         <v>42682</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="3" t="n">
         <f aca="false">F6-3</f>
         <v>42687</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="3" t="n">
         <f aca="false">G6-2</f>
         <v>42690</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="3" t="n">
         <f aca="false">G5+7</f>
         <v>42692</v>
       </c>
@@ -3141,7 +2950,7 @@
         <v>60</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>9</v>
@@ -3165,27 +2974,27 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="3" t="n">
         <f aca="false">D7-10</f>
         <v>42679</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <f aca="false">E7-5</f>
         <v>42689</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="3" t="n">
         <f aca="false">F7-3</f>
         <v>42694</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="3" t="n">
         <f aca="false">G7-2</f>
         <v>42697</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="3" t="n">
         <f aca="false">G6+7</f>
         <v>42699</v>
       </c>
@@ -3204,7 +3013,7 @@
         <v>60</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>12</v>
@@ -3220,34 +3029,32 @@
         <f aca="false">VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 8: Daten und Funktionen</v>
       </c>
-      <c r="R7" s="0" t="inlineStr">
+      <c r="R7" s="0" t="e">
         <f aca="false">VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="3" t="n">
         <f aca="false">D8-10</f>
         <v>42686</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="3" t="n">
         <f aca="false">E8-5</f>
         <v>42696</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="3" t="n">
         <f aca="false">F8-3</f>
         <v>42701</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="3" t="n">
         <f aca="false">G8-2</f>
         <v>42704</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="3" t="n">
         <f aca="false">G7+7</f>
         <v>42706</v>
       </c>
@@ -3266,7 +3073,7 @@
         <v>62</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>14</v>
@@ -3287,30 +3094,30 @@
       </c>
       <c r="R8" s="0" t="str">
         <f aca="false">VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Klassifkation, Gemeinsamkeiten </v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="3" t="n">
         <f aca="false">D9-10</f>
         <v>42693</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <f aca="false">E9-5</f>
         <v>42703</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="3" t="n">
         <f aca="false">F9-3</f>
         <v>42708</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="3" t="n">
         <f aca="false">G9-2</f>
         <v>42711</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="3" t="n">
         <f aca="false">G8+7</f>
         <v>42713</v>
       </c>
@@ -3329,7 +3136,7 @@
         <v>62</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>17</v>
@@ -3345,34 +3152,32 @@
         <f aca="false">VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ende Kapitel 9</v>
       </c>
-      <c r="R9" s="0" t="inlineStr">
+      <c r="R9" s="0" t="e">
         <f aca="false">VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="3" t="n">
         <f aca="false">D10-10</f>
         <v>42700</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="3" t="n">
         <f aca="false">E10-5</f>
         <v>42710</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="3" t="n">
         <f aca="false">F10-3</f>
         <v>42715</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="3" t="n">
         <f aca="false">G10-2</f>
         <v>42718</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="3" t="n">
         <f aca="false">G9+7</f>
         <v>42720</v>
       </c>
@@ -3391,7 +3196,7 @@
         <v>62</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>19</v>
@@ -3415,27 +3220,27 @@
         <v>Ch 11: Eingerahmte Ausgabe</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="3" t="n">
         <f aca="false">D11-10</f>
         <v>42707</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="3" t="n">
         <f aca="false">E11-5</f>
         <v>42717</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <f aca="false">F11-3</f>
         <v>42722</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="3" t="n">
         <f aca="false">G11-2</f>
         <v>42725</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="3" t="n">
         <f aca="false">G10+7</f>
         <v>42727</v>
       </c>
@@ -3454,7 +3259,7 @@
         <v>62</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>22</v>
@@ -3464,40 +3269,38 @@
       </c>
       <c r="P11" s="0" t="str">
         <f aca="false">VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: MRO (vor Linearisierung) </v>
+        <v>Ch 12: MRO (vor Linearisierung)</v>
       </c>
       <c r="Q11" s="0" t="str">
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 12: Dependency injection</v>
       </c>
-      <c r="R11" s="0" t="inlineStr">
+      <c r="R11" s="0" t="e">
         <f aca="false">VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="3" t="n">
         <f aca="false">D12-10</f>
         <v>42728</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="3" t="n">
         <f aca="false">E12-5</f>
         <v>42738</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="3" t="n">
         <f aca="false">F12-3</f>
         <v>42743</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="3" t="n">
         <f aca="false">G12-2</f>
         <v>42746</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">G11+21</f>
         <v>42748</v>
       </c>
@@ -3516,7 +3319,7 @@
         <v>67</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>24</v>
@@ -3532,34 +3335,32 @@
         <f aca="false">VLOOKUP(N12,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
-      <c r="R12" s="0" t="inlineStr">
+      <c r="R12" s="0" t="e">
         <f aca="false">VLOOKUP(O12,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="3" t="n">
         <f aca="false">D13-10</f>
         <v>42735</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="3" t="n">
         <f aca="false">E13-5</f>
         <v>42745</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <f aca="false">F13-3</f>
         <v>42750</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="3" t="n">
         <f aca="false">G13-2</f>
         <v>42753</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="3" t="n">
         <f aca="false">G12+7</f>
         <v>42755</v>
       </c>
@@ -3578,7 +3379,7 @@
         <v>67</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>26</v>
@@ -3594,34 +3395,32 @@
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 16: Klassische for, Multiplikation</v>
       </c>
-      <c r="R13" s="0" t="inlineStr">
+      <c r="R13" s="0" t="e">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="3" t="n">
         <f aca="false">D14-10</f>
         <v>42742</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="3" t="n">
         <f aca="false">E14-5</f>
         <v>42752</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="3" t="n">
         <f aca="false">F14-3</f>
         <v>42757</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="3" t="n">
         <f aca="false">G14-2</f>
         <v>42760</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">G13+7</f>
         <v>42762</v>
       </c>
@@ -3640,7 +3439,7 @@
         <v>67</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>28</v>
@@ -3649,40 +3448,36 @@
         <f aca="false">VLOOKUP(M14,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
-      <c r="Q14" s="0" t="inlineStr">
+      <c r="Q14" s="0" t="e">
         <f aca="false">VLOOKUP(N14,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R14" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="0" t="e">
         <f aca="false">VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="3" t="n">
         <f aca="false">D15-10</f>
         <v>42749</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="3" t="n">
         <f aca="false">E15-5</f>
         <v>42759</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <f aca="false">F15-3</f>
         <v>42764</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="3" t="n">
         <f aca="false">G15-2</f>
         <v>42767</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="3" t="n">
         <f aca="false">G14+7</f>
         <v>42769</v>
       </c>
@@ -3701,7 +3496,7 @@
         <v>67</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>30</v>
@@ -3710,19 +3505,28 @@
         <f aca="false">VLOOKUP(M15,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 18 Ende!</v>
       </c>
-      <c r="Q15" s="0" t="inlineStr">
+      <c r="Q15" s="0" t="e">
         <f aca="false">VLOOKUP(N15,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R15" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="0" t="e">
         <f aca="false">VLOOKUP(O15,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="M1:O1"/>
@@ -3769,7 +3573,7 @@
   <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="K3:K15 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -3777,42 +3581,42 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9"/>
   </cols>
   <sheetData>
-    <row r="2" s="2" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="11" t="n">
         <v>4</v>
       </c>
@@ -3843,15 +3647,15 @@
       <c r="M3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>82</v>
+      <c r="N3" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="P3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="14" t="n">
         <v>14</v>
       </c>
@@ -3882,8 +3686,8 @@
       <c r="M4" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>83</v>
+      <c r="N4" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
@@ -3892,10 +3696,10 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>84</v>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="D5" s="14" t="n">
         <v>1</v>
@@ -3931,8 +3735,8 @@
         <f aca="false">SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>85</v>
+      <c r="N5" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
@@ -3941,47 +3745,47 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f aca="false">COUNTIF(C$13:C$21,$B6)</f>
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="J6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="N6" s="1" t="n">
         <f aca="false">SUMPRODUCT(D6:M6,D$10:M$10,D$11:M$11)</f>
         <v>174.666666666667</v>
       </c>
@@ -3992,44 +3796,44 @@
       <c r="T6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <f aca="false">COUNTIF(C$13:C$21,$B7)</f>
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="L7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="M7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N7" s="1" t="n">
         <f aca="false">SUMPRODUCT(D7:M7,D$10:M$10,D$11:M$11)</f>
         <v>254</v>
       </c>
@@ -4041,50 +3845,50 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <f aca="false">COUNTIF(C$13:C$21,$B8)</f>
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">D7*0.5</f>
         <v>0.5</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="1" t="n">
         <f aca="false">E7*0.5</f>
         <v>0.5</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">F7*0.5</f>
         <v>0</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">G7*0.5</f>
         <v>0.5</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="1" t="n">
         <f aca="false">H7*0.5</f>
         <v>0</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="1" t="n">
         <f aca="false">I7*0.5</f>
         <v>0</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="J8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="1" t="n">
         <f aca="false">K7*0.5</f>
         <v>1</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="L8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M8" s="2" t="n">
+      <c r="M8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="N8" s="1" t="n">
         <f aca="false">SUMPRODUCT(D8:M8,D$10:M$10,D$11:M$11)</f>
         <v>162</v>
       </c>
@@ -4096,7 +3900,7 @@
     </row>
     <row r="9" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="n">
@@ -4139,7 +3943,7 @@
         <f aca="false">SUMPRODUCT($C6:$C8,M6:M8)</f>
         <v>9</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="N9" s="1" t="n">
         <f aca="false">SUMPRODUCT(N6:N8,C6:C8)</f>
         <v>1864</v>
       </c>
@@ -4151,7 +3955,7 @@
     </row>
     <row r="10" s="13" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D10" s="13" t="n">
         <f aca="false">1/D9</f>
@@ -4194,51 +3998,51 @@
         <v>0.111111111111111</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="2" t="n">
+    <row r="11" s="1" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <f aca="false">D3*D4*D5</f>
         <v>56</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="1" t="n">
         <f aca="false">E3*E4*E5</f>
         <v>28</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="1" t="n">
         <f aca="false">F3*F4*F5</f>
         <v>104</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="1" t="n">
         <f aca="false">G3*G4*G5</f>
         <v>52</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="1" t="n">
         <f aca="false">H3*H4*H5</f>
         <v>28</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="1" t="n">
         <f aca="false">I3*I4*I5</f>
         <v>14</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="1" t="n">
         <f aca="false">J3*J4*J5</f>
         <v>378</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="1" t="n">
         <f aca="false">K3*K4*K5</f>
         <v>448</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="L11" s="1" t="n">
         <f aca="false">L3*L4*L5</f>
         <v>504</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="M11" s="1" t="n">
         <f aca="false">M3*M4*M5</f>
         <v>252</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="N11" s="1" t="n">
         <f aca="false">SUM(D11:M11)</f>
         <v>1864</v>
       </c>
@@ -4249,23 +4053,23 @@
       <c r="T11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="N12" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
@@ -4275,13 +4079,13 @@
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D13" s="20" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B13)</f>
@@ -4297,7 +4101,7 @@
       </c>
       <c r="G13" s="22" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L16,Tutoren!$B13)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H13" s="22" t="n">
         <f aca="false">F13</f>
@@ -4324,7 +4128,7 @@
       </c>
       <c r="N13" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D13:M13)</f>
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="O13" s="25" t="n">
         <f aca="false">VLOOKUP(C13,B$6:N$8,13,0)</f>
@@ -4338,13 +4142,13 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D14" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B14)</f>
@@ -4360,7 +4164,7 @@
       </c>
       <c r="G14" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L17,Tutoren!$B14)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H14" s="28" t="n">
         <f aca="false">F14</f>
@@ -4387,7 +4191,7 @@
       </c>
       <c r="N14" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D14:M14)</f>
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="O14" s="25" t="n">
         <f aca="false">VLOOKUP(C14,B$6:N$8,13,0)</f>
@@ -4401,13 +4205,13 @@
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D15" s="31" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B15)</f>
@@ -4423,7 +4227,7 @@
       </c>
       <c r="G15" s="33" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L18,Tutoren!$B15)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H15" s="33" t="n">
         <f aca="false">F15</f>
@@ -4450,7 +4254,7 @@
       </c>
       <c r="N15" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D15:M15)</f>
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="O15" s="25" t="n">
         <f aca="false">VLOOKUP(C15,B$6:N$8,13,0)</f>
@@ -4464,13 +4268,13 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D16" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B16)</f>
@@ -4486,7 +4290,7 @@
       </c>
       <c r="G16" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L19,Tutoren!$B16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="28" t="n">
         <f aca="false">F16</f>
@@ -4513,7 +4317,7 @@
       </c>
       <c r="N16" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D16:M16)</f>
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="O16" s="25" t="n">
         <f aca="false">VLOOKUP(C16,B$6:N$8,13,0)</f>
@@ -4527,13 +4331,13 @@
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D17" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B17)</f>
@@ -4549,7 +4353,7 @@
       </c>
       <c r="G17" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L20,Tutoren!$B17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="28" t="n">
         <f aca="false">F17</f>
@@ -4576,7 +4380,7 @@
       </c>
       <c r="N17" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D17:M17)</f>
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O17" s="25" t="n">
         <f aca="false">VLOOKUP(C17,B$6:N$8,13,0)</f>
@@ -4590,13 +4394,13 @@
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D18" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B18)</f>
@@ -4612,7 +4416,7 @@
       </c>
       <c r="G18" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L21,Tutoren!$B18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="28" t="n">
         <f aca="false">F18</f>
@@ -4639,7 +4443,7 @@
       </c>
       <c r="N18" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D18:M18)</f>
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="O18" s="25" t="n">
         <f aca="false">VLOOKUP(C18,B$6:N$8,13,0)</f>
@@ -4653,13 +4457,13 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>61</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D19" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B19)</f>
@@ -4675,7 +4479,7 @@
       </c>
       <c r="G19" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L22,Tutoren!$B19)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="28" t="n">
         <f aca="false">F19</f>
@@ -4702,7 +4506,7 @@
       </c>
       <c r="N19" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D19:M19)</f>
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O19" s="25" t="n">
         <f aca="false">VLOOKUP(C19,B$6:N$8,13,0)</f>
@@ -4716,13 +4520,13 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D20" s="26" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B20)</f>
@@ -4738,7 +4542,7 @@
       </c>
       <c r="G20" s="28" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L23,Tutoren!$B20)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="28" t="n">
         <f aca="false">F20</f>
@@ -4765,7 +4569,7 @@
       </c>
       <c r="N20" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D20:M20)</f>
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="O20" s="25" t="n">
         <f aca="false">VLOOKUP(C20,B$6:N$8,13,0)</f>
@@ -4779,13 +4583,13 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D21" s="36" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B21)</f>
@@ -4801,7 +4605,7 @@
       </c>
       <c r="G21" s="38" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L24,Tutoren!$B21)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="38" t="n">
         <f aca="false">F21</f>
@@ -4828,7 +4632,7 @@
       </c>
       <c r="N21" s="11" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D21:M21)</f>
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="O21" s="25" t="n">
         <f aca="false">VLOOKUP(C21,B$6:N$8,13,0)</f>

</xml_diff>

<commit_message>
Vorlesungstand nach VL 6
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="23460" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="209">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -656,6 +656,12 @@
   </si>
   <si>
     <t>4:1-49</t>
+  </si>
+  <si>
+    <t>4:49-Ende; 5:1-12</t>
+  </si>
+  <si>
+    <t>Bis Slicing von Tuples</t>
   </si>
 </sst>
 </file>
@@ -1670,7 +1676,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,9 +1882,11 @@
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" ref="H8:H33" si="1">F9</f>
-        <v>Ch 4: Pass-by-assignment</v>
+      <c r="H9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1900,7 +1908,7 @@
         <v>16</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H9:H33" si="1">F10</f>
         <v>Ch 5, Slicing, Länge</v>
       </c>
     </row>
@@ -2896,7 +2904,7 @@
       </c>
       <c r="P7" t="str">
         <f>VLOOKUP(M7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 4: Pass-by-assignment</v>
+        <v>4:49-Ende; 5:1-12</v>
       </c>
       <c r="Q7" t="str">
         <f>VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3521,10 +3529,13 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -3727,7 +3738,7 @@
       </c>
       <c r="R4" t="str">
         <f>VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 4: Pass-by-assignment</v>
+        <v>4:49-Ende; 5:1-12</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
PUE und HUE Themen leicht aktualisiert
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="212">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -662,6 +662,15 @@
   </si>
   <si>
     <t>Bis Slicing von Tuples</t>
+  </si>
+  <si>
+    <t>Erreichte Vorlesung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE ok </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE leidlich ok </t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1142,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1259,6 +1268,36 @@
       <font>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1675,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1908,7 +1947,7 @@
         <v>16</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" ref="H9:H33" si="1">F10</f>
+        <f t="shared" ref="H10:H33" si="1">F10</f>
         <v>Ch 5, Slicing, Länge</v>
       </c>
     </row>
@@ -2508,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2551,7 +2590,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2599,6 +2638,9 @@
       </c>
       <c r="R2" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
@@ -2631,9 +2673,9 @@
         <f t="shared" ref="H3:H11" si="4">G3+7</f>
         <v>42671</v>
       </c>
-      <c r="I3" s="7" t="e">
+      <c r="I3" s="7">
         <f>VLOOKUP(MAX(M3:O3),vorlesung!A$4:B$33,2,1)</f>
-        <v>#N/A</v>
+        <v>42661</v>
       </c>
       <c r="J3" t="s">
         <v>60</v>
@@ -2644,9 +2686,12 @@
       <c r="L3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="P3" t="e">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="str">
         <f>VLOOKUP(M3,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>0; 1:1-22</v>
       </c>
       <c r="Q3" t="e">
         <f>VLOOKUP(N3,vorlesung!$A$4:$H$33,8,0)</f>
@@ -2656,6 +2701,10 @@
         <f>VLOOKUP(O3,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
+      <c r="S3">
+        <f>MAX(M3:O3)</f>
+        <v>1</v>
+      </c>
       <c r="T3" s="2" t="s">
         <v>63</v>
       </c>
@@ -2693,7 +2742,7 @@
       </c>
       <c r="I4" s="7">
         <f>VLOOKUP(MAX(M4:O4),vorlesung!A$4:B$33,2,1)</f>
-        <v>42661</v>
+        <v>42665</v>
       </c>
       <c r="J4" t="s">
         <v>64</v>
@@ -2705,20 +2754,27 @@
         <v>62</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
       </c>
       <c r="P4" t="str">
         <f>VLOOKUP(M4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>0; 1:1-22</v>
-      </c>
-      <c r="Q4" t="e">
+        <v>1:23-Ende</v>
+      </c>
+      <c r="Q4" t="str">
         <f>VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>2:1-19</v>
       </c>
       <c r="R4" t="e">
         <f>VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
+      <c r="S4" s="47">
+        <f t="shared" ref="S4:S16" si="6">MAX(M4:O4)</f>
+        <v>3</v>
+      </c>
       <c r="T4" t="s">
         <v>66</v>
       </c>
@@ -2756,7 +2812,7 @@
       </c>
       <c r="I5" s="7">
         <f>VLOOKUP(MAX(M5:O5),vorlesung!A$4:B$33,2,1)</f>
-        <v>42665</v>
+        <v>42668</v>
       </c>
       <c r="J5" t="s">
         <v>65</v>
@@ -2768,23 +2824,27 @@
         <v>62</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P5" t="str">
         <f>VLOOKUP(M5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>1:23-Ende</v>
+        <v>2:20-Ende; 3 komplett</v>
       </c>
       <c r="Q5" t="str">
         <f>VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>2:1-19</v>
+        <v>4:1-49</v>
       </c>
       <c r="R5" t="e">
         <f>VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
+      <c r="S5" s="47">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -2819,7 +2879,7 @@
       </c>
       <c r="I6" s="7">
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A$4:B$33,2,1)</f>
-        <v>42668</v>
+        <v>42669</v>
       </c>
       <c r="J6" t="s">
         <v>67</v>
@@ -2831,23 +2891,27 @@
         <v>62</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6" t="str">
         <f>VLOOKUP(M6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>2:20-Ende; 3 komplett</v>
+        <v>4:1-49</v>
       </c>
       <c r="Q6" t="str">
         <f>VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>4:1-49</v>
+        <v>4:49-Ende; 5:1-12</v>
       </c>
       <c r="R6" t="e">
         <f>VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
+      <c r="S6" s="47">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -2894,25 +2958,26 @@
         <v>62</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N7">
-        <v>7</v>
-      </c>
-      <c r="O7">
         <v>8</v>
       </c>
       <c r="P7" t="str">
         <f>VLOOKUP(M7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>4:49-Ende; 5:1-12</v>
+        <v>Ch 5, Slicing, Länge</v>
       </c>
       <c r="Q7" t="str">
         <f>VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5, Slicing, Länge</v>
-      </c>
-      <c r="R7" t="str">
+        <v>Ch 5: dicts, Operationen darauf</v>
+      </c>
+      <c r="R7" t="e">
         <f>VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5: dicts, Operationen darauf</v>
+        <v>#N/A</v>
+      </c>
+      <c r="S7" s="47">
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -2948,7 +3013,7 @@
       </c>
       <c r="I8" s="7">
         <f>VLOOKUP(MAX(M8:O8),vorlesung!A$4:B$33,2,1)</f>
-        <v>42689</v>
+        <v>42690</v>
       </c>
       <c r="J8" t="s">
         <v>64</v>
@@ -2964,6 +3029,9 @@
       </c>
       <c r="N8">
         <v>10</v>
+      </c>
+      <c r="O8">
+        <v>11</v>
       </c>
       <c r="P8" t="str">
         <f>VLOOKUP(M8,vorlesung!$A$4:$H$33,8,0)</f>
@@ -2973,9 +3041,13 @@
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
-      <c r="R8" t="e">
+      <c r="R8" t="str">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>Ch 6: Mischen mit Slicing</v>
+      </c>
+      <c r="S8" s="47">
+        <f t="shared" si="6"/>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -3023,25 +3095,26 @@
         <v>70</v>
       </c>
       <c r="M9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N9">
-        <v>12</v>
-      </c>
-      <c r="O9">
         <v>13</v>
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 6: Mischen mit Slicing</v>
+        <v>Ch 7: globale Variabeln; Scopes</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 7: globale Variabeln; Scopes</v>
-      </c>
-      <c r="R9" t="str">
+        <v>Ch 8: Daten und Funktionen</v>
+      </c>
+      <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 8: Daten und Funktionen</v>
+        <v>#N/A</v>
+      </c>
+      <c r="S9" s="47">
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -3077,7 +3150,7 @@
       </c>
       <c r="I10" s="7">
         <f>VLOOKUP(MAX(M10:O10),vorlesung!A$4:B$33,2,1)</f>
-        <v>42697</v>
+        <v>42703</v>
       </c>
       <c r="J10" t="s">
         <v>69</v>
@@ -3093,6 +3166,9 @@
       </c>
       <c r="N10">
         <v>15</v>
+      </c>
+      <c r="O10">
+        <v>16</v>
       </c>
       <c r="P10" t="str">
         <f>VLOOKUP(M10,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3102,9 +3178,13 @@
         <f>VLOOKUP(N10,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 8: Stack, Code</v>
       </c>
-      <c r="R10" t="e">
+      <c r="R10" t="str">
         <f>VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
+      </c>
+      <c r="S10" s="47">
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -3139,7 +3219,7 @@
         <v>42727</v>
       </c>
       <c r="I11" s="7">
-        <f>VLOOKUP(MAX(M11:O11),vorlesung!A$4:B$33,2,1)</f>
+        <f>VLOOKUP(MAX(M11:N11),vorlesung!A$4:B$33,2,1)</f>
         <v>42710</v>
       </c>
       <c r="J11" t="s">
@@ -3152,25 +3232,26 @@
         <v>70</v>
       </c>
       <c r="M11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N11">
-        <v>17</v>
-      </c>
-      <c r="O11">
         <v>18</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P11" t="e">
+        <f>VLOOKUP(#REF!,vorlesung!$A$4:$H$33,8,0)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" t="str">
         <f>VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
-      </c>
-      <c r="Q11" t="str">
+        <v>Ch 9: Vernschaulichung von isinstance</v>
+      </c>
+      <c r="R11" t="str">
         <f>VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Vernschaulichung von isinstance</v>
-      </c>
-      <c r="R11" t="str">
-        <f>VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ende Kapitel 9</v>
+      </c>
+      <c r="S11" s="47">
+        <f>MAX(M11:N11)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -3206,7 +3287,7 @@
       </c>
       <c r="I12" s="7">
         <f>VLOOKUP(MAX(M12:O12),vorlesung!A$4:B$33,2,1)</f>
-        <v>42717</v>
+        <v>42724</v>
       </c>
       <c r="J12" t="s">
         <v>61</v>
@@ -3222,6 +3303,9 @@
       </c>
       <c r="N12">
         <v>20</v>
+      </c>
+      <c r="O12">
+        <v>21</v>
       </c>
       <c r="P12" t="str">
         <f>VLOOKUP(M12,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3231,9 +3315,13 @@
         <f>VLOOKUP(N12,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 11, LEGB</v>
       </c>
-      <c r="R12" t="e">
+      <c r="R12" t="str">
         <f>VLOOKUP(O12,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>Ch 11: Eingerahmte Ausgabe</v>
+      </c>
+      <c r="S12" s="47">
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -3281,25 +3369,26 @@
         <v>60</v>
       </c>
       <c r="M13">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N13">
-        <v>22</v>
-      </c>
-      <c r="O13">
         <v>23</v>
       </c>
       <c r="P13" t="str">
         <f>VLOOKUP(M13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 11: Eingerahmte Ausgabe</v>
+        <v>Ch 12: MRO (vor Linearisierung)</v>
       </c>
       <c r="Q13" t="str">
         <f>VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: MRO (vor Linearisierung)</v>
-      </c>
-      <c r="R13" t="str">
+        <v>Ch 12: Dependency injection</v>
+      </c>
+      <c r="R13" t="e">
         <f>VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: Dependency injection</v>
+        <v>#N/A</v>
+      </c>
+      <c r="S13" s="47">
+        <f t="shared" si="6"/>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -3335,7 +3424,7 @@
       </c>
       <c r="I14" s="7">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A$4:B$33,2,1)</f>
-        <v>42752</v>
+        <v>42753</v>
       </c>
       <c r="J14" t="s">
         <v>61</v>
@@ -3351,6 +3440,9 @@
       </c>
       <c r="N14">
         <v>25</v>
+      </c>
+      <c r="O14">
+        <v>26</v>
       </c>
       <c r="P14" t="str">
         <f>VLOOKUP(M14,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3360,9 +3452,13 @@
         <f>VLOOKUP(N14,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 14: Compiler vs. Interpreter</v>
       </c>
-      <c r="R14" t="e">
+      <c r="R14" t="str">
         <f>VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>Ch 16, Kommentare</v>
+      </c>
+      <c r="S14" s="47">
+        <f t="shared" si="6"/>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -3409,18 +3505,15 @@
       <c r="L15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M15">
-        <v>26</v>
-      </c>
       <c r="N15">
         <v>27</v>
       </c>
       <c r="O15">
         <v>28</v>
       </c>
-      <c r="P15" t="str">
+      <c r="P15" t="e">
         <f>VLOOKUP(M15,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 16, Kommentare</v>
+        <v>#N/A</v>
       </c>
       <c r="Q15" t="str">
         <f>VLOOKUP(N15,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3430,6 +3523,10 @@
         <f>VLOOKUP(O15,vorlesung!$A$4:$H$33,8,0)</f>
         <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
+      <c r="S15" s="47">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -3489,6 +3586,10 @@
       <c r="R16" t="e">
         <f>VLOOKUP(O16,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
+      </c>
+      <c r="S16" s="47">
+        <f t="shared" si="6"/>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3496,27 +3597,40 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="lessThan">
       <formula>$H3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I16">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="lessThan">
       <formula>$H4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+      <formula>$S$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+      <formula>$S$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:O3">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+      <formula>$S$3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3526,18 +3640,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.83203125" customWidth="1"/>
+    <col min="17" max="17" width="27.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -3558,8 +3677,14 @@
       <c r="T1" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="U1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>47</v>
@@ -3613,7 +3738,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3677,8 +3802,16 @@
       <c r="T3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3" t="b">
+        <f>MAX(M3:O3)&lt;=MAX(PUE!M3:O3)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="47" t="b">
+        <f>MAX(N3:P3)&lt;=MAX(PUE!N4:P4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3708,7 +3841,7 @@
       </c>
       <c r="I4" s="7">
         <f>VLOOKUP(MAX(M4:O4),vorlesung!A5:B34,2,1)</f>
-        <v>42669</v>
+        <v>42665</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>62</v>
@@ -3720,28 +3853,33 @@
         <v>61</v>
       </c>
       <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
         <v>4</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4">
-        <v>6</v>
       </c>
       <c r="P4" t="str">
         <f>VLOOKUP(M4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>2:20-Ende; 3 komplett</v>
+        <v>2:1-19</v>
       </c>
       <c r="Q4" t="str">
         <f>VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>4:1-49</v>
-      </c>
-      <c r="R4" t="str">
+        <v>2:20-Ende; 3 komplett</v>
+      </c>
+      <c r="R4" t="e">
         <f>VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>4:49-Ende; 5:1-12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+        <v>#N/A</v>
+      </c>
+      <c r="U4" s="47" t="b">
+        <f>MAX(M4:O4)&lt;=MAX(PUE!M4:O4)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="47" t="b">
+        <f>MAX(N4:P4)&lt;=MAX(PUE!N5:P5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3771,7 +3909,7 @@
       </c>
       <c r="I5" s="7">
         <f>VLOOKUP(MAX(M5:O5),vorlesung!A6:B35,2,1)</f>
-        <v>42682</v>
+        <v>42668</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>62</v>
@@ -3783,25 +3921,33 @@
         <v>68</v>
       </c>
       <c r="M5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P5" t="str">
         <f>VLOOKUP(M5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5, Slicing, Länge</v>
+        <v>2:20-Ende; 3 komplett</v>
       </c>
       <c r="Q5" t="str">
         <f>VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5: dicts, Operationen darauf</v>
+        <v>4:1-49</v>
       </c>
       <c r="R5" t="e">
         <f>VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5" s="47" t="b">
+        <f>MAX(M5:O5)&lt;=MAX(PUE!M5:O5)</f>
+        <v>1</v>
+      </c>
+      <c r="V5" s="47" t="b">
+        <f>MAX(N5:P5)&lt;=MAX(PUE!N6:P6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3831,7 +3977,7 @@
       </c>
       <c r="I6" s="7">
         <f>VLOOKUP(MAX(M6:O6),vorlesung!A7:B36,2,1)</f>
-        <v>42690</v>
+        <v>42676</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>62</v>
@@ -3843,28 +3989,33 @@
         <v>69</v>
       </c>
       <c r="M6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="P6" t="str">
         <f>VLOOKUP(M6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 6: Eindeutigkeit von else</v>
+        <v>4:49-Ende; 5:1-12</v>
       </c>
       <c r="Q6" t="str">
         <f>VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 6: Schleifenvariable nach Schleifenende</v>
-      </c>
-      <c r="R6" t="str">
+        <v>Ch 5, Slicing, Länge</v>
+      </c>
+      <c r="R6" t="e">
         <f>VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 6: Mischen mit Slicing</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+        <v>#N/A</v>
+      </c>
+      <c r="U6" s="47" t="b">
+        <f>MAX(M6:O6)&lt;=MAX(PUE!M6:O6)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="47" t="b">
+        <f>MAX(N6:P6)&lt;=MAX(PUE!N7:P7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3894,7 +4045,7 @@
       </c>
       <c r="I7" s="7">
         <f>VLOOKUP(MAX(M7:O7),vorlesung!A8:B37,2,1)</f>
-        <v>42693</v>
+        <v>42683</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>62</v>
@@ -3906,25 +4057,33 @@
         <v>67</v>
       </c>
       <c r="M7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="N7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="P7" t="str">
         <f>VLOOKUP(M7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 7: globale Variabeln; Scopes</v>
+        <v>Ch 5: dicts, Operationen darauf</v>
       </c>
       <c r="Q7" t="str">
         <f>VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 8: Daten und Funktionen</v>
+        <v>Ch 6: Eindeutigkeit von else</v>
       </c>
       <c r="R7" t="e">
         <f>VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U7" s="47" t="b">
+        <f>MAX(M7:O7)&lt;=MAX(PUE!M7:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="47" t="b">
+        <f>MAX(N7:P7)&lt;=MAX(PUE!N8:P8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3954,7 +4113,7 @@
       </c>
       <c r="I8" s="7">
         <f>VLOOKUP(MAX(M8:O8),vorlesung!A9:B38,2,1)</f>
-        <v>42703</v>
+        <v>42690</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>70</v>
@@ -3966,28 +4125,33 @@
         <v>65</v>
       </c>
       <c r="M8">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N8">
-        <v>15</v>
-      </c>
-      <c r="O8">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P8" t="str">
         <f>VLOOKUP(M8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 8: Aufruf, Kurzschreibweise</v>
+        <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
       <c r="Q8" t="str">
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 8: Stack, Code</v>
-      </c>
-      <c r="R8" t="str">
+        <v>Ch 6: Mischen mit Slicing</v>
+      </c>
+      <c r="R8" t="e">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+        <v>#N/A</v>
+      </c>
+      <c r="U8" s="47" t="b">
+        <f>MAX(M8:O8)&lt;=MAX(PUE!M8:O8)</f>
+        <v>1</v>
+      </c>
+      <c r="V8" s="47" t="b">
+        <f>MAX(N8:P8)&lt;=MAX(PUE!N9:P9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4017,7 +4181,7 @@
       </c>
       <c r="I9" s="7">
         <f>VLOOKUP(MAX(M9:O9),vorlesung!A10:B39,2,1)</f>
-        <v>42710</v>
+        <v>42693</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>70</v>
@@ -4029,25 +4193,33 @@
         <v>64</v>
       </c>
       <c r="M9">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N9">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 9: Vernschaulichung von isinstance</v>
+        <v>Ch 7: globale Variabeln; Scopes</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ende Kapitel 9</v>
+        <v>Ch 8: Daten und Funktionen</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U9" s="47" t="b">
+        <f>MAX(M9:O9)&lt;=MAX(PUE!M9:O9)</f>
+        <v>1</v>
+      </c>
+      <c r="V9" s="47" t="b">
+        <f>MAX(N9:P9)&lt;=MAX(PUE!N10:P10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4077,7 +4249,7 @@
       </c>
       <c r="I10" s="7">
         <f>VLOOKUP(MAX(M10:O10),vorlesung!A11:B40,2,1)</f>
-        <v>42724</v>
+        <v>42703</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>70</v>
@@ -4089,28 +4261,36 @@
         <v>61</v>
       </c>
       <c r="M10">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O10">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="P10" t="str">
         <f>VLOOKUP(M10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 10, Geschachtelte try</v>
+        <v>Ch 8: Aufruf, Kurzschreibweise</v>
       </c>
       <c r="Q10" t="str">
         <f>VLOOKUP(N10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 11, LEGB</v>
+        <v>Ch 8: Stack, Code</v>
       </c>
       <c r="R10" t="str">
         <f>VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 11: Eingerahmte Ausgabe</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+        <v>Ch 9: Klassifkation, Gemeinsamkeiten</v>
+      </c>
+      <c r="U10" s="47" t="b">
+        <f>MAX(M10:O10)&lt;=MAX(PUE!M10:O10)</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="47" t="e">
+        <f>MAX(N10:P10)&lt;=MAX(PUE!N11:P11)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4140,7 +4320,7 @@
       </c>
       <c r="I11" s="7">
         <f>VLOOKUP(MAX(M11:O11),vorlesung!A12:B41,2,1)</f>
-        <v>42745</v>
+        <v>42710</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>70</v>
@@ -4152,25 +4332,33 @@
         <v>68</v>
       </c>
       <c r="M11">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="N11">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="P11" t="str">
         <f>VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: MRO (vor Linearisierung)</v>
+        <v>Ch 9: Vernschaulichung von isinstance</v>
       </c>
       <c r="Q11" t="str">
         <f>VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 12: Dependency injection</v>
+        <v>Ende Kapitel 9</v>
       </c>
       <c r="R11" t="e">
         <f>VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U11" s="47" t="b">
+        <f>MAX(M11:O11)&lt;=MAX(PUE!M11:N11)</f>
+        <v>1</v>
+      </c>
+      <c r="V11" s="47" t="b">
+        <f>MAX(N11:P11)&lt;=MAX(PUE!N12:P12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4200,7 +4388,7 @@
       </c>
       <c r="I12" s="7">
         <f>VLOOKUP(MAX(M12:O12),vorlesung!A13:B42,2,1)</f>
-        <v>42752</v>
+        <v>42724</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>60</v>
@@ -4212,25 +4400,36 @@
         <v>69</v>
       </c>
       <c r="M12">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N12">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="O12">
+        <v>21</v>
       </c>
       <c r="P12" t="str">
         <f>VLOOKUP(M12,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Cg 14: Virtualenv</v>
+        <v>Ch 10, Geschachtelte try</v>
       </c>
       <c r="Q12" t="str">
         <f>VLOOKUP(N12,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 14: Compiler vs. Interpreter</v>
-      </c>
-      <c r="R12" t="e">
+        <v>Ch 11, LEGB</v>
+      </c>
+      <c r="R12" t="str">
         <f>VLOOKUP(O12,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+        <v>Ch 11: Eingerahmte Ausgabe</v>
+      </c>
+      <c r="U12" s="47" t="b">
+        <f>MAX(M12:O12)&lt;=MAX(PUE!M12:O12)</f>
+        <v>1</v>
+      </c>
+      <c r="V12" s="47" t="b">
+        <f>MAX(N12:P12)&lt;=MAX(PUE!N13:P13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4260,7 +4459,7 @@
       </c>
       <c r="I13" s="7">
         <f>VLOOKUP(MAX(M13:O13),vorlesung!A14:B43,2,1)</f>
-        <v>42759</v>
+        <v>42745</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>60</v>
@@ -4272,25 +4471,33 @@
         <v>61</v>
       </c>
       <c r="M13">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N13">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P13" t="str">
         <f>VLOOKUP(M13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 16, Kommentare</v>
+        <v>Ch 12: MRO (vor Linearisierung)</v>
       </c>
       <c r="Q13" t="str">
         <f>VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 16: Klassische for, Multiplikation</v>
+        <v>Ch 12: Dependency injection</v>
       </c>
       <c r="R13" t="e">
         <f>VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U13" s="47" t="b">
+        <f>MAX(M13:O13)&lt;=MAX(PUE!M13:O13)</f>
+        <v>1</v>
+      </c>
+      <c r="V13" s="47" t="b">
+        <f>MAX(N13:P13)&lt;=MAX(PUE!N14:P14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4320,7 +4527,7 @@
       </c>
       <c r="I14" s="7">
         <f>VLOOKUP(MAX(M14:O14),vorlesung!A15:B44,2,1)</f>
-        <v>42760</v>
+        <v>42753</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>60</v>
@@ -4332,22 +4539,36 @@
         <v>68</v>
       </c>
       <c r="M14">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="N14">
+        <v>25</v>
+      </c>
+      <c r="O14">
+        <v>26</v>
       </c>
       <c r="P14" t="str">
         <f>VLOOKUP(M14,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 17: Zuweisungskompatibilität</v>
-      </c>
-      <c r="Q14" t="e">
+        <v>Cg 14: Virtualenv</v>
+      </c>
+      <c r="Q14" t="str">
         <f>VLOOKUP(N14,vorlesung!$A$4:$H$33,8,0)</f>
+        <v>Ch 14: Compiler vs. Interpreter</v>
+      </c>
+      <c r="R14" t="str">
+        <f>VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
+        <v>Ch 16, Kommentare</v>
+      </c>
+      <c r="U14" s="47" t="b">
+        <f>MAX(M14:O14)&lt;=MAX(PUE!M14:O14)</f>
+        <v>1</v>
+      </c>
+      <c r="V14" s="47" t="e">
+        <f>MAX(N14:P14)&lt;=MAX(PUE!N15:P15)</f>
         <v>#N/A</v>
       </c>
-      <c r="R14" t="e">
-        <f>VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4377,7 +4598,7 @@
       </c>
       <c r="I15" s="7">
         <f>VLOOKUP(MAX(M15:O15),vorlesung!A16:B45,2,1)</f>
-        <v>42767</v>
+        <v>42760</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>60</v>
@@ -4389,19 +4610,30 @@
         <v>69</v>
       </c>
       <c r="M15">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="N15">
+        <v>28</v>
       </c>
       <c r="P15" t="str">
         <f>VLOOKUP(M15,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 18 Ende!</v>
-      </c>
-      <c r="Q15" t="e">
+        <v>Ch 16: Klassische for, Multiplikation</v>
+      </c>
+      <c r="Q15" t="str">
         <f>VLOOKUP(N15,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <v>Ch 17: Zuweisungskompatibilität</v>
       </c>
       <c r="R15" t="e">
         <f>VLOOKUP(O15,vorlesung!$A$4:$H$33,8,0)</f>
         <v>#N/A</v>
+      </c>
+      <c r="U15" s="47" t="b">
+        <f>MAX(M15:O15)&lt;=MAX(PUE!M15:O15)</f>
+        <v>1</v>
+      </c>
+      <c r="V15" s="47" t="b">
+        <f>MAX(N15:P15)&lt;=MAX(PUE!N16:P16)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4409,26 +4641,26 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="between">
       <formula>$G3</formula>
       <formula>$H3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
       <formula>$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I15">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="between">
       <formula>$G4</formula>
       <formula>$H4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
       <formula>$G4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Stand nach VL 7
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="214">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t xml:space="preserve">PUE leidlich ok </t>
+  </si>
+  <si>
+    <t>5:12-Ende</t>
+  </si>
+  <si>
+    <t>Tuple, Listen, Dicts. Komplett; Sets ausgelassen</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1946,9 +1952,11 @@
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" ref="H10:H33" si="1">F10</f>
-        <v>Ch 5, Slicing, Länge</v>
+      <c r="H10" t="s">
+        <v>212</v>
+      </c>
+      <c r="I10" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1970,7 +1978,7 @@
         <v>17</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H10:H33" si="1">F11</f>
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
@@ -2547,7 +2555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -2965,7 +2973,7 @@
       </c>
       <c r="P7" t="str">
         <f>VLOOKUP(M7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5, Slicing, Länge</v>
+        <v>5:12-Ende</v>
       </c>
       <c r="Q7" t="str">
         <f>VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4000,7 +4008,7 @@
       </c>
       <c r="Q6" t="str">
         <f>VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>Ch 5, Slicing, Länge</v>
+        <v>5:12-Ende</v>
       </c>
       <c r="R6" t="e">
         <f>VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>

</xml_diff>

<commit_message>
Review getauscht, PÜ7-12, JH-JR
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="994" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,8 @@
     <sheet name="Uebungsgruppen" sheetId="5" r:id="rId5"/>
     <sheet name="Deadlines sortiert" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1144,9 +1141,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1451,6 +1448,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1720,11 +1720,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -1733,13 +1733,13 @@
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1978,11 +1978,11 @@
         <v>17</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" ref="H10:H33" si="1">F11</f>
+        <f t="shared" ref="H11:H33" si="1">F11</f>
         <v>Ch 5: dicts, Operationen darauf</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>Ch 6: Eindeutigkeit von else</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>Ch 6: Schleifenvariable nach Schleifenende</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>Ch 6: Mischen mit Slicing</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2555,11 +2555,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2573,7 +2573,7 @@
     <col min="18" max="18" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>68</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>70</v>
@@ -3125,7 +3125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>61</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>60</v>
@@ -3469,7 +3469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3642,7 +3642,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3654,7 +3654,7 @@
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3664,7 +3664,7 @@
     <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>47</v>
@@ -3746,7 +3746,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4685,9 +4685,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="D2" s="8" t="s">
         <v>75</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4801,7 +4801,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4850,7 +4850,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -4901,7 +4901,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>91</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>92</v>
       </c>
@@ -5004,7 +5004,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>93</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
         <v>94</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>95</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>96</v>
       </c>
@@ -5183,7 +5183,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -5246,7 +5246,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -5309,7 +5309,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -5372,7 +5372,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -5435,7 +5435,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -5498,7 +5498,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -5561,7 +5561,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>110</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D22" s="40">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -5838,9 +5838,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>111</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>104</v>
       </c>
@@ -5883,7 +5883,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>103</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>109</v>
       </c>
@@ -5917,7 +5917,7 @@
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>108</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
         <v>110</v>
       </c>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="41" t="s">
         <v>107</v>
       </c>
@@ -5966,7 +5966,7 @@
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>106</v>
       </c>
@@ -5981,7 +5981,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>102</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>105</v>
       </c>
@@ -6033,9 +6033,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>123</v>
       </c>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="U2" s="32"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>1</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>2</v>
       </c>
@@ -6179,7 +6179,7 @@
       </c>
       <c r="U4" s="47"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>3</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>4</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>6</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="26">
         <v>8</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="26">
         <v>9</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="26">
         <v>10</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="26">
         <v>11</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="26">
         <v>12</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="26">
         <v>13</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="26">
         <v>14</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="26">
         <v>15</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="26">
         <v>16</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="26">
         <v>17</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>18</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="26">
         <v>19</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>20</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="26">
         <v>21</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="26">
         <v>22</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="26">
         <v>23</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>24</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="26">
         <v>25</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>26</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>27</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>28</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="26">
         <v>29</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>30</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
JH und JR getausch in PÜ7
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,8 @@
     <sheet name="Uebungsgruppen" sheetId="5" r:id="rId5"/>
     <sheet name="Deadlines sortiert" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1163,9 +1160,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1470,6 +1467,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1739,11 +1739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -1752,13 +1752,13 @@
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2575,11 +2575,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2593,7 +2593,7 @@
     <col min="18" max="18" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>49</v>
@@ -3145,7 +3145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3674,7 +3674,7 @@
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3684,7 +3684,7 @@
     <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -3766,7 +3766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4705,9 +4705,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4778,7 +4778,7 @@
       </c>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4821,7 +4821,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4870,7 +4870,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +4921,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
@@ -4969,7 +4969,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -5024,7 +5024,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>72</v>
       </c>
@@ -5079,7 +5079,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
         <v>73</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
@@ -5178,7 +5178,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
@@ -5203,7 +5203,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -5266,7 +5266,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -5392,7 +5392,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="E16" s="26">
         <f>COUNTIF(PUE!K$3:L$16,$B16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="27">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B16)</f>
@@ -5443,7 +5443,7 @@
       </c>
       <c r="N16" s="10">
         <f t="shared" si="9"/>
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="O16" s="24">
         <f t="shared" si="10"/>
@@ -5455,7 +5455,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="E17" s="26">
         <f>COUNTIF(PUE!K$3:L$16,$B17)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" s="27">
         <f>COUNTIF(HUE!J$3:J$16,Tutoren!$B17)</f>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="N17" s="10">
         <f t="shared" si="9"/>
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O17" s="24">
         <f t="shared" si="10"/>
@@ -5518,7 +5518,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -5581,7 +5581,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -5644,7 +5644,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -5707,7 +5707,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D22" s="40">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -5858,9 +5858,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>90</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>83</v>
       </c>
@@ -5903,7 +5903,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>82</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>88</v>
       </c>
@@ -5937,7 +5937,7 @@
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>87</v>
       </c>
@@ -5954,7 +5954,7 @@
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
         <v>89</v>
       </c>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="41" t="s">
         <v>86</v>
       </c>
@@ -5986,7 +5986,7 @@
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>85</v>
       </c>
@@ -6001,7 +6001,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>81</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>84</v>
       </c>
@@ -6053,9 +6053,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>102</v>
       </c>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="U2" s="32"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>1</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>2</v>
       </c>
@@ -6199,7 +6199,7 @@
       </c>
       <c r="U4" s="47"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>3</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>4</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>6</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="26">
         <v>8</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="26">
         <v>9</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="26">
         <v>10</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="26">
         <v>11</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="26">
         <v>12</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="26">
         <v>13</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="26">
         <v>14</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="26">
         <v>15</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="26">
         <v>16</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="26">
         <v>17</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>18</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="26">
         <v>19</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>20</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="26">
         <v>21</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="26">
         <v>22</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="26">
         <v>23</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>24</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="26">
         <v>25</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>26</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>27</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>28</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="26">
         <v>29</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>30</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
vl 12 und 13 beschrieben
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23460" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="Uebungsgruppen" sheetId="5" r:id="rId5"/>
     <sheet name="Deadlines sortiert" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -692,6 +695,24 @@
   </si>
   <si>
     <t>7: Formale Parameter mit vorbelegten Werten</t>
+  </si>
+  <si>
+    <t>7: String umdrehen -- Code</t>
+  </si>
+  <si>
+    <t>7:12-7:60</t>
+  </si>
+  <si>
+    <t>7:60-Ende; 8:1-32</t>
+  </si>
+  <si>
+    <t>8:Konstruktor; Ablaufbeispiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:Klassenatrtibute </t>
+  </si>
+  <si>
+    <t>8:32-75</t>
   </si>
 </sst>
 </file>
@@ -1160,9 +1181,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1739,11 +1760,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -1752,13 +1773,13 @@
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1787,7 +1808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1816,7 +1837,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1844,7 +1865,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1872,7 +1893,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1900,7 +1921,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1928,7 +1949,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1956,7 +1977,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1984,7 +2005,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2012,7 +2033,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2040,7 +2061,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2068,7 +2089,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2079,18 +2100,24 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D14" s="55">
+        <v>42690</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>221</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2101,21 +2128,27 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D15" s="4">
+        <v>42693</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>214</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
+      </c>
+      <c r="I15" t="s">
+        <v>223</v>
       </c>
       <c r="O15" s="4">
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2126,21 +2159,27 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D16" s="4">
+        <v>42693</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>199</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>199</v>
+        <v>225</v>
+      </c>
+      <c r="I16" t="s">
+        <v>224</v>
       </c>
       <c r="O16" s="4">
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2165,7 +2204,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2190,7 +2229,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2215,7 +2254,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2240,7 +2279,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2265,7 +2304,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2290,7 +2329,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2315,7 +2354,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2340,7 +2379,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2365,7 +2404,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2390,7 +2429,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2415,7 +2454,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2440,7 +2479,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2465,7 +2504,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2490,7 +2529,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2515,7 +2554,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2540,7 +2579,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2575,11 +2614,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2593,7 +2632,7 @@
     <col min="18" max="18" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2618,7 +2657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2710,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2737,7 +2776,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2807,7 +2846,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2874,7 +2913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2941,7 +2980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3008,7 +3047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3071,14 +3110,14 @@
       </c>
       <c r="R8" t="str">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7: String umdrehen</v>
+        <v>7:12-7:60</v>
       </c>
       <c r="S8" s="47">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3130,11 +3169,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Objekte/Instanzen: Graphische Notation</v>
+        <v>7:60-Ende; 8:1-32</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: self-lose Methoden</v>
+        <v>8:32-75</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3145,7 +3184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3215,7 +3254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3282,7 +3321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3352,7 +3391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3419,7 +3458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3489,7 +3528,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3559,7 +3598,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3671,10 +3710,10 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3684,7 +3723,7 @@
     <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3712,7 +3751,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -3766,7 +3805,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3839,7 +3878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3907,7 +3946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3975,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4043,7 +4082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4111,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4164,7 +4203,7 @@
       </c>
       <c r="Q8" t="str">
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7: String umdrehen</v>
+        <v>7:12-7:60</v>
       </c>
       <c r="R8" t="e">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4179,7 +4218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4228,11 +4267,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Objekte/Instanzen: Graphische Notation</v>
+        <v>7:60-Ende; 8:1-32</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: self-lose Methoden</v>
+        <v>8:32-75</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4247,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4318,7 +4357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4386,7 +4425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4457,7 +4496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4525,7 +4564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4596,7 +4635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4705,9 +4744,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
@@ -4739,7 +4778,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4778,7 +4817,7 @@
       </c>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4821,7 +4860,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4870,7 +4909,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +4960,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
@@ -4969,7 +5008,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -5024,7 +5063,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>72</v>
       </c>
@@ -5079,7 +5118,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>73</v>
       </c>
@@ -5124,7 +5163,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
@@ -5178,7 +5217,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
@@ -5203,7 +5242,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -5266,7 +5305,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -5329,7 +5368,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -5392,7 +5431,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5455,7 +5494,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5518,7 +5557,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -5581,7 +5620,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -5644,7 +5683,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -5707,7 +5746,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -5765,7 +5804,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D22" s="40">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -5858,9 +5897,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>90</v>
       </c>
@@ -5886,7 +5925,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>83</v>
       </c>
@@ -5903,7 +5942,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>82</v>
       </c>
@@ -5920,7 +5959,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>88</v>
       </c>
@@ -5937,7 +5976,7 @@
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>87</v>
       </c>
@@ -5954,7 +5993,7 @@
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>89</v>
       </c>
@@ -5971,7 +6010,7 @@
       </c>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>86</v>
       </c>
@@ -5986,7 +6025,7 @@
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>85</v>
       </c>
@@ -6001,7 +6040,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>81</v>
       </c>
@@ -6018,7 +6057,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
         <v>84</v>
       </c>
@@ -6053,9 +6092,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -6063,7 +6102,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>102</v>
       </c>
@@ -6105,7 +6144,7 @@
       </c>
       <c r="U2" s="32"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="26">
         <v>1</v>
       </c>
@@ -6153,7 +6192,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="26">
         <v>2</v>
       </c>
@@ -6199,7 +6238,7 @@
       </c>
       <c r="U4" s="47"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
         <v>3</v>
       </c>
@@ -6251,7 +6290,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
         <v>4</v>
       </c>
@@ -6297,7 +6336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -6338,7 +6377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>6</v>
       </c>
@@ -6384,7 +6423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -6430,7 +6469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="26">
         <v>8</v>
       </c>
@@ -6481,7 +6520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <v>9</v>
       </c>
@@ -6527,7 +6566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>10</v>
       </c>
@@ -6568,7 +6607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>11</v>
       </c>
@@ -6622,7 +6661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>12</v>
       </c>
@@ -6663,7 +6702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
         <v>13</v>
       </c>
@@ -6714,7 +6753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
         <v>14</v>
       </c>
@@ -6760,7 +6799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
         <v>15</v>
       </c>
@@ -6811,7 +6850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="26">
         <v>16</v>
       </c>
@@ -6860,7 +6899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
         <v>17</v>
       </c>
@@ -6901,7 +6940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="26">
         <v>18</v>
       </c>
@@ -6957,7 +6996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <v>19</v>
       </c>
@@ -7001,7 +7040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="26">
         <v>20</v>
       </c>
@@ -7047,7 +7086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <v>21</v>
       </c>
@@ -7091,7 +7130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
         <v>22</v>
       </c>
@@ -7142,7 +7181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
         <v>23</v>
       </c>
@@ -7193,7 +7232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="26">
         <v>24</v>
       </c>
@@ -7239,7 +7278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <v>25</v>
       </c>
@@ -7290,7 +7329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="26">
         <v>26</v>
       </c>
@@ -7336,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
         <v>27</v>
       </c>
@@ -7382,7 +7421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="26">
         <v>28</v>
       </c>
@@ -7423,7 +7462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <v>29</v>
       </c>
@@ -7468,7 +7507,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="26">
         <v>30</v>
       </c>
@@ -7507,7 +7546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
termine aktualisiert vom samstag
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23460" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,8 @@
     <sheet name="Uebungsgruppen" sheetId="5" r:id="rId5"/>
     <sheet name="Deadlines sortiert" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="220">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -695,24 +692,6 @@
   </si>
   <si>
     <t>7: Formale Parameter mit vorbelegten Werten</t>
-  </si>
-  <si>
-    <t>7: String umdrehen -- Code</t>
-  </si>
-  <si>
-    <t>7:12-7:60</t>
-  </si>
-  <si>
-    <t>7:60-Ende; 8:1-32</t>
-  </si>
-  <si>
-    <t>8:Konstruktor; Ablaufbeispiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:Klassenatrtibute </t>
-  </si>
-  <si>
-    <t>8:32-75</t>
   </si>
 </sst>
 </file>
@@ -1181,9 +1160,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1760,11 +1739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -1773,13 +1752,13 @@
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1808,7 +1787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1837,7 +1816,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1865,7 +1844,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1893,7 +1872,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1921,7 +1900,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1949,7 +1928,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1977,7 +1956,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2005,7 +1984,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2033,7 +2012,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2061,7 +2040,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2089,7 +2068,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2100,24 +2079,18 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D14" s="55">
-        <v>42690</v>
-      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H14" t="s">
-        <v>221</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="H14" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2128,27 +2101,21 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D15" s="4">
-        <v>42693</v>
-      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>214</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I15" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="O15" s="4">
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2159,27 +2126,21 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D16" s="4">
-        <v>42693</v>
-      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>199</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="I16" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="O16" s="4">
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2204,7 +2165,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2229,7 +2190,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2254,7 +2215,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2279,7 +2240,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2304,7 +2265,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2329,7 +2290,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2354,7 +2315,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2379,7 +2340,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2404,7 +2365,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2429,7 +2390,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2454,7 +2415,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2479,7 +2440,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2504,7 +2465,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2529,7 +2490,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2554,7 +2515,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2579,7 +2540,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2614,11 +2575,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2632,7 +2593,7 @@
     <col min="18" max="18" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2657,7 +2618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
@@ -2710,7 +2671,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2776,7 +2737,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2846,7 +2807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2913,7 +2874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2980,7 +2941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3047,7 +3008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3110,14 +3071,14 @@
       </c>
       <c r="R8" t="str">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7:12-7:60</v>
+        <v>7: String umdrehen</v>
       </c>
       <c r="S8" s="47">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3169,11 +3130,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7:60-Ende; 8:1-32</v>
+        <v>8: Objekte/Instanzen: Graphische Notation</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8:32-75</v>
+        <v>8: self-lose Methoden</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3184,7 +3145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3254,7 +3215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3321,7 +3282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3391,7 +3352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3458,7 +3419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3528,7 +3489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3598,7 +3559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3710,10 +3671,10 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3723,7 +3684,7 @@
     <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +3712,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -3805,7 +3766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3878,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3946,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4014,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4082,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4150,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4203,7 +4164,7 @@
       </c>
       <c r="Q8" t="str">
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7:12-7:60</v>
+        <v>7: String umdrehen</v>
       </c>
       <c r="R8" t="e">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4218,7 +4179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4267,11 +4228,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7:60-Ende; 8:1-32</v>
+        <v>8: Objekte/Instanzen: Graphische Notation</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8:32-75</v>
+        <v>8: self-lose Methoden</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4286,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4357,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4425,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4496,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4564,7 +4525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4635,7 +4596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4744,9 +4705,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
@@ -4778,7 +4739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4817,7 +4778,7 @@
       </c>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4860,7 +4821,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4909,7 +4870,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -4960,7 +4921,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
@@ -5008,7 +4969,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -5063,7 +5024,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
         <v>72</v>
       </c>
@@ -5118,7 +5079,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
         <v>73</v>
       </c>
@@ -5163,7 +5124,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
@@ -5217,7 +5178,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
@@ -5242,7 +5203,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -5305,7 +5266,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -5368,7 +5329,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -5431,7 +5392,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5494,7 +5455,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5557,7 +5518,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -5620,7 +5581,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -5683,7 +5644,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -5746,7 +5707,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -5804,7 +5765,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D22" s="40">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -5897,9 +5858,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>90</v>
       </c>
@@ -5925,7 +5886,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>83</v>
       </c>
@@ -5942,7 +5903,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>82</v>
       </c>
@@ -5959,7 +5920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>88</v>
       </c>
@@ -5976,7 +5937,7 @@
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>87</v>
       </c>
@@ -5993,7 +5954,7 @@
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
         <v>89</v>
       </c>
@@ -6010,7 +5971,7 @@
       </c>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="41" t="s">
         <v>86</v>
       </c>
@@ -6025,7 +5986,7 @@
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>85</v>
       </c>
@@ -6040,7 +6001,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>81</v>
       </c>
@@ -6057,7 +6018,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>84</v>
       </c>
@@ -6092,9 +6053,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -6102,7 +6063,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>102</v>
       </c>
@@ -6144,7 +6105,7 @@
       </c>
       <c r="U2" s="32"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>1</v>
       </c>
@@ -6192,7 +6153,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>2</v>
       </c>
@@ -6238,7 +6199,7 @@
       </c>
       <c r="U4" s="47"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>3</v>
       </c>
@@ -6290,7 +6251,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>4</v>
       </c>
@@ -6336,7 +6297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -6377,7 +6338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>6</v>
       </c>
@@ -6423,7 +6384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -6469,7 +6430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="26">
         <v>8</v>
       </c>
@@ -6520,7 +6481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="26">
         <v>9</v>
       </c>
@@ -6566,7 +6527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="26">
         <v>10</v>
       </c>
@@ -6607,7 +6568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="26">
         <v>11</v>
       </c>
@@ -6661,7 +6622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="26">
         <v>12</v>
       </c>
@@ -6702,7 +6663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="26">
         <v>13</v>
       </c>
@@ -6753,7 +6714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="26">
         <v>14</v>
       </c>
@@ -6799,7 +6760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="26">
         <v>15</v>
       </c>
@@ -6850,7 +6811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="26">
         <v>16</v>
       </c>
@@ -6899,7 +6860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="26">
         <v>17</v>
       </c>
@@ -6940,7 +6901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>18</v>
       </c>
@@ -6996,7 +6957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="26">
         <v>19</v>
       </c>
@@ -7040,7 +7001,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>20</v>
       </c>
@@ -7086,7 +7047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="26">
         <v>21</v>
       </c>
@@ -7130,7 +7091,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="26">
         <v>22</v>
       </c>
@@ -7181,7 +7142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="26">
         <v>23</v>
       </c>
@@ -7232,7 +7193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>24</v>
       </c>
@@ -7278,7 +7239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="26">
         <v>25</v>
       </c>
@@ -7329,7 +7290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>26</v>
       </c>
@@ -7375,7 +7336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>27</v>
       </c>
@@ -7421,7 +7382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>28</v>
       </c>
@@ -7462,7 +7423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="26">
         <v>29</v>
       </c>
@@ -7507,7 +7468,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>30</v>
       </c>
@@ -7546,7 +7507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
VL bis einschlisesslich 15 beschrieben
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/gp1/meetings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="23460" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="Uebungsgruppen" sheetId="5" r:id="rId5"/>
     <sheet name="Deadlines sortiert" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="229">
   <si>
     <t>Aktuelles Semester</t>
   </si>
@@ -692,6 +695,33 @@
   </si>
   <si>
     <t>7: Formale Parameter mit vorbelegten Werten</t>
+  </si>
+  <si>
+    <t>7:11-7:60</t>
+  </si>
+  <si>
+    <t>7:60-Ende; 8:1-34</t>
+  </si>
+  <si>
+    <t>8:35-75</t>
+  </si>
+  <si>
+    <t>8:75-100(5)</t>
+  </si>
+  <si>
+    <t>Rekusrion; Coding mit funktionen; Klassen und Objekte Einführung; bis Konstruktor</t>
+  </si>
+  <si>
+    <t>Konstruktor; mehrere Objekte; Methodenaufruf; Gleichheit; self-lose Methoden/statische vs. dynamische Methoden</t>
+  </si>
+  <si>
+    <t>Namensräume; Refernezen zählen als Beispiel für statische Attribute; string; stack; Anfang binärer Suchbaum</t>
+  </si>
+  <si>
+    <t>8:100-Ende; 9:1-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binäre Suchbaum rekursives Einfügen (insbes.: wo State speichern?). Vererbung. Liskov Substituion. </t>
   </si>
 </sst>
 </file>
@@ -1160,9 +1190,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1739,11 +1769,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -1752,13 +1782,13 @@
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1787,7 +1817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1816,7 +1846,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1844,7 +1874,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1872,7 +1902,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1900,7 +1930,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1928,7 +1958,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1956,7 +1986,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1984,7 +2014,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2012,7 +2042,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2040,7 +2070,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2068,7 +2098,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2079,18 +2109,24 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D14" s="4">
+        <v>42690</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
+        <v>220</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2101,21 +2137,27 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D15" s="4">
+        <v>42693</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>214</v>
+      <c r="H15" t="s">
+        <v>221</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="O15" s="4">
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2126,21 +2168,27 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="D16" s="4">
+        <v>42693</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>199</v>
+      <c r="H16" t="s">
+        <v>222</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="O16" s="4">
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2151,21 +2199,27 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
+      <c r="D17" s="4">
+        <v>42696</v>
+      </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>200</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>200</v>
+        <v>223</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="O17" s="4">
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2176,21 +2230,27 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
+      <c r="D18" s="4">
+        <v>42697</v>
+      </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>201</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>201</v>
+        <v>227</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="O18" s="4">
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2215,7 +2275,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2240,7 +2300,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2265,7 +2325,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2290,7 +2350,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2315,7 +2375,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2340,7 +2400,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2365,7 +2425,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2390,7 +2450,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2415,7 +2475,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2440,7 +2500,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2465,7 +2525,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2490,7 +2550,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2515,7 +2575,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2540,7 +2600,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2575,11 +2635,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2593,7 +2653,7 @@
     <col min="18" max="18" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2618,7 +2678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2731,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2737,7 +2797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2807,7 +2867,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2874,7 +2934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2941,7 +3001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3008,7 +3068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3071,14 +3131,14 @@
       </c>
       <c r="R8" t="str">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7: String umdrehen</v>
+        <v>7:11-7:60</v>
       </c>
       <c r="S8" s="47">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3130,11 +3190,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Objekte/Instanzen: Graphische Notation</v>
+        <v>7:60-Ende; 8:1-34</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: self-lose Methoden</v>
+        <v>8:35-75</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3145,7 +3205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3200,11 +3260,11 @@
       </c>
       <c r="P10" t="str">
         <f>VLOOKUP(M10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Punkt: Abstand bestimmen</v>
+        <v>8:75-100(5)</v>
       </c>
       <c r="Q10" t="str">
         <f>VLOOKUP(N10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>9: Gemeinsamkeiten in Klassen fassen</v>
+        <v>8:100-Ende; 9:1-32</v>
       </c>
       <c r="R10" t="str">
         <f>VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
@@ -3215,7 +3275,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3269,20 +3329,20 @@
         <f>VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>9: Ende</v>
       </c>
-      <c r="Q11" t="str">
-        <f>VLOOKUP(M11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>9: Ende</v>
-      </c>
-      <c r="R11" t="str">
+      <c r="Q11" s="47" t="str">
         <f>VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>10: try in try</v>
+      </c>
+      <c r="R11" s="47" t="e">
+        <f>VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="S11" s="47">
         <f>MAX(M11:N11)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3352,7 +3412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3419,7 +3479,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3489,7 +3549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3559,7 +3619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3674,7 +3734,7 @@
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3684,7 +3744,7 @@
     <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3712,7 +3772,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -3766,7 +3826,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3839,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3907,7 +3967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3975,7 +4035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4043,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4111,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4164,7 +4224,7 @@
       </c>
       <c r="Q8" t="str">
         <f>VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>7: String umdrehen</v>
+        <v>7:11-7:60</v>
       </c>
       <c r="R8" t="e">
         <f>VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4179,7 +4239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4228,11 +4288,11 @@
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(M9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Objekte/Instanzen: Graphische Notation</v>
+        <v>7:60-Ende; 8:1-34</v>
       </c>
       <c r="Q9" t="str">
         <f>VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: self-lose Methoden</v>
+        <v>8:35-75</v>
       </c>
       <c r="R9" t="e">
         <f>VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4247,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4299,11 +4359,11 @@
       </c>
       <c r="P10" t="str">
         <f>VLOOKUP(M10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>8: Punkt: Abstand bestimmen</v>
+        <v>8:75-100(5)</v>
       </c>
       <c r="Q10" t="str">
         <f>VLOOKUP(N10,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>9: Gemeinsamkeiten in Klassen fassen</v>
+        <v>8:100-Ende; 9:1-32</v>
       </c>
       <c r="R10" t="str">
         <f>VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
@@ -4318,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4386,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4457,7 +4517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4525,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4596,7 +4656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4705,9 +4765,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
@@ -4739,7 +4799,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4778,7 +4838,7 @@
       </c>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4821,7 +4881,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4870,7 +4930,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +4981,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
@@ -4969,7 +5029,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -5024,7 +5084,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>72</v>
       </c>
@@ -5079,7 +5139,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>73</v>
       </c>
@@ -5124,7 +5184,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
@@ -5178,7 +5238,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
@@ -5203,7 +5263,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -5266,7 +5326,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -5329,7 +5389,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -5392,7 +5452,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5455,7 +5515,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5518,7 +5578,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -5581,7 +5641,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -5644,7 +5704,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -5707,7 +5767,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -5765,7 +5825,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D22" s="40">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -5858,9 +5918,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>90</v>
       </c>
@@ -5886,7 +5946,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>83</v>
       </c>
@@ -5903,7 +5963,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>82</v>
       </c>
@@ -5920,7 +5980,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>88</v>
       </c>
@@ -5937,7 +5997,7 @@
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>87</v>
       </c>
@@ -5954,7 +6014,7 @@
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>89</v>
       </c>
@@ -5971,7 +6031,7 @@
       </c>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>86</v>
       </c>
@@ -5986,7 +6046,7 @@
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>85</v>
       </c>
@@ -6001,7 +6061,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>81</v>
       </c>
@@ -6018,7 +6078,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
         <v>84</v>
       </c>
@@ -6053,9 +6113,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -6063,7 +6123,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>102</v>
       </c>
@@ -6105,7 +6165,7 @@
       </c>
       <c r="U2" s="32"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="26">
         <v>1</v>
       </c>
@@ -6153,7 +6213,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="26">
         <v>2</v>
       </c>
@@ -6199,7 +6259,7 @@
       </c>
       <c r="U4" s="47"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
         <v>3</v>
       </c>
@@ -6251,7 +6311,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
         <v>4</v>
       </c>
@@ -6297,7 +6357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -6338,7 +6398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>6</v>
       </c>
@@ -6384,7 +6444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -6430,7 +6490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="26">
         <v>8</v>
       </c>
@@ -6481,7 +6541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <v>9</v>
       </c>
@@ -6527,7 +6587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>10</v>
       </c>
@@ -6568,7 +6628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>11</v>
       </c>
@@ -6622,7 +6682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>12</v>
       </c>
@@ -6663,7 +6723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
         <v>13</v>
       </c>
@@ -6714,7 +6774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
         <v>14</v>
       </c>
@@ -6760,7 +6820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
         <v>15</v>
       </c>
@@ -6811,7 +6871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="26">
         <v>16</v>
       </c>
@@ -6860,7 +6920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
         <v>17</v>
       </c>
@@ -6901,7 +6961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="26">
         <v>18</v>
       </c>
@@ -6957,7 +7017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <v>19</v>
       </c>
@@ -7001,7 +7061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="26">
         <v>20</v>
       </c>
@@ -7047,7 +7107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
         <v>21</v>
       </c>
@@ -7091,7 +7151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
         <v>22</v>
       </c>
@@ -7142,7 +7202,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
         <v>23</v>
       </c>
@@ -7193,7 +7253,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="26">
         <v>24</v>
       </c>
@@ -7239,7 +7299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <v>25</v>
       </c>
@@ -7290,7 +7350,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="26">
         <v>26</v>
       </c>
@@ -7336,7 +7396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
         <v>27</v>
       </c>
@@ -7382,7 +7442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="26">
         <v>28</v>
       </c>
@@ -7423,7 +7483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <v>29</v>
       </c>
@@ -7468,7 +7528,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="26">
         <v>30</v>
       </c>
@@ -7507,7 +7567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Marked PÜ8 as ready-to-upload
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" state="visible" r:id="rId2"/>
@@ -806,7 +806,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -817,6 +817,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9BBB59"/>
         <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF009933"/>
       </patternFill>
     </fill>
     <fill>
@@ -1082,7 +1088,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1131,19 +1137,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1151,11 +1161,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1163,7 +1173,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,7 +1205,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1275,19 +1285,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1315,6 +1321,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1325,7 +1335,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="9">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1443,169 +1453,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1676,9 +1530,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2393,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2554,13 +2408,13 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3115,8 +2969,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -3633,7 +3487,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3654,7 +3508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4667,7 +4521,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4682,13 +4536,13 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4769,35 +4623,35 @@
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -4842,7 +4696,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4863,38 +4717,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="13" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4902,83 +4756,83 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="15" t="n">
+      <c r="E3" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="G3" s="15" t="n">
+      <c r="G3" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="14" t="n">
+      <c r="H3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="15" t="n">
+      <c r="I3" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="14" t="n">
+      <c r="J3" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="K3" s="14" t="n">
+      <c r="K3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="14" t="n">
+      <c r="L3" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="14" t="n">
+      <c r="M3" s="15" t="n">
         <v>2</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P3" s="16"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="17" t="n">
+      <c r="D4" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="18" t="n">
         <v>13</v>
       </c>
-      <c r="G4" s="18" t="n">
+      <c r="G4" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="I4" s="18" t="n">
+      <c r="I4" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="J4" s="17" t="n">
+      <c r="J4" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="L4" s="17" t="n">
+      <c r="L4" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="M4" s="17" t="n">
+      <c r="M4" s="18" t="n">
         <v>14</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
@@ -4986,48 +4840,48 @@
       <c r="C5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="17" t="n">
+      <c r="D5" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="17" t="n">
+      <c r="F5" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="18" t="n">
+      <c r="G5" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="18" t="n">
+      <c r="I5" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="17" t="n">
+      <c r="J5" s="18" t="n">
         <f aca="false">SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="18" t="n">
         <f aca="false">SUMPRODUCT(K6:K8,C6:C8)</f>
         <v>16</v>
       </c>
-      <c r="L5" s="17" t="n">
+      <c r="L5" s="18" t="n">
         <f aca="false">SUM(C6:C8)</f>
         <v>9</v>
       </c>
-      <c r="M5" s="17" t="n">
+      <c r="M5" s="18" t="n">
         <f aca="false">SUM(C6:C8)</f>
         <v>9</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -5061,7 +4915,7 @@
       <c r="J6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="20" t="n">
+      <c r="K6" s="21" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="2" t="n">
@@ -5074,11 +4928,11 @@
         <f aca="false">SUMPRODUCT(D6:M6,D$10:M$10,D$11:M$11)</f>
         <v>174.666666666667</v>
       </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
@@ -5122,11 +4976,11 @@
         <f aca="false">SUMPRODUCT(D7:M7,D$10:M$10,D$11:M$11)</f>
         <v>254</v>
       </c>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
@@ -5177,54 +5031,54 @@
         <f aca="false">SUMPRODUCT(D8:M8,D$10:M$10,D$11:M$11)</f>
         <v>162</v>
       </c>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21" t="n">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,D6:D8)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="21" t="n">
+      <c r="E9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,E6:E8)</f>
         <v>5</v>
       </c>
-      <c r="F9" s="21" t="n">
+      <c r="F9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,F6:F8)</f>
         <v>3</v>
       </c>
-      <c r="G9" s="21" t="n">
+      <c r="G9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,G6:G8)</f>
         <v>5</v>
       </c>
-      <c r="H9" s="21" t="n">
+      <c r="H9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,H6:H8)</f>
         <v>3</v>
       </c>
-      <c r="I9" s="21" t="n">
+      <c r="I9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,I6:I8)</f>
         <v>3</v>
       </c>
-      <c r="J9" s="21" t="n">
+      <c r="J9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,J6:J8)</f>
         <v>9</v>
       </c>
-      <c r="K9" s="21" t="n">
+      <c r="K9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,K6:K8)</f>
         <v>16</v>
       </c>
-      <c r="L9" s="21" t="n">
+      <c r="L9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,L6:L8)</f>
         <v>10</v>
       </c>
-      <c r="M9" s="21" t="n">
+      <c r="M9" s="22" t="n">
         <f aca="false">SUMPRODUCT($C6:$C8,M6:M8)</f>
         <v>9</v>
       </c>
@@ -5232,53 +5086,53 @@
         <f aca="false">SUMPRODUCT(N6:N8,C6:C8)</f>
         <v>1864</v>
       </c>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-    </row>
-    <row r="10" s="16" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16" t="s">
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+    </row>
+    <row r="10" s="17" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="17" t="n">
         <f aca="false">1/D9</f>
         <v>0.2</v>
       </c>
-      <c r="E10" s="16" t="n">
+      <c r="E10" s="17" t="n">
         <f aca="false">1/E9</f>
         <v>0.2</v>
       </c>
-      <c r="F10" s="16" t="n">
+      <c r="F10" s="17" t="n">
         <f aca="false">1/F9</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="G10" s="16" t="n">
+      <c r="G10" s="17" t="n">
         <f aca="false">1/G9</f>
         <v>0.2</v>
       </c>
-      <c r="H10" s="16" t="n">
+      <c r="H10" s="17" t="n">
         <f aca="false">1/H9</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="I10" s="16" t="n">
+      <c r="I10" s="17" t="n">
         <f aca="false">1/I9</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="J10" s="16" t="n">
+      <c r="J10" s="17" t="n">
         <f aca="false">1/J9</f>
         <v>0.111111111111111</v>
       </c>
-      <c r="K10" s="16" t="n">
+      <c r="K10" s="17" t="n">
         <f aca="false">1/K9</f>
         <v>0.0625</v>
       </c>
-      <c r="L10" s="16" t="n">
+      <c r="L10" s="17" t="n">
         <f aca="false">1/L9</f>
         <v>0.1</v>
       </c>
-      <c r="M10" s="16" t="n">
+      <c r="M10" s="17" t="n">
         <f aca="false">1/M9</f>
         <v>0.111111111111111</v>
       </c>
@@ -5331,11 +5185,11 @@
         <f aca="false">SUM(D11:M11)</f>
         <v>1864</v>
       </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -5350,17 +5204,17 @@
       <c r="D12" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="O12" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="19"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="20"/>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -5372,58 +5226,58 @@
       <c r="C13" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="23" t="n">
+      <c r="D13" s="24" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="24" t="n">
+      <c r="E13" s="25" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B13)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="25" t="n">
+      <c r="F13" s="26" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B13)</f>
         <v>5</v>
       </c>
-      <c r="G13" s="25" t="n">
+      <c r="G13" s="26" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L16,Tutoren!$B13)</f>
         <v>4</v>
       </c>
-      <c r="H13" s="25" t="n">
+      <c r="H13" s="26" t="n">
         <f aca="false">F13</f>
         <v>5</v>
       </c>
-      <c r="I13" s="24" t="n">
+      <c r="I13" s="25" t="n">
         <f aca="false">H13</f>
         <v>5</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="25" t="n">
         <v>14</v>
       </c>
-      <c r="K13" s="24" t="n">
+      <c r="K13" s="25" t="n">
         <f aca="false">VLOOKUP($C13,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L13" s="26" t="n">
+      <c r="L13" s="27" t="n">
         <f aca="false">VLOOKUP($C13,$B$6:$L$9,11,0)*L$4</f>
         <v>0</v>
       </c>
-      <c r="M13" s="27" t="n">
+      <c r="M13" s="28" t="n">
         <f aca="false">VLOOKUP($C13,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N13" s="14" t="n">
+      <c r="N13" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D13:M13)</f>
         <v>194</v>
       </c>
-      <c r="O13" s="28" t="n">
+      <c r="O13" s="29" t="n">
         <f aca="false">VLOOKUP(C13,B$6:N$8,13,0)</f>
         <v>174.666666666667</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -5435,58 +5289,58 @@
       <c r="C14" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B14)</f>
         <v>1</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B14)</f>
         <v>4</v>
       </c>
-      <c r="F14" s="31" t="n">
+      <c r="F14" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B14)</f>
         <v>4</v>
       </c>
-      <c r="G14" s="31" t="n">
+      <c r="G14" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L17,Tutoren!$B14)</f>
         <v>5</v>
       </c>
-      <c r="H14" s="31" t="n">
+      <c r="H14" s="32" t="n">
         <f aca="false">F14</f>
         <v>4</v>
       </c>
-      <c r="I14" s="30" t="n">
+      <c r="I14" s="31" t="n">
         <f aca="false">H14</f>
         <v>4</v>
       </c>
-      <c r="J14" s="30" t="n">
+      <c r="J14" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K14" s="30" t="n">
+      <c r="K14" s="31" t="n">
         <f aca="false">VLOOKUP($C14,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L14" s="32" t="n">
+      <c r="L14" s="33" t="n">
         <f aca="false">VLOOKUP($C14,$B$6:$L$9,11,0)*L$4</f>
         <v>0</v>
       </c>
-      <c r="M14" s="33" t="n">
+      <c r="M14" s="34" t="n">
         <f aca="false">VLOOKUP($C14,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N14" s="14" t="n">
+      <c r="N14" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D14:M14)</f>
         <v>188</v>
       </c>
-      <c r="O14" s="28" t="n">
+      <c r="O14" s="29" t="n">
         <f aca="false">VLOOKUP(C14,B$6:N$8,13,0)</f>
         <v>174.666666666667</v>
       </c>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -5498,58 +5352,58 @@
       <c r="C15" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="34" t="n">
+      <c r="D15" s="35" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="35" t="n">
+      <c r="E15" s="36" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B15)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="36" t="n">
+      <c r="F15" s="37" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B15)</f>
         <v>4</v>
       </c>
-      <c r="G15" s="36" t="n">
+      <c r="G15" s="37" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L18,Tutoren!$B15)</f>
         <v>4</v>
       </c>
-      <c r="H15" s="36" t="n">
+      <c r="H15" s="37" t="n">
         <f aca="false">F15</f>
         <v>4</v>
       </c>
-      <c r="I15" s="35" t="n">
+      <c r="I15" s="36" t="n">
         <f aca="false">H15</f>
         <v>4</v>
       </c>
-      <c r="J15" s="35" t="n">
+      <c r="J15" s="36" t="n">
         <v>14</v>
       </c>
-      <c r="K15" s="35" t="n">
+      <c r="K15" s="36" t="n">
         <f aca="false">VLOOKUP($C15,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L15" s="37" t="n">
+      <c r="L15" s="38" t="n">
         <f aca="false">VLOOKUP($C15,$B$6:$L$9,11,0)*L$4</f>
         <v>0</v>
       </c>
-      <c r="M15" s="38" t="n">
+      <c r="M15" s="39" t="n">
         <f aca="false">VLOOKUP($C15,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N15" s="14" t="n">
+      <c r="N15" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D15:M15)</f>
         <v>183</v>
       </c>
-      <c r="O15" s="28" t="n">
+      <c r="O15" s="29" t="n">
         <f aca="false">VLOOKUP(C15,B$6:N$8,13,0)</f>
         <v>174.666666666667</v>
       </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -5561,58 +5415,58 @@
       <c r="C16" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="29" t="n">
+      <c r="D16" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B16)</f>
         <v>2</v>
       </c>
-      <c r="E16" s="30" t="n">
+      <c r="E16" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B16)</f>
         <v>3</v>
       </c>
-      <c r="F16" s="31" t="n">
+      <c r="F16" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="31" t="n">
+      <c r="G16" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L19,Tutoren!$B16)</f>
         <v>2</v>
       </c>
-      <c r="H16" s="31" t="n">
+      <c r="H16" s="32" t="n">
         <f aca="false">F16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="30" t="n">
+      <c r="I16" s="31" t="n">
         <f aca="false">H16</f>
         <v>0</v>
       </c>
-      <c r="J16" s="30" t="n">
+      <c r="J16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K16" s="30" t="n">
+      <c r="K16" s="31" t="n">
         <f aca="false">VLOOKUP($C16,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L16" s="32" t="n">
+      <c r="L16" s="33" t="n">
         <f aca="false">VLOOKUP($C16,$B$6:$L$9,11,0)*L$4</f>
         <v>28</v>
       </c>
-      <c r="M16" s="33" t="n">
+      <c r="M16" s="34" t="n">
         <f aca="false">VLOOKUP($C16,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N16" s="14" t="n">
+      <c r="N16" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D16:M16)</f>
         <v>253</v>
       </c>
-      <c r="O16" s="28" t="n">
+      <c r="O16" s="29" t="n">
         <f aca="false">VLOOKUP(C16,B$6:N$8,13,0)</f>
         <v>254</v>
       </c>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -5624,58 +5478,58 @@
       <c r="C17" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D17" s="29" t="n">
+      <c r="D17" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B17)</f>
         <v>1</v>
       </c>
-      <c r="E17" s="30" t="n">
+      <c r="E17" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B17)</f>
         <v>3</v>
       </c>
-      <c r="F17" s="31" t="n">
+      <c r="F17" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="31" t="n">
+      <c r="G17" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L20,Tutoren!$B17)</f>
         <v>1</v>
       </c>
-      <c r="H17" s="31" t="n">
+      <c r="H17" s="32" t="n">
         <f aca="false">F17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="30" t="n">
+      <c r="I17" s="31" t="n">
         <f aca="false">H17</f>
         <v>0</v>
       </c>
-      <c r="J17" s="30" t="n">
+      <c r="J17" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K17" s="30" t="n">
+      <c r="K17" s="31" t="n">
         <f aca="false">VLOOKUP($C17,$B$6:$L$9,10,0)*K$4</f>
         <v>14</v>
       </c>
-      <c r="L17" s="32" t="n">
+      <c r="L17" s="33" t="n">
         <f aca="false">VLOOKUP($C17,$B$6:$L$9,11,0)*L$4</f>
         <v>14</v>
       </c>
-      <c r="M17" s="33" t="n">
+      <c r="M17" s="34" t="n">
         <f aca="false">VLOOKUP($C17,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N17" s="14" t="n">
+      <c r="N17" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D17:M17)</f>
         <v>163</v>
       </c>
-      <c r="O17" s="28" t="n">
+      <c r="O17" s="29" t="n">
         <f aca="false">VLOOKUP(C17,B$6:N$8,13,0)</f>
         <v>162</v>
       </c>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -5687,58 +5541,58 @@
       <c r="C18" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="29" t="n">
+      <c r="D18" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B18)</f>
         <v>1</v>
       </c>
-      <c r="E18" s="30" t="n">
+      <c r="E18" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B18)</f>
         <v>2</v>
       </c>
-      <c r="F18" s="31" t="n">
+      <c r="F18" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B18)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="31" t="n">
+      <c r="G18" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L21,Tutoren!$B18)</f>
         <v>1</v>
       </c>
-      <c r="H18" s="31" t="n">
+      <c r="H18" s="32" t="n">
         <f aca="false">F18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="30" t="n">
+      <c r="I18" s="31" t="n">
         <f aca="false">H18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="30" t="n">
+      <c r="J18" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K18" s="30" t="n">
+      <c r="K18" s="31" t="n">
         <f aca="false">VLOOKUP($C18,$B$6:$L$9,10,0)*K$4</f>
         <v>14</v>
       </c>
-      <c r="L18" s="32" t="n">
+      <c r="L18" s="33" t="n">
         <f aca="false">VLOOKUP($C18,$B$6:$L$9,11,0)*L$4</f>
         <v>14</v>
       </c>
-      <c r="M18" s="33" t="n">
+      <c r="M18" s="34" t="n">
         <f aca="false">VLOOKUP($C18,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N18" s="14" t="n">
+      <c r="N18" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D18:M18)</f>
         <v>162</v>
       </c>
-      <c r="O18" s="28" t="n">
+      <c r="O18" s="29" t="n">
         <f aca="false">VLOOKUP(C18,B$6:N$8,13,0)</f>
         <v>162</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -5750,58 +5604,58 @@
       <c r="C19" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="29" t="n">
+      <c r="D19" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B19)</f>
         <v>3</v>
       </c>
-      <c r="E19" s="30" t="n">
+      <c r="E19" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B19)</f>
         <v>3</v>
       </c>
-      <c r="F19" s="31" t="n">
+      <c r="F19" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B19)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="31" t="n">
+      <c r="G19" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L22,Tutoren!$B19)</f>
         <v>3</v>
       </c>
-      <c r="H19" s="31" t="n">
+      <c r="H19" s="32" t="n">
         <f aca="false">F19</f>
         <v>0</v>
       </c>
-      <c r="I19" s="30" t="n">
+      <c r="I19" s="31" t="n">
         <f aca="false">H19</f>
         <v>0</v>
       </c>
-      <c r="J19" s="30" t="n">
+      <c r="J19" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K19" s="30" t="n">
+      <c r="K19" s="31" t="n">
         <f aca="false">VLOOKUP($C19,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L19" s="32" t="n">
+      <c r="L19" s="33" t="n">
         <f aca="false">VLOOKUP($C19,$B$6:$L$9,11,0)*L$4</f>
         <v>28</v>
       </c>
-      <c r="M19" s="33" t="n">
+      <c r="M19" s="34" t="n">
         <f aca="false">VLOOKUP($C19,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N19" s="14" t="n">
+      <c r="N19" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D19:M19)</f>
         <v>259</v>
       </c>
-      <c r="O19" s="28" t="n">
+      <c r="O19" s="29" t="n">
         <f aca="false">VLOOKUP(C19,B$6:N$8,13,0)</f>
         <v>254</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -5813,58 +5667,58 @@
       <c r="C20" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="29" t="n">
+      <c r="D20" s="30" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B20)</f>
         <v>2</v>
       </c>
-      <c r="E20" s="30" t="n">
+      <c r="E20" s="31" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B20)</f>
         <v>2</v>
       </c>
-      <c r="F20" s="31" t="n">
+      <c r="F20" s="32" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B20)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="31" t="n">
+      <c r="G20" s="32" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L23,Tutoren!$B20)</f>
         <v>3</v>
       </c>
-      <c r="H20" s="31" t="n">
+      <c r="H20" s="32" t="n">
         <f aca="false">F20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="30" t="n">
+      <c r="I20" s="31" t="n">
         <f aca="false">H20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="30" t="n">
+      <c r="J20" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="K20" s="30" t="n">
+      <c r="K20" s="31" t="n">
         <f aca="false">VLOOKUP($C20,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L20" s="32" t="n">
+      <c r="L20" s="33" t="n">
         <f aca="false">VLOOKUP($C20,$B$6:$L$9,11,0)*L$4</f>
         <v>28</v>
       </c>
-      <c r="M20" s="33" t="n">
+      <c r="M20" s="34" t="n">
         <f aca="false">VLOOKUP($C20,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N20" s="14" t="n">
+      <c r="N20" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D20:M20)</f>
         <v>254</v>
       </c>
-      <c r="O20" s="28" t="n">
+      <c r="O20" s="29" t="n">
         <f aca="false">VLOOKUP(C20,B$6:N$8,13,0)</f>
         <v>254</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -5876,108 +5730,108 @@
       <c r="C21" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D21" s="39" t="n">
+      <c r="D21" s="40" t="n">
         <f aca="false">COUNTIF(PUE!J$3:J$16,Tutoren!$B21)</f>
         <v>3</v>
       </c>
-      <c r="E21" s="40" t="n">
+      <c r="E21" s="41" t="n">
         <f aca="false">COUNTIF(PUE!K$3:L$16,$B21)</f>
         <v>1</v>
       </c>
-      <c r="F21" s="41" t="n">
+      <c r="F21" s="42" t="n">
         <f aca="false">COUNTIF(HUE!J$3:J$16,Tutoren!$B21)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="41" t="n">
+      <c r="G21" s="42" t="n">
         <f aca="false">COUNTIF(HUE!K$3:$L24,Tutoren!$B21)</f>
         <v>3</v>
       </c>
-      <c r="H21" s="41" t="n">
+      <c r="H21" s="42" t="n">
         <f aca="false">F21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="40" t="n">
+      <c r="I21" s="41" t="n">
         <f aca="false">H21</f>
         <v>0</v>
       </c>
-      <c r="J21" s="40" t="n">
+      <c r="J21" s="41" t="n">
         <v>14</v>
       </c>
-      <c r="K21" s="40" t="n">
+      <c r="K21" s="41" t="n">
         <f aca="false">VLOOKUP($C21,$B$6:$L$9,10,0)*K$4</f>
         <v>28</v>
       </c>
-      <c r="L21" s="42" t="n">
+      <c r="L21" s="43" t="n">
         <f aca="false">VLOOKUP($C21,$B$6:$L$9,11,0)*L$4</f>
         <v>28</v>
       </c>
-      <c r="M21" s="43" t="n">
+      <c r="M21" s="44" t="n">
         <f aca="false">VLOOKUP($C21,$B$6:$M$9,12,0)*M$4</f>
         <v>14</v>
       </c>
-      <c r="N21" s="14" t="n">
+      <c r="N21" s="15" t="n">
         <f aca="false">SUMPRODUCT(D$3:M$3,D21:M21)</f>
         <v>257</v>
       </c>
-      <c r="O21" s="28" t="n">
+      <c r="O21" s="29" t="n">
         <f aca="false">VLOOKUP(C21,B$6:N$8,13,0)</f>
         <v>254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="44" t="n">
+      <c r="D22" s="45" t="n">
         <f aca="false">D3*SUM(D13:D21)</f>
         <v>52</v>
       </c>
-      <c r="E22" s="44" t="n">
+      <c r="E22" s="45" t="n">
         <f aca="false">E3*SUM(E13:E21)</f>
         <v>28</v>
       </c>
-      <c r="F22" s="44" t="n">
+      <c r="F22" s="45" t="n">
         <f aca="false">F3*SUM(F13:F21)</f>
         <v>104</v>
       </c>
-      <c r="G22" s="44" t="n">
+      <c r="G22" s="45" t="n">
         <f aca="false">G3*SUM(G13:G21)</f>
         <v>52</v>
       </c>
-      <c r="H22" s="44" t="n">
+      <c r="H22" s="45" t="n">
         <f aca="false">H3*SUM(H13:H21)</f>
         <v>26</v>
       </c>
-      <c r="I22" s="44" t="n">
+      <c r="I22" s="45" t="n">
         <f aca="false">I3*SUM(I13:I21)</f>
         <v>13</v>
       </c>
-      <c r="J22" s="44" t="n">
+      <c r="J22" s="45" t="n">
         <f aca="false">J3*SUM(J13:J21)</f>
         <v>378</v>
       </c>
-      <c r="K22" s="44" t="n">
+      <c r="K22" s="45" t="n">
         <f aca="false">K3*SUM(K13:K21)</f>
         <v>448</v>
       </c>
-      <c r="L22" s="44" t="n">
+      <c r="L22" s="45" t="n">
         <f aca="false">L3*SUM(L13:L21)</f>
         <v>560</v>
       </c>
-      <c r="M22" s="44" t="n">
+      <c r="M22" s="45" t="n">
         <f aca="false">M3*SUM(M13:M21)</f>
         <v>252</v>
       </c>
-      <c r="N22" s="14" t="n">
+      <c r="N22" s="15" t="n">
         <f aca="false">SUM(N13:N21)</f>
         <v>1913</v>
       </c>
-      <c r="O22" s="14" t="n">
+      <c r="O22" s="15" t="n">
         <f aca="false">SUM(O13:O21)</f>
         <v>1864</v>
       </c>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N13:N21">
@@ -6006,7 +5860,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6027,7 +5881,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6057,158 +5911,158 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46" t="s">
+      <c r="G6" s="47"/>
+      <c r="H6" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="46"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46" t="s">
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="I10" s="46"/>
+      <c r="I10" s="47"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -6229,7 +6083,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6241,1424 +6095,1424 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="35" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="L2" s="35" t="s">
+      <c r="J2" s="37"/>
+      <c r="L2" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="35" t="s">
+      <c r="M2" s="37"/>
+      <c r="N2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="35" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="35" t="s">
+      <c r="Q2" s="37"/>
+      <c r="R2" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="35" t="s">
+      <c r="S2" s="37"/>
+      <c r="T2" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="U2" s="36"/>
+      <c r="U2" s="37"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="n">
+      <c r="A3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="30" t="n">
+      <c r="C3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="30" t="n">
+      <c r="E3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="30" t="n">
+      <c r="G3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="30" t="n">
+      <c r="I3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="L3" s="30" t="n">
+      <c r="L3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="30" t="n">
+      <c r="N3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="O3" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="P3" s="30" t="n">
+      <c r="P3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="R3" s="30" t="n">
+      <c r="R3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="T3" s="30" t="n">
+      <c r="T3" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="n">
+      <c r="A4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="30" t="n">
+      <c r="C4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="30" t="n">
+      <c r="E4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="G4" s="30" t="n">
+      <c r="G4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="30" t="n">
+      <c r="I4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="30" t="n">
+      <c r="L4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="N4" s="30" t="n">
+      <c r="N4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="P4" s="30" t="n">
+      <c r="P4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="R4" s="30" t="n">
+      <c r="R4" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="T4" s="30" t="n">
+      <c r="T4" s="31" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="n">
+      <c r="A5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="30" t="n">
+      <c r="C5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="n">
+      <c r="E5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="30" t="n">
+      <c r="G5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="30" t="n">
+      <c r="I5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="L5" s="30" t="n">
+      <c r="L5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="N5" s="30" t="n">
+      <c r="N5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="P5" s="30" t="n">
+      <c r="P5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="55" t="s">
+      <c r="Q5" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="R5" s="30" t="n">
+      <c r="R5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="S5" s="51" t="s">
+      <c r="S5" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="T5" s="30" t="n">
+      <c r="T5" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="U5" s="54" t="s">
+      <c r="U5" s="55" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="n">
+      <c r="A6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="30" t="n">
+      <c r="C6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="E6" s="30" t="n">
+      <c r="E6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="30" t="n">
+      <c r="G6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="30" t="n">
+      <c r="I6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="L6" s="30" t="n">
+      <c r="L6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="N6" s="30" t="n">
+      <c r="N6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="O6" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="P6" s="30" t="n">
+      <c r="P6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="57" t="s">
+      <c r="Q6" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="R6" s="30" t="n">
+      <c r="R6" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="T6" s="30" t="n">
+      <c r="T6" s="31" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="n">
+      <c r="A7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="30" t="n">
+      <c r="C7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="30" t="n">
+      <c r="E7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="30" t="n">
+      <c r="G7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="I7" s="30" t="n">
+      <c r="I7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="L7" s="30" t="n">
+      <c r="L7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="N7" s="30" t="n">
+      <c r="N7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="O7" s="55" t="s">
+      <c r="O7" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="P7" s="30" t="n">
+      <c r="P7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="R7" s="30" t="n">
+      <c r="R7" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="T7" s="30" t="n">
+      <c r="T7" s="31" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="n">
+      <c r="A8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="30" t="n">
+      <c r="C8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E8" s="30" t="n">
+      <c r="E8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="G8" s="30" t="n">
+      <c r="G8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="30" t="n">
+      <c r="I8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="L8" s="30" t="n">
+      <c r="L8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="N8" s="30" t="n">
+      <c r="N8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="O8" s="57" t="s">
+      <c r="O8" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="P8" s="30" t="n">
+      <c r="P8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="R8" s="30" t="n">
+      <c r="R8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="T8" s="30" t="n">
+      <c r="T8" s="31" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="n">
+      <c r="A9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="30" t="n">
+      <c r="C9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="30" t="n">
+      <c r="E9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="G9" s="30" t="n">
+      <c r="G9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="H9" s="48" t="s">
+      <c r="H9" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="I9" s="30" t="n">
+      <c r="I9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="L9" s="30" t="n">
+      <c r="L9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="N9" s="30" t="n">
+      <c r="N9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="P9" s="30" t="n">
+      <c r="P9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="52" t="s">
+      <c r="Q9" s="53" t="s">
         <v>191</v>
       </c>
-      <c r="R9" s="30" t="n">
+      <c r="R9" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="S9" s="55" t="s">
+      <c r="S9" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="T9" s="30" t="n">
+      <c r="T9" s="31" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="n">
+      <c r="A10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="30" t="n">
+      <c r="C10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="30" t="n">
+      <c r="E10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="G10" s="30" t="n">
+      <c r="G10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="I10" s="30" t="n">
+      <c r="I10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="L10" s="30" t="n">
+      <c r="L10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="N10" s="30" t="n">
+      <c r="N10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="O10" s="51" t="s">
+      <c r="O10" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="P10" s="30" t="n">
+      <c r="P10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="R10" s="30" t="n">
+      <c r="R10" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="S10" s="57" t="s">
+      <c r="S10" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="T10" s="30" t="n">
+      <c r="T10" s="31" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="n">
+      <c r="A11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="30" t="n">
+      <c r="C11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="E11" s="30" t="n">
+      <c r="E11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="G11" s="30" t="n">
+      <c r="G11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="I11" s="30" t="n">
+      <c r="I11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="L11" s="30" t="n">
+      <c r="L11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="N11" s="30" t="n">
+      <c r="N11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="O11" s="52" t="s">
+      <c r="O11" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="P11" s="30" t="n">
+      <c r="P11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" s="54" t="s">
+      <c r="Q11" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="R11" s="30" t="n">
+      <c r="R11" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="T11" s="30" t="n">
+      <c r="T11" s="31" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="n">
+      <c r="A12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="30" t="n">
+      <c r="C12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="E12" s="30" t="n">
+      <c r="E12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="G12" s="30" t="n">
+      <c r="G12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="I12" s="30" t="n">
+      <c r="I12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="L12" s="30" t="n">
+      <c r="L12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="N12" s="30" t="n">
+      <c r="N12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="P12" s="30" t="n">
+      <c r="P12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="R12" s="30" t="n">
+      <c r="R12" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="S12" s="51" t="s">
+      <c r="S12" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="T12" s="30" t="n">
+      <c r="T12" s="31" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="n">
+      <c r="A13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="30" t="n">
+      <c r="C13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="E13" s="30" t="n">
+      <c r="E13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="G13" s="30" t="n">
+      <c r="G13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="H13" s="50" t="s">
+      <c r="H13" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="I13" s="30" t="n">
+      <c r="I13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="L13" s="30" t="n">
+      <c r="L13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="N13" s="30" t="n">
+      <c r="N13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="55" t="s">
         <v>179</v>
       </c>
-      <c r="P13" s="30" t="n">
+      <c r="P13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="Q13" s="57" t="s">
+      <c r="Q13" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="R13" s="30" t="n">
+      <c r="R13" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="T13" s="30" t="n">
+      <c r="T13" s="31" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="n">
+      <c r="A14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="I14" s="30" t="n">
+      <c r="I14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="L14" s="30" t="n">
+      <c r="L14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="N14" s="30" t="n">
+      <c r="N14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="O14" s="55" t="s">
+      <c r="O14" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="P14" s="30" t="n">
+      <c r="P14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="R14" s="30" t="n">
+      <c r="R14" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="T14" s="30" t="n">
+      <c r="T14" s="31" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="n">
+      <c r="A15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="C15" s="30" t="n">
+      <c r="C15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="E15" s="30" t="n">
+      <c r="E15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="G15" s="30" t="n">
+      <c r="G15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="H15" s="53" t="s">
+      <c r="H15" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="I15" s="30" t="n">
+      <c r="I15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="L15" s="30" t="n">
+      <c r="L15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="N15" s="30" t="n">
+      <c r="N15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="O15" s="57" t="s">
+      <c r="O15" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="P15" s="30" t="n">
+      <c r="P15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="Q15" s="51" t="s">
+      <c r="Q15" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="R15" s="30" t="n">
+      <c r="R15" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="S15" s="54" t="s">
+      <c r="S15" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="T15" s="30" t="n">
+      <c r="T15" s="31" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="n">
+      <c r="A16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="C16" s="30" t="n">
+      <c r="C16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="E16" s="30" t="n">
+      <c r="E16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="G16" s="30" t="n">
+      <c r="G16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="I16" s="30" t="n">
+      <c r="I16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="L16" s="30" t="n">
+      <c r="L16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="N16" s="30" t="n">
+      <c r="N16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="P16" s="30" t="n">
+      <c r="P16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="Q16" s="52" t="s">
+      <c r="Q16" s="53" t="s">
         <v>189</v>
       </c>
-      <c r="R16" s="30" t="n">
+      <c r="R16" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="S16" s="55" t="s">
+      <c r="S16" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="T16" s="30" t="n">
+      <c r="T16" s="31" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="n">
+      <c r="A17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="30" t="n">
+      <c r="C17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="E17" s="30" t="n">
+      <c r="E17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="G17" s="30" t="n">
+      <c r="G17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="H17" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="I17" s="30" t="n">
+      <c r="I17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="L17" s="30" t="n">
+      <c r="L17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="M17" s="55" t="s">
+      <c r="M17" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="N17" s="30" t="n">
+      <c r="N17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="O17" s="51" t="s">
+      <c r="O17" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="P17" s="30" t="n">
+      <c r="P17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="R17" s="30" t="n">
+      <c r="R17" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="S17" s="57" t="s">
+      <c r="S17" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="T17" s="30" t="n">
+      <c r="T17" s="31" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="n">
+      <c r="A18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="30" t="n">
+      <c r="C18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="E18" s="30" t="n">
+      <c r="E18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="G18" s="30" t="n">
+      <c r="G18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="I18" s="30" t="n">
+      <c r="I18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="L18" s="30" t="n">
+      <c r="L18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="N18" s="30" t="n">
+      <c r="N18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="O18" s="52" t="s">
+      <c r="O18" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="P18" s="30" t="n">
+      <c r="P18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="Q18" s="54" t="s">
+      <c r="Q18" s="55" t="s">
         <v>198</v>
       </c>
-      <c r="R18" s="30" t="n">
+      <c r="R18" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="T18" s="30" t="n">
+      <c r="T18" s="31" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="n">
+      <c r="A19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="C19" s="30" t="n">
+      <c r="C19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="E19" s="30" t="n">
+      <c r="E19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="G19" s="30" t="n">
+      <c r="G19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="I19" s="30" t="n">
+      <c r="I19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="L19" s="30" t="n">
+      <c r="L19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="N19" s="30" t="n">
+      <c r="N19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="P19" s="30" t="n">
+      <c r="P19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="R19" s="30" t="n">
+      <c r="R19" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="S19" s="51" t="s">
+      <c r="S19" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="T19" s="30" t="n">
+      <c r="T19" s="31" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="n">
+      <c r="A20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="C20" s="30" t="n">
+      <c r="C20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="30" t="n">
+      <c r="E20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="G20" s="30" t="n">
+      <c r="G20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="H20" s="50" t="s">
+      <c r="H20" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="I20" s="30" t="n">
+      <c r="I20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="L20" s="30" t="n">
+      <c r="L20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="M20" s="51" t="s">
+      <c r="M20" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="N20" s="30" t="n">
+      <c r="N20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="O20" s="54" t="s">
+      <c r="O20" s="55" t="s">
         <v>201</v>
       </c>
-      <c r="P20" s="30" t="n">
+      <c r="P20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="Q20" s="57" t="s">
+      <c r="Q20" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="R20" s="30" t="n">
+      <c r="R20" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="S20" s="52" t="s">
+      <c r="S20" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="T20" s="30" t="n">
+      <c r="T20" s="31" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="n">
+      <c r="A21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="C21" s="30" t="n">
+      <c r="C21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="E21" s="30" t="n">
+      <c r="E21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="G21" s="30" t="n">
+      <c r="G21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="I21" s="30" t="n">
+      <c r="I21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="L21" s="30" t="n">
+      <c r="L21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="N21" s="30" t="n">
+      <c r="N21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="O21" s="55" t="s">
+      <c r="O21" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="P21" s="30" t="n">
+      <c r="P21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="R21" s="30" t="n">
+      <c r="R21" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="T21" s="30" t="n">
+      <c r="T21" s="31" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30" t="n">
+      <c r="A22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="C22" s="30" t="n">
+      <c r="C22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="57" t="s">
         <v>223</v>
       </c>
-      <c r="E22" s="30" t="n">
+      <c r="E22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="G22" s="30" t="n">
+      <c r="G22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="H22" s="53" t="s">
+      <c r="H22" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="I22" s="30" t="n">
+      <c r="I22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="L22" s="30" t="n">
+      <c r="L22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="N22" s="30" t="n">
+      <c r="N22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="O22" s="57" t="s">
+      <c r="O22" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="P22" s="30" t="n">
+      <c r="P22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="R22" s="30" t="n">
+      <c r="R22" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="S22" s="54" t="s">
+      <c r="S22" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="T22" s="30" t="n">
+      <c r="T22" s="31" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30" t="n">
+      <c r="A23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="30" t="n">
+      <c r="C23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="E23" s="30" t="n">
+      <c r="E23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="G23" s="30" t="n">
+      <c r="G23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="I23" s="30" t="n">
+      <c r="I23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="L23" s="30" t="n">
+      <c r="L23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="N23" s="30" t="n">
+      <c r="N23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="P23" s="30" t="n">
+      <c r="P23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="Q23" s="52" t="s">
+      <c r="Q23" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="R23" s="30" t="n">
+      <c r="R23" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="T23" s="30" t="n">
+      <c r="T23" s="31" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="n">
+      <c r="A24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="30" t="n">
+      <c r="C24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="E24" s="30" t="n">
+      <c r="E24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="G24" s="30" t="n">
+      <c r="G24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="H24" s="56" t="s">
+      <c r="H24" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="I24" s="30" t="n">
+      <c r="I24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="L24" s="30" t="n">
+      <c r="L24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="M24" s="55" t="s">
+      <c r="M24" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="N24" s="30" t="n">
+      <c r="N24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="O24" s="51" t="s">
+      <c r="O24" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="P24" s="30" t="n">
+      <c r="P24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="R24" s="30" t="n">
+      <c r="R24" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="S24" s="57" t="s">
+      <c r="S24" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="T24" s="30" t="n">
+      <c r="T24" s="31" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="n">
+      <c r="A25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="C25" s="30" t="n">
+      <c r="C25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="E25" s="30" t="n">
+      <c r="E25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="G25" s="30" t="n">
+      <c r="G25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="I25" s="30" t="n">
+      <c r="I25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="L25" s="30" t="n">
+      <c r="L25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="M25" s="57" t="s">
+      <c r="M25" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="N25" s="30" t="n">
+      <c r="N25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="O25" s="52" t="s">
+      <c r="O25" s="53" t="s">
         <v>215</v>
       </c>
-      <c r="P25" s="30" t="n">
+      <c r="P25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="Q25" s="54" t="s">
+      <c r="Q25" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="R25" s="30" t="n">
+      <c r="R25" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="T25" s="30" t="n">
+      <c r="T25" s="31" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="n">
+      <c r="A26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="C26" s="30" t="n">
+      <c r="C26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="E26" s="30" t="n">
+      <c r="E26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="49" t="s">
         <v>231</v>
       </c>
-      <c r="G26" s="30" t="n">
+      <c r="G26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="H26" s="49" t="s">
+      <c r="H26" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="I26" s="30" t="n">
+      <c r="I26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="L26" s="30" t="n">
+      <c r="L26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="N26" s="30" t="n">
+      <c r="N26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="P26" s="30" t="n">
+      <c r="P26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="Q26" s="55" t="s">
+      <c r="Q26" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="R26" s="30" t="n">
+      <c r="R26" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="S26" s="51" t="s">
+      <c r="S26" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="T26" s="30" t="n">
+      <c r="T26" s="31" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30" t="n">
+      <c r="A27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="30" t="n">
+      <c r="C27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D27" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="E27" s="30" t="n">
+      <c r="E27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="G27" s="30" t="n">
+      <c r="G27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="H27" s="50" t="s">
+      <c r="H27" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="I27" s="30" t="n">
+      <c r="I27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="L27" s="30" t="n">
+      <c r="L27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="M27" s="51" t="s">
+      <c r="M27" s="52" t="s">
         <v>218</v>
       </c>
-      <c r="N27" s="30" t="n">
+      <c r="N27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="O27" s="54" t="s">
+      <c r="O27" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="P27" s="30" t="n">
+      <c r="P27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="R27" s="30" t="n">
+      <c r="R27" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="S27" s="52" t="s">
+      <c r="S27" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="T27" s="30" t="n">
+      <c r="T27" s="31" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="n">
+      <c r="A28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="30" t="n">
+      <c r="C28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="E28" s="30" t="n">
+      <c r="E28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="G28" s="30" t="n">
+      <c r="G28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="I28" s="30" t="n">
+      <c r="I28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="L28" s="30" t="n">
+      <c r="L28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="M28" s="52" t="s">
+      <c r="M28" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="N28" s="30" t="n">
+      <c r="N28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="O28" s="55" t="s">
+      <c r="O28" s="56" t="s">
         <v>222</v>
       </c>
-      <c r="P28" s="30" t="n">
+      <c r="P28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="R28" s="30" t="n">
+      <c r="R28" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="T28" s="30" t="n">
+      <c r="T28" s="31" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30" t="n">
+      <c r="A29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="C29" s="30" t="n">
+      <c r="C29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="E29" s="30" t="n">
+      <c r="E29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="G29" s="30" t="n">
+      <c r="G29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="H29" s="53" t="s">
+      <c r="H29" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="30" t="n">
+      <c r="I29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="L29" s="30" t="n">
+      <c r="L29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="N29" s="30" t="n">
+      <c r="N29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="O29" s="57" t="s">
+      <c r="O29" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="P29" s="30" t="n">
+      <c r="P29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="R29" s="30" t="n">
+      <c r="R29" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="S29" s="54" t="s">
+      <c r="S29" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="T29" s="30" t="n">
+      <c r="T29" s="31" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30" t="n">
+      <c r="A30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="C30" s="30" t="n">
+      <c r="C30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="E30" s="30" t="n">
+      <c r="E30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="G30" s="30" t="n">
+      <c r="G30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="I30" s="30" t="n">
+      <c r="I30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="L30" s="30" t="n">
+      <c r="L30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="M30" s="54" t="s">
+      <c r="M30" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="N30" s="30" t="n">
+      <c r="N30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="P30" s="30" t="n">
+      <c r="P30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="R30" s="30" t="n">
+      <c r="R30" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="T30" s="30" t="n">
+      <c r="T30" s="31" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="n">
+      <c r="A31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="30" t="n">
+      <c r="C31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="30" t="n">
+      <c r="E31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="G31" s="30" t="n">
+      <c r="G31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="H31" s="56" t="s">
+      <c r="H31" s="57" t="s">
         <v>233</v>
       </c>
-      <c r="L31" s="30" t="n">
+      <c r="L31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="M31" s="55" t="s">
+      <c r="M31" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="N31" s="30" t="n">
+      <c r="N31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="O31" s="51" t="s">
+      <c r="O31" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="P31" s="30" t="n">
+      <c r="P31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="R31" s="30" t="n">
+      <c r="R31" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="S31" s="57" t="s">
+      <c r="S31" s="58" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="n">
+      <c r="A32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="30" t="n">
+      <c r="C32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="D32" s="50" t="s">
+      <c r="D32" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="30" t="n">
+      <c r="E32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="G32" s="30" t="n">
+      <c r="G32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="L32" s="30" t="n">
+      <c r="L32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="M32" s="57" t="s">
+      <c r="M32" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="N32" s="30" t="n">
+      <c r="N32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="O32" s="52" t="s">
+      <c r="O32" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="P32" s="30" t="n">
+      <c r="P32" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="R32" s="30" t="n">
+      <c r="R32" s="31" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="n">
+      <c r="A33" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="E33" s="30" t="n">
+      <c r="E33" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="F33" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="G33" s="30" t="n">
+      <c r="G33" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="L33" s="30" t="n">
+      <c r="L33" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="P33" s="30" t="n">
+      <c r="P33" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="Q33" s="55" t="s">
+      <c r="Q33" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="R33" s="30" t="n">
+      <c r="R33" s="31" t="n">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
fertig mit Korrektur JR
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="943" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,724 +17,729 @@
     <sheet name="Deadlines sortiert" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="238">
   <si>
-    <t>Aktuelles Semester</t>
-  </si>
-  <si>
-    <t>Vorlesungsnummer</t>
-  </si>
-  <si>
-    <t>Geplantes Datum</t>
-  </si>
-  <si>
-    <t>Geplante KW</t>
-  </si>
-  <si>
-    <t>Ist-Datum</t>
-  </si>
-  <si>
-    <t>Ist-KW</t>
-  </si>
-  <si>
-    <t>Gplantes Thema (bis einschliesslich)</t>
-  </si>
-  <si>
-    <t>Geplantes Kapitel</t>
-  </si>
-  <si>
-    <t>Ist-Kapitel</t>
-  </si>
-  <si>
-    <t>Ist-Thema</t>
-  </si>
-  <si>
-    <t>Ch 0;  Ch1: Datenstrukturen</t>
-  </si>
-  <si>
-    <t>0; 1:1-22</t>
-  </si>
-  <si>
-    <t>Ch 1, Versionsverwaltung</t>
-  </si>
-  <si>
-    <t>1:23-Ende</t>
-  </si>
-  <si>
-    <t>bis Ch1, Ausführungsmodell</t>
-  </si>
-  <si>
-    <t>Ch2, Zahldarstellung</t>
-  </si>
-  <si>
-    <t>2:1-19</t>
-  </si>
-  <si>
-    <t>einschließliche einfache Datentypen</t>
-  </si>
-  <si>
-    <t>Ch 3, Animation von Programmen</t>
-  </si>
-  <si>
-    <t>2:20-Ende; 3 komplett</t>
-  </si>
-  <si>
-    <t>Kapitel 3 komplett</t>
-  </si>
-  <si>
-    <t>Ch 4: Namenkonvention für Funktionsnamen</t>
-  </si>
-  <si>
-    <t>4:1-49</t>
-  </si>
-  <si>
-    <t>Kapitel 4: Funktionen mit Parameter: Aufruf mit Ausdruck</t>
-  </si>
-  <si>
-    <t>Ch 4: Pass-by-assignment</t>
-  </si>
-  <si>
-    <t>4:49-Ende; 5:1-12</t>
-  </si>
-  <si>
-    <t>Bis Slicing von Tuples</t>
-  </si>
-  <si>
-    <t>Ch 5, Slicing, Länge</t>
-  </si>
-  <si>
-    <t>5:12-Ende</t>
-  </si>
-  <si>
-    <t>Tuple, Listen, Dicts. Komplett; Sets ausgelassen</t>
-  </si>
-  <si>
-    <t>Ch 5: dicts, Operationen darauf</t>
-  </si>
-  <si>
-    <t>6:1-6:39</t>
-  </si>
-  <si>
-    <t>if; Anfang while bis Finden von Schleifeninvarianten</t>
-  </si>
-  <si>
-    <t>Ch 6: Eindeutigkeit von else</t>
-  </si>
-  <si>
-    <t>6:39-6:53</t>
-  </si>
-  <si>
-    <t>bis  einschlieslich list comprehensions</t>
-  </si>
-  <si>
-    <t>7:Funktionen rufen Funktionen</t>
-  </si>
-  <si>
-    <t>6:53-Ende; 7:1-7:11</t>
-  </si>
-  <si>
-    <t>7: Formale Parameter mit vorbelegten Werten</t>
-  </si>
-  <si>
-    <t>7: String umdrehen</t>
-  </si>
-  <si>
-    <t>7:11-7:60</t>
-  </si>
-  <si>
-    <t>8: Objekte/Instanzen: Graphische Notation</t>
-  </si>
-  <si>
-    <t>7:60-Ende; 8:1-34</t>
-  </si>
-  <si>
-    <t>Rekusrion; Coding mit funktionen; Klassen und Objekte Einführung; bis Konstruktor</t>
-  </si>
-  <si>
-    <t>8: self-lose Methoden</t>
-  </si>
-  <si>
-    <t>8:35-75</t>
-  </si>
-  <si>
-    <t>Konstruktor; mehrere Objekte; Methodenaufruf; Gleichheit; self-lose Methoden/statische vs. dynamische Methoden</t>
-  </si>
-  <si>
-    <t>8: Punkt: Abstand bestimmen</t>
-  </si>
-  <si>
-    <t>8:75-100(5)</t>
-  </si>
-  <si>
-    <t>Namensräume; Refernezen zählen als Beispiel für statische Attribute; string; stack; Anfang binärer Suchbaum</t>
-  </si>
-  <si>
-    <t>9: Gemeinsamkeiten in Klassen fassen</t>
-  </si>
-  <si>
-    <t>8:100-Ende; 9:1-32</t>
-  </si>
-  <si>
-    <t>Binäre Suchbaum rekursives Einfügen (insbes.: wo State speichern?). Vererbung. Liskov Substituion.</t>
-  </si>
-  <si>
-    <t>9: vernaschaulichung isinstnace</t>
-  </si>
-  <si>
-    <t>9:1:34-9:92</t>
-  </si>
-  <si>
-    <t>Vererbung praktisch in Python; getter/setter; property;</t>
-  </si>
-  <si>
-    <t>9: Ende</t>
-  </si>
-  <si>
-    <t>9:92-Ende; 10:1-24</t>
-  </si>
-  <si>
-    <t>Verberbung wie strukturieren und nutzen. Excpetions bis geschachtelte try-Blöcke</t>
-  </si>
-  <si>
-    <t>10: try in try</t>
-  </si>
-  <si>
-    <t>10 bis Ende; 11</t>
-  </si>
-  <si>
-    <t>try komplett; 10 erster Teil bis vor closures</t>
-  </si>
-  <si>
-    <t>11: Zugriff auf globale Variabeln</t>
-  </si>
-  <si>
-    <t>11 bis vor generatoren</t>
-  </si>
-  <si>
-    <t>closures, lambda-Ausdrücke, Generatoren </t>
-  </si>
-  <si>
-    <t>11: Werte auf Aufforderung</t>
-  </si>
-  <si>
-    <t>12: Beispiel Uhr und Kalender</t>
-  </si>
-  <si>
-    <t>12: Beobachtung: Teilsequenz</t>
-  </si>
-  <si>
-    <t>13: Code reuse</t>
-  </si>
-  <si>
-    <t>14: Vorgehen: Basics</t>
-  </si>
-  <si>
-    <t>15: Zuweisung inkompatibler Typen</t>
-  </si>
-  <si>
-    <t>16: Klassen als Datentypen</t>
-  </si>
-  <si>
-    <t>16: Funktionen</t>
-  </si>
-  <si>
-    <t>17: Zugriff auf Felder</t>
-  </si>
-  <si>
-    <t>17: interface vs. Levak</t>
-  </si>
-  <si>
-    <t>18: Ende</t>
-  </si>
-  <si>
-    <t>Blattnummer</t>
-  </si>
-  <si>
-    <t>Bearbeitet in Woche</t>
-  </si>
-  <si>
-    <t>Termine</t>
-  </si>
-  <si>
-    <t>Wer?</t>
-  </si>
-  <si>
-    <t>Bezug auf Vorlesungen</t>
-  </si>
-  <si>
-    <t>Bezug auf Vorlesungen; Themen (einschliesslich)</t>
-  </si>
-  <si>
-    <t>Sonderthemen</t>
-  </si>
-  <si>
-    <t>Themen fertig</t>
-  </si>
-  <si>
-    <t>Entwurf fertig</t>
-  </si>
-  <si>
-    <t>Review fertig</t>
-  </si>
-  <si>
-    <t>Endfassung fertig</t>
-  </si>
-  <si>
-    <t>Ausgabe</t>
-  </si>
-  <si>
-    <t>Fertig</t>
-  </si>
-  <si>
-    <t>Vorlesungen</t>
-  </si>
-  <si>
-    <t>Entwurf</t>
-  </si>
-  <si>
-    <t>Review 1</t>
-  </si>
-  <si>
-    <t>Review 2 (WIMi)</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Erreichte Vorlesung</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>TK</t>
-  </si>
-  <si>
-    <t>DP</t>
-  </si>
-  <si>
-    <t>Anmelden, Markup</t>
-  </si>
-  <si>
-    <t>JH</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>Terminal, Programme ausführen</t>
-  </si>
-  <si>
-    <t>JR</t>
-  </si>
-  <si>
-    <t>PB</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>MF</t>
-  </si>
-  <si>
-    <t>PUE ok</t>
-  </si>
-  <si>
-    <t>PUE leidlich ok</t>
-  </si>
-  <si>
-    <t>Abgabe</t>
-  </si>
-  <si>
-    <t>Vorlesung fertig</t>
-  </si>
-  <si>
-    <t>Entwurf (wIMi)</t>
-  </si>
-  <si>
-    <t>Review 2</t>
-  </si>
-  <si>
-    <t>Korrekturen fertig</t>
-  </si>
-  <si>
-    <t>Donald Parruca</t>
-  </si>
-  <si>
-    <t>Alexander Setzer</t>
-  </si>
-  <si>
-    <t>Michael Feldmann</t>
-  </si>
-  <si>
-    <t>Jonas Harbig</t>
-  </si>
-  <si>
-    <t>Jost Rossel</t>
-  </si>
-  <si>
-    <t>Moritz Thiele</t>
-  </si>
-  <si>
-    <t>Thomas Kellner</t>
-  </si>
-  <si>
-    <t>Paul Börding</t>
-  </si>
-  <si>
-    <t>Patrick Steffens</t>
-  </si>
-  <si>
-    <t>#PUE entwerfen</t>
-  </si>
-  <si>
-    <t>#PUE review</t>
-  </si>
-  <si>
-    <t>#HUE entwerfen</t>
-  </si>
-  <si>
-    <t>#HUE review</t>
-  </si>
-  <si>
-    <t>ZUE vorbereiten</t>
-  </si>
-  <si>
-    <t>ZUE abhalten</t>
-  </si>
-  <si>
-    <t>Tut vorbereiten</t>
-  </si>
-  <si>
-    <t>Tut abhalten (inkl. korrigieren!)</t>
-  </si>
-  <si>
-    <t>Korrigieren, ein Tutorium</t>
-  </si>
-  <si>
-    <t>Fixer Aufwand (Meeting etc.)</t>
-  </si>
-  <si>
-    <t>Aufwand (in Stunden)</t>
-  </si>
-  <si>
-    <t>Wie oft im Semester?</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>Wieviele Betroffen?</t>
-  </si>
-  <si>
-    <t>Gewichte</t>
-  </si>
-  <si>
-    <t>WM</t>
-  </si>
-  <si>
-    <t>SHK</t>
-  </si>
-  <si>
-    <t>SHK (1/2)</t>
-  </si>
-  <si>
-    <t>Gesamtgewicht</t>
-  </si>
-  <si>
-    <t>1/Gesamtgewicht</t>
-  </si>
-  <si>
-    <t>Gesamtaufwand (h)</t>
-  </si>
-  <si>
-    <t>Tutoren</t>
-  </si>
-  <si>
-    <t>Kürzel</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Anzahl:</t>
-  </si>
-  <si>
-    <t>Erreichte Leistung</t>
-  </si>
-  <si>
-    <t>Soll Leistung</t>
-  </si>
-  <si>
-    <t>Mo 14-16</t>
-  </si>
-  <si>
-    <t>Di 11-13</t>
-  </si>
-  <si>
-    <t>Di 16-18</t>
-  </si>
-  <si>
-    <t>Mi 11-13</t>
-  </si>
-  <si>
-    <t>Mi 16-18</t>
-  </si>
-  <si>
-    <t>Do 9-11</t>
-  </si>
-  <si>
-    <t>Do 14-16</t>
-  </si>
-  <si>
-    <t>Fr 9-11</t>
-  </si>
-  <si>
-    <t>D3.301</t>
-  </si>
-  <si>
-    <t>E1.111</t>
-  </si>
-  <si>
-    <t>PUE</t>
-  </si>
-  <si>
-    <t>HUE</t>
-  </si>
-  <si>
-    <t>Oktober</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>Dezember</t>
-  </si>
-  <si>
-    <t>Januar</t>
-  </si>
-  <si>
-    <t>Februar</t>
-  </si>
-  <si>
-    <t>Themen fertig(1)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(4)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(14)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(3)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(13)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(3)</t>
-  </si>
-  <si>
-    <t>Ausgabe(7)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(2)</t>
-  </si>
-  <si>
-    <t>Ausgabe(6)</t>
-  </si>
-  <si>
-    <t>Themen fertig(10)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(11)</t>
-  </si>
-  <si>
-    <t>Ausgabe(14)</t>
-  </si>
-  <si>
-    <t>Themen fertig(9)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(10)</t>
-  </si>
-  <si>
-    <t>Ausgabe(13)</t>
-  </si>
-  <si>
-    <t>Ausgabe(3)</t>
-  </si>
-  <si>
-    <t>Review fertig(8)</t>
-  </si>
-  <si>
-    <t>Ausgabe(2)</t>
-  </si>
-  <si>
-    <t>Review fertig(7)</t>
-  </si>
-  <si>
-    <t>Themen fertig(6)</t>
-  </si>
-  <si>
-    <t>Themen fertig(5)</t>
-  </si>
-  <si>
-    <t>Review fertig(4)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(9)</t>
-  </si>
-  <si>
-    <t>Review fertig(3)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(8)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(8)</t>
-  </si>
-  <si>
-    <t>Themen fertig(13)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(7)</t>
-  </si>
-  <si>
-    <t>Themen fertig(12)</t>
-  </si>
-  <si>
-    <t>Themen fertig(2)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(5)</t>
-  </si>
-  <si>
-    <t>Review fertig(11)</t>
-  </si>
-  <si>
-    <t>Review fertig(10)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(4)</t>
-  </si>
-  <si>
-    <t>Ausgabe(8)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(12)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(1)</t>
-  </si>
-  <si>
-    <t>Ausgabe(4)</t>
-  </si>
-  <si>
-    <t>Review fertig(9)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(11)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(10)</t>
-  </si>
-  <si>
-    <t>Themen fertig(7)</t>
-  </si>
-  <si>
-    <t>Review fertig(5)</t>
-  </si>
-  <si>
-    <t>Ausgabe(11)</t>
-  </si>
-  <si>
-    <t>Ausgabe(10)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(9)</t>
-  </si>
-  <si>
-    <t>Themen fertig(14)</t>
-  </si>
-  <si>
-    <t>Themen fertig(3)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(6)</t>
-  </si>
-  <si>
-    <t>Review fertig(12)</t>
-  </si>
-  <si>
-    <t>Review fertig(1)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(5)</t>
-  </si>
-  <si>
-    <t>Ausgabe(9)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(13)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(2)</t>
-  </si>
-  <si>
-    <t>Ausgabe(5)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(12)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(1)</t>
-  </si>
-  <si>
-    <t>Themen fertig(8)</t>
-  </si>
-  <si>
-    <t>Review fertig(6)</t>
-  </si>
-  <si>
-    <t>Ausgabe(12)</t>
-  </si>
-  <si>
-    <t>Ausgabe(1)</t>
-  </si>
-  <si>
-    <t>Themen fertig(4)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(7)</t>
-  </si>
-  <si>
-    <t>Review fertig(13)</t>
-  </si>
-  <si>
-    <t>Review fertig(2)</t>
-  </si>
-  <si>
-    <t>Endfassung fertig(6)</t>
-  </si>
-  <si>
-    <t>Themen fertig(11)</t>
-  </si>
-  <si>
-    <t>Entwurf fertig(14)</t>
-  </si>
-  <si>
-    <t>Review fertig(14)</t>
+    <t xml:space="preserve">Aktuelles Semester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorlesungsnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geplantes Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geplante KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist-Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist-KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gplantes Thema (bis einschliesslich)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geplantes Kapitel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist-Kapitel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist-Thema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 0;  Ch1: Datenstrukturen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0; 1:1-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 1, Versionsverwaltung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:23-Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bis Ch1, Ausführungsmodell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch2, Zahldarstellung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:1-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">einschließliche einfache Datentypen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 3, Animation von Programmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:20-Ende; 3 komplett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapitel 3 komplett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 4: Namenkonvention für Funktionsnamen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:1-49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapitel 4: Funktionen mit Parameter: Aufruf mit Ausdruck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 4: Pass-by-assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:49-Ende; 5:1-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bis Slicing von Tuples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 5, Slicing, Länge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:12-Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuple, Listen, Dicts. Komplett; Sets ausgelassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 5: dicts, Operationen darauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:1-6:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if; Anfang while bis Finden von Schleifeninvarianten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ch 6: Eindeutigkeit von else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:39-6:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bis  einschlieslich list comprehensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:Funktionen rufen Funktionen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:53-Ende; 7:1-7:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: Formale Parameter mit vorbelegten Werten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: String umdrehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:11-7:60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: Objekte/Instanzen: Graphische Notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:60-Ende; 8:1-34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rekusrion; Coding mit funktionen; Klassen und Objekte Einführung; bis Konstruktor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: self-lose Methoden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:35-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konstruktor; mehrere Objekte; Methodenaufruf; Gleichheit; self-lose Methoden/statische vs. dynamische Methoden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: Punkt: Abstand bestimmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:75-100(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namensräume; Refernezen zählen als Beispiel für statische Attribute; string; stack; Anfang binärer Suchbaum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: Gemeinsamkeiten in Klassen fassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:100-Ende; 9:1-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binäre Suchbaum rekursives Einfügen (insbes.: wo State speichern?). Vererbung. Liskov Substituion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: vernaschaulichung isinstnace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:1:34-9:92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vererbung praktisch in Python; getter/setter; property;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:92-Ende; 10:1-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verberbung wie strukturieren und nutzen. Excpetions bis geschachtelte try-Blöcke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: try in try</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 bis Ende; 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try komplett; 10 erster Teil bis vor closures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: Zugriff auf globale Variabeln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 bis vor generatoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closures, lambda-Ausdrücke, Generatoren </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: Werte auf Aufforderung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: Beispiel Uhr und Kalender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: Beobachtung: Teilsequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: Code reuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: Vorgehen: Basics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15: Zuweisung inkompatibler Typen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: Klassen als Datentypen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: Funktionen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: Zugriff auf Felder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: interface vs. Levak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18: Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blattnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearbeitet in Woche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezug auf Vorlesungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezug auf Vorlesungen; Themen (einschliesslich)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonderthemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorlesungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review 2 (WIMi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreichte Vorlesung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmelden, Markup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminal, Programme ausführen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE leidlich ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abgabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorlesung fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf (wIMi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korrekturen fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donald Parruca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexander Setzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Feldmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonas Harbig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jost Rossel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moritz Thiele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas Kellner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Börding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick Steffens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#PUE entwerfen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#PUE review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#HUE entwerfen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#HUE review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZUE vorbereiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZUE abhalten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tut vorbereiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tut abhalten (inkl. korrigieren!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korrigieren, ein Tutorium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixer Aufwand (Meeting etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufwand (in Stunden)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie oft im Semester?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wieviele Betroffen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gewichte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHK (1/2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtgewicht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/Gesamtgewicht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtaufwand (h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kürzel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreichte Leistung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soll Leistung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo 14-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di 11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di 16-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mi 11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mi 16-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do 9-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do 14-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr 9-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3.301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1.111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oktober</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dezember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Januar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Februar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabe(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endfassung fertig(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Themen fertig(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwurf fertig(14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review fertig(14)</t>
   </si>
 </sst>
 </file>
@@ -742,7 +747,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -1341,16 +1346,15 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="9">
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1360,11 +1364,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1374,11 +1377,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1388,11 +1390,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1402,11 +1403,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1416,11 +1416,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1430,11 +1429,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1444,11 +1442,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1458,183 +1455,14 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1710,14 +1538,14 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="C9 D22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="F9 D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.12093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.12093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,14 +2434,14 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="C9 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="F9 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.12093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.8697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2818,11 +2646,9 @@
         <f aca="false">VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>2:1-19</v>
       </c>
-      <c r="R4" s="0" t="inlineStr">
+      <c r="R4" s="0" t="e">
         <f aca="false">VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S4" s="0" t="n">
         <f aca="false">MAX(M4:O4)</f>
@@ -2890,11 +2716,9 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:1-49</v>
       </c>
-      <c r="R5" s="0" t="inlineStr">
+      <c r="R5" s="0" t="e">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">MAX(M5:O5)</f>
@@ -2959,11 +2783,9 @@
         <f aca="false">VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:49-Ende; 5:1-12</v>
       </c>
-      <c r="R6" s="0" t="inlineStr">
+      <c r="R6" s="0" t="e">
         <f aca="false">VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S6" s="0" t="n">
         <f aca="false">MAX(M6:O6)</f>
@@ -3028,11 +2850,9 @@
         <f aca="false">VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>6:1-6:39</v>
       </c>
-      <c r="R7" s="0" t="inlineStr">
+      <c r="R7" s="0" t="e">
         <f aca="false">VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S7" s="0" t="n">
         <f aca="false">MAX(M7:O7)</f>
@@ -3167,11 +2987,9 @@
         <f aca="false">VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>8:35-75</v>
       </c>
-      <c r="R9" s="0" t="inlineStr">
+      <c r="R9" s="0" t="e">
         <f aca="false">VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S9" s="0" t="n">
         <f aca="false">MAX(M9:O9)</f>
@@ -3306,11 +3124,9 @@
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>10 bis Ende; 11</v>
       </c>
-      <c r="R11" s="0" t="inlineStr">
+      <c r="R11" s="0" t="e">
         <f aca="false">VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S11" s="0" t="n">
         <f aca="false">MAX(M11:N11)</f>
@@ -3445,11 +3261,9 @@
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>13: Code reuse</v>
       </c>
-      <c r="R13" s="0" t="inlineStr">
+      <c r="R13" s="0" t="e">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">MAX(M13:O13)</f>
@@ -3716,12 +3530,12 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="C9 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="F9 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3934,23 +3748,17 @@
         <f aca="false">VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>2:20-Ende; 3 komplett</v>
       </c>
-      <c r="R4" s="0" t="inlineStr">
+      <c r="R4" s="0" t="e">
         <f aca="false">VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U4" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U4" s="0" t="n">
         <f aca="false">MAX(M4:O4)&lt;=MAX(PUE!M4:O4)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V4" s="0" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="V4" s="0" t="n">
         <f aca="false">MAX(M4:O4)&lt;=MAX(PUE!M5:O5)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4008,23 +3816,17 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:1-49</v>
       </c>
-      <c r="R5" s="0" t="inlineStr">
+      <c r="R5" s="0" t="e">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U5" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U5" s="0" t="n">
         <f aca="false">MAX(M5:O5)&lt;=MAX(PUE!M5:O5)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V5" s="0" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="V5" s="0" t="n">
         <f aca="false">MAX(M5:O5)&lt;=MAX(PUE!M6:O6)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4082,23 +3884,17 @@
         <f aca="false">VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>5:12-Ende</v>
       </c>
-      <c r="R6" s="0" t="inlineStr">
+      <c r="R6" s="0" t="e">
         <f aca="false">VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U6" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U6" s="0" t="n">
         <f aca="false">MAX(M6:O6)&lt;=MAX(PUE!M6:O6)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V6" s="0" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="V6" s="0" t="n">
         <f aca="false">MAX(M6:O6)&lt;=MAX(PUE!M7:O7)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4156,23 +3952,17 @@
         <f aca="false">VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>6:39-6:53</v>
       </c>
-      <c r="R7" s="0" t="inlineStr">
+      <c r="R7" s="0" t="e">
         <f aca="false">VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U7" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U7" s="0" t="n">
         <f aca="false">MAX(M7:O7)&lt;=MAX(PUE!M7:O7)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V7" s="0" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="V7" s="0" t="n">
         <f aca="false">MAX(M7:O7)&lt;=MAX(PUE!M8:O8)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4230,23 +4020,17 @@
         <f aca="false">VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
         <v>7:11-7:60</v>
       </c>
-      <c r="R8" s="0" t="inlineStr">
+      <c r="R8" s="0" t="e">
         <f aca="false">VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U8" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U8" s="0" t="n">
         <f aca="false">MAX(M8:O8)&lt;=MAX(PUE!M8:O8)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V8" s="0" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="V8" s="0" t="n">
         <f aca="false">MAX(M8:O8)&lt;=MAX(PUE!M9:O9)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4304,23 +4088,17 @@
         <f aca="false">VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>8:35-75</v>
       </c>
-      <c r="R9" s="0" t="inlineStr">
+      <c r="R9" s="0" t="e">
         <f aca="false">VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U9" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U9" s="0" t="n">
         <f aca="false">MAX(M9:O9)&lt;=MAX(PUE!M9:O9)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V9" s="0" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="V9" s="0" t="n">
         <f aca="false">MAX(M9:O9)&lt;=MAX(PUE!M10:O10)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,17 +4163,13 @@
         <f aca="false">VLOOKUP(O10,vorlesung!$A$4:$H$33,8,0)</f>
         <v>9:1:34-9:92</v>
       </c>
-      <c r="U10" s="0" t="inlineStr">
+      <c r="U10" s="0" t="n">
         <f aca="false">MAX(M10:O10)&lt;=MAX(PUE!M10:O10)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V10" s="0" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="V10" s="0" t="n">
         <f aca="false">MAX(M10:O10)&lt;=MAX(PUE!M11:O11)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4453,21 +4227,17 @@
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>10 bis Ende; 11</v>
       </c>
-      <c r="R11" s="0" t="inlineStr">
+      <c r="R11" s="0" t="e">
         <f aca="false">VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="U11" s="0" t="n">
         <f aca="false">MAX(M11:O11)&lt;=MAX(PUE!M11:N11)</f>
         <v>1</v>
       </c>
-      <c r="V11" s="0" t="inlineStr">
+      <c r="V11" s="0" t="n">
         <f aca="false">MAX(M11:O11)&lt;=MAX(PUE!M12:O12)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,11 +4306,9 @@
         <f aca="false">MAX(M12:O12)&lt;=MAX(PUE!M12:O12)</f>
         <v>1</v>
       </c>
-      <c r="V12" s="0" t="inlineStr">
+      <c r="V12" s="0" t="n">
         <f aca="false">MAX(M12:O12)&lt;=MAX(PUE!M13:O13)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4598,23 +4366,17 @@
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>13: Code reuse</v>
       </c>
-      <c r="R13" s="0" t="inlineStr">
+      <c r="R13" s="0" t="e">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="U13" s="0" t="inlineStr">
+        <v>#N/A</v>
+      </c>
+      <c r="U13" s="0" t="n">
         <f aca="false">MAX(M13:O13)&lt;=MAX(PUE!M13:O13)</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V13" s="0" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="V13" s="0" t="n">
         <f aca="false">MAX(M13:O13)&lt;=MAX(PUE!M14:O14)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,11 +4441,9 @@
         <f aca="false">VLOOKUP(O14,vorlesung!$A$4:$H$33,8,0)</f>
         <v>16: Klassen als Datentypen</v>
       </c>
-      <c r="U14" s="0" t="inlineStr">
+      <c r="U14" s="0" t="n">
         <f aca="false">MAX(M14:O14)&lt;=MAX(PUE!M14:O14)</f>
-        <is>
-          <t/>
-        </is>
+        <v>1</v>
       </c>
       <c r="V14" s="0" t="n">
         <f aca="false">MAX(M14:O14)&lt;=MAX(PUE!M15:N15)</f>
@@ -4745,11 +4505,9 @@
         <f aca="false">VLOOKUP(N15,vorlesung!$A$4:$H$33,8,0)</f>
         <v>17: Zugriff auf Felder</v>
       </c>
-      <c r="R15" s="0" t="inlineStr">
+      <c r="R15" s="0" t="e">
         <f aca="false">VLOOKUP(O15,vorlesung!$A$4:$H$33,8,0)</f>
-        <is>
-          <t/>
-        </is>
+        <v>#N/A</v>
       </c>
       <c r="U15" s="0" t="n">
         <f aca="false">MAX(M15:O15)&lt;=MAX(PUE!M15:N15)</f>
@@ -4806,12 +4564,12 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4950,6 +4708,7 @@
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
+      <c r="F9" s="11"/>
       <c r="I9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5001,12 +4760,12 @@
   <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="C9 B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="F9 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6165,12 +5924,12 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="C9 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="F9 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6367,12 +6126,12 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="1" sqref="C9 F43"/>
+      <selection pane="topLeft" activeCell="F43" activeCellId="1" sqref="F9 F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
jonas Harbig Hü7 korregiert
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/gp1-jupyter/meetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\GIT_GP1_16\gp1-jupyter\meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,11 +20,8 @@
     <sheet name="Uebungsgruppen" sheetId="6" r:id="rId6"/>
     <sheet name="Deadlines sortiert" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1241,8 +1238,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Erklärender Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -1550,6 +1547,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1823,18 +1823,18 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>Ch 0;  Ch1: Datenstrukturen</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="93" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="192" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>42696</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="256" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="248" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="240" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>42703</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="224" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="217" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="124" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="160" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="155" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>42711</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="93" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>42717</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="93" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>42724</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="93" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="176" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>42745</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="124" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>42746</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>42752</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>42753</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="93" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>42766</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="62" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2727,9 +2727,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>87</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3810,7 +3810,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -3819,7 +3819,7 @@
     <col min="17" max="17" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>87</v>
@@ -3901,7 +3901,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4837,12 +4837,12 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>118</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4906,17 +4906,17 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4930,7 +4930,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4944,7 +4944,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4958,7 +4958,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4972,43 +4972,44 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5027,9 +5028,9 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="D2" s="12" t="s">
         <v>128</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5100,7 +5101,7 @@
       </c>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -5143,7 +5144,7 @@
       <c r="S4" s="19"/>
       <c r="T4" s="19"/>
     </row>
-    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -5192,7 +5193,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>142</v>
       </c>
@@ -5243,7 +5244,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>144</v>
       </c>
@@ -5291,7 +5292,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>145</v>
       </c>
@@ -5346,7 +5347,7 @@
       <c r="S8" s="19"/>
       <c r="T8" s="19"/>
     </row>
-    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="B9" s="21" t="s">
         <v>146</v>
       </c>
@@ -5401,7 +5402,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
     </row>
-    <row r="10" spans="1:20" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16" t="s">
         <v>147</v>
       </c>
@@ -5446,7 +5447,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>148</v>
       </c>
@@ -5500,7 +5501,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
     </row>
-    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>149</v>
       </c>
@@ -5525,7 +5526,7 @@
       <c r="S12" s="22"/>
       <c r="T12" s="19"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -5588,7 +5589,7 @@
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -5651,7 +5652,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5714,7 +5715,7 @@
       <c r="S15" s="22"/>
       <c r="T15" s="22"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -5777,7 +5778,7 @@
       <c r="S16" s="22"/>
       <c r="T16" s="22"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -5840,7 +5841,7 @@
       <c r="S17" s="22"/>
       <c r="T17" s="22"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -5903,7 +5904,7 @@
       <c r="S18" s="22"/>
       <c r="T18" s="22"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -5966,7 +5967,7 @@
       <c r="S19" s="22"/>
       <c r="T19" s="22"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -6029,7 +6030,7 @@
       <c r="S20" s="22"/>
       <c r="T20" s="22"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -6087,7 +6088,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D22" s="44">
         <f t="shared" ref="D22:M22" si="11">D3*SUM(D13:D21)</f>
         <v>52</v>
@@ -6180,9 +6181,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>155</v>
       </c>
@@ -6208,7 +6209,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>121</v>
       </c>
@@ -6225,7 +6226,7 @@
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="45" t="s">
         <v>120</v>
       </c>
@@ -6242,7 +6243,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>126</v>
       </c>
@@ -6259,7 +6260,7 @@
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>125</v>
       </c>
@@ -6276,7 +6277,7 @@
       <c r="H5" s="46"/>
       <c r="I5" s="46"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
         <v>127</v>
       </c>
@@ -6293,7 +6294,7 @@
       </c>
       <c r="I6" s="46"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
         <v>124</v>
       </c>
@@ -6308,7 +6309,7 @@
       <c r="H7" s="46"/>
       <c r="I7" s="46"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
         <v>123</v>
       </c>
@@ -6323,7 +6324,7 @@
       <c r="H8" s="46"/>
       <c r="I8" s="46"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="45" t="s">
         <v>119</v>
       </c>
@@ -6340,7 +6341,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
         <v>122</v>
       </c>
@@ -6375,9 +6376,9 @@
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -6385,7 +6386,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>167</v>
       </c>
@@ -6427,7 +6428,7 @@
       </c>
       <c r="U2" s="36"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="30">
         <v>1</v>
       </c>
@@ -6474,7 +6475,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="30">
         <v>2</v>
       </c>
@@ -6518,7 +6519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="30">
         <v>3</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="30">
         <v>4</v>
       </c>
@@ -6612,7 +6613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="30">
         <v>5</v>
       </c>
@@ -6650,7 +6651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="30">
         <v>6</v>
       </c>
@@ -6694,7 +6695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="30">
         <v>7</v>
       </c>
@@ -6738,7 +6739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="30">
         <v>8</v>
       </c>
@@ -6788,7 +6789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="30">
         <v>9</v>
       </c>
@@ -6832,7 +6833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="30">
         <v>10</v>
       </c>
@@ -6870,7 +6871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="30">
         <v>11</v>
       </c>
@@ -6923,7 +6924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="30">
         <v>12</v>
       </c>
@@ -6961,7 +6962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="30">
         <v>13</v>
       </c>
@@ -7011,7 +7012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>14</v>
       </c>
@@ -7055,7 +7056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="30">
         <v>15</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="30">
         <v>16</v>
       </c>
@@ -7152,7 +7153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="30">
         <v>17</v>
       </c>
@@ -7190,7 +7191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="30">
         <v>18</v>
       </c>
@@ -7246,7 +7247,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="30">
         <v>19</v>
       </c>
@@ -7287,7 +7288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="30">
         <v>20</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="30">
         <v>21</v>
       </c>
@@ -7372,7 +7373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="30">
         <v>22</v>
       </c>
@@ -7422,7 +7423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="30">
         <v>23</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="30">
         <v>24</v>
       </c>
@@ -7516,7 +7517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="30">
         <v>25</v>
       </c>
@@ -7566,7 +7567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="30">
         <v>26</v>
       </c>
@@ -7610,7 +7611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="30">
         <v>27</v>
       </c>
@@ -7654,7 +7655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="30">
         <v>28</v>
       </c>
@@ -7692,7 +7693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="30">
         <v>29</v>
       </c>
@@ -7736,7 +7737,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="30">
         <v>30</v>
       </c>
@@ -7774,7 +7775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="30">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
kleine Korrektur in ML von HUE11
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -17,765 +17,760 @@
     <sheet name="Deadlines sortiert" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="250">
   <si>
-    <t xml:space="preserve">Aktuelles Semester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vorlesungsnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geplantes Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geplante KW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ist-Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ist-KW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gplantes Thema (bis einschliesslich)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geplantes Kapitel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ist-Kapitel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ist-Thema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 0;  Ch1: Datenstrukturen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0; 1:1-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 1, Versionsverwaltung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:23-Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bis Ch1, Ausführungsmodell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch2, Zahldarstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2:1-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">einschließliche einfache Datentypen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 3, Animation von Programmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2:20-Ende; 3 komplett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapitel 3 komplett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 4: Namenkonvention für Funktionsnamen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4:1-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapitel 4: Funktionen mit Parameter: Aufruf mit Ausdruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 4: Pass-by-assignment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4:49-Ende; 5:1-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bis Slicing von Tuples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 5, Slicing, Länge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5:12-Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuple, Listen, Dicts. Komplett; Sets ausgelassen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 5: dicts, Operationen darauf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6:1-6:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if; Anfang while bis Finden von Schleifeninvarianten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 6: Eindeutigkeit von else</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6:39-6:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bis  einschlieslich list comprehensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7:Funktionen rufen Funktionen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6:53-Ende; 7:1-7:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7: Formale Parameter mit vorbelegten Werten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7: String umdrehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7:11-7:60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8: Objekte/Instanzen: Graphische Notation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7:60-Ende; 8:1-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rekusrion; Coding mit funktionen; Klassen und Objekte Einführung; bis Konstruktor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8: self-lose Methoden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:35-75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Konstruktor; mehrere Objekte; Methodenaufruf; Gleichheit; self-lose Methoden/statische vs. dynamische Methoden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8: Punkt: Abstand bestimmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:75-100(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namensräume; Refernezen zählen als Beispiel für statische Attribute; string; stack; Anfang binärer Suchbaum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9: Gemeinsamkeiten in Klassen fassen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:100-Ende; 9:1-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binäre Suchbaum rekursives Einfügen (insbes.: wo State speichern?). Vererbung. Liskov Substituion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9: vernaschaulichung isinstnace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:1:34-9:92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vererbung praktisch in Python; getter/setter; property;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9: Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:92-Ende; 10:1-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verberbung wie strukturieren und nutzen. Excpetions bis geschachtelte try-Blöcke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10: try in try</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 bis Ende; 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">try komplett; 10 erster Teil bis vor closures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11: Zugriff auf globale Variabeln</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 bis vor generatoren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closures, lambda-Ausdrücke, Generatoren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11: Werte auf Aufforderung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11: bis ende. 12:1-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generatoren. Verfachverebrung, einfache Beispiele.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12: Beispiel Uhr und Kalender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:18-56. Linearisierung. C3-Algorithmus, Bis Beispiel 2 einschließlich (mit viel Tafel-anschrieb)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12: Beobachtung: Teilsequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:56-Ende. C3 Wiederholung; MRO; dependency injection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13: Code reuse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14: Virtualenvwrapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:komplett; 14:1-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14: Vorgehen: Basics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14: 11-Ende; 15:1-29. bis zu Typen und Klassen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15: Zuweisung inkompatibler Typen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:-Ende: 16:1-20. (Variablendeklaration mit Typen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16: Klassen als Datentypen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16: bis Ende.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16: Funktionen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17: 1-37 (boxing/unboxing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17: Zugriff auf Felder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:37-71 (bis abstrakte Methoden)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17: interface vs. Levak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18: Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blattnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bearbeitet in Woche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Termine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wer?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezug auf Vorlesungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezug auf Vorlesungen; Themen (einschliesslich)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonderthemen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vorlesungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review 2 (WIMi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erreichte Vorlesung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anmelden, Markup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terminal, Programme ausführen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUE ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUE leidlich ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abgabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vorlesung fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf (wIMi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korrekturen fertig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donald Parruca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexander Setzer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Feldmann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonas Harbig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jost Rossel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moritz Thiele</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas Kellner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Börding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patrick Steffens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#PUE entwerfen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#PUE review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#HUE entwerfen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#HUE review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZUE vorbereiten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZUE abhalten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tut vorbereiten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tut abhalten (inkl. korrigieren!)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korrigieren, ein Tutorium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixer Aufwand (Meeting etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufwand (in Stunden)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wie oft im Semester?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wieviele Betroffen?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gewichte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHK (1/2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesamtgewicht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/Gesamtgewicht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesamtaufwand (h)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutoren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kürzel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzahl:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erreichte Leistung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soll Leistung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mo 14-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Di 11-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Di 16-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mi 11-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mi 16-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do 9-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do 14-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr 9-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3.301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1.111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E3.303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oktober</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dezember</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Januar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Februar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausgabe(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endfassung fertig(6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Themen fertig(11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entwurf fertig(14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review fertig(14)</t>
+    <t>Aktuelles Semester</t>
+  </si>
+  <si>
+    <t>Vorlesungsnummer</t>
+  </si>
+  <si>
+    <t>Geplantes Datum</t>
+  </si>
+  <si>
+    <t>Geplante KW</t>
+  </si>
+  <si>
+    <t>Ist-Datum</t>
+  </si>
+  <si>
+    <t>Ist-KW</t>
+  </si>
+  <si>
+    <t>Gplantes Thema (bis einschliesslich)</t>
+  </si>
+  <si>
+    <t>Geplantes Kapitel</t>
+  </si>
+  <si>
+    <t>Ist-Kapitel</t>
+  </si>
+  <si>
+    <t>Ist-Thema</t>
+  </si>
+  <si>
+    <t>Ch 0;  Ch1: Datenstrukturen</t>
+  </si>
+  <si>
+    <t>0; 1:1-22</t>
+  </si>
+  <si>
+    <t>Ch 1, Versionsverwaltung</t>
+  </si>
+  <si>
+    <t>1:23-Ende</t>
+  </si>
+  <si>
+    <t>bis Ch1, Ausführungsmodell</t>
+  </si>
+  <si>
+    <t>Ch2, Zahldarstellung</t>
+  </si>
+  <si>
+    <t>2:1-19</t>
+  </si>
+  <si>
+    <t>einschließliche einfache Datentypen</t>
+  </si>
+  <si>
+    <t>Ch 3, Animation von Programmen</t>
+  </si>
+  <si>
+    <t>2:20-Ende; 3 komplett</t>
+  </si>
+  <si>
+    <t>Kapitel 3 komplett</t>
+  </si>
+  <si>
+    <t>Ch 4: Namenkonvention für Funktionsnamen</t>
+  </si>
+  <si>
+    <t>4:1-49</t>
+  </si>
+  <si>
+    <t>Kapitel 4: Funktionen mit Parameter: Aufruf mit Ausdruck</t>
+  </si>
+  <si>
+    <t>Ch 4: Pass-by-assignment</t>
+  </si>
+  <si>
+    <t>4:49-Ende; 5:1-12</t>
+  </si>
+  <si>
+    <t>Bis Slicing von Tuples</t>
+  </si>
+  <si>
+    <t>Ch 5, Slicing, Länge</t>
+  </si>
+  <si>
+    <t>5:12-Ende</t>
+  </si>
+  <si>
+    <t>Tuple, Listen, Dicts. Komplett; Sets ausgelassen</t>
+  </si>
+  <si>
+    <t>Ch 5: dicts, Operationen darauf</t>
+  </si>
+  <si>
+    <t>6:1-6:39</t>
+  </si>
+  <si>
+    <t>if; Anfang while bis Finden von Schleifeninvarianten</t>
+  </si>
+  <si>
+    <t>Ch 6: Eindeutigkeit von else</t>
+  </si>
+  <si>
+    <t>6:39-6:53</t>
+  </si>
+  <si>
+    <t>bis  einschlieslich list comprehensions</t>
+  </si>
+  <si>
+    <t>7:Funktionen rufen Funktionen</t>
+  </si>
+  <si>
+    <t>6:53-Ende; 7:1-7:11</t>
+  </si>
+  <si>
+    <t>7: Formale Parameter mit vorbelegten Werten</t>
+  </si>
+  <si>
+    <t>7: String umdrehen</t>
+  </si>
+  <si>
+    <t>7:11-7:60</t>
+  </si>
+  <si>
+    <t>8: Objekte/Instanzen: Graphische Notation</t>
+  </si>
+  <si>
+    <t>7:60-Ende; 8:1-34</t>
+  </si>
+  <si>
+    <t>Rekusrion; Coding mit funktionen; Klassen und Objekte Einführung; bis Konstruktor</t>
+  </si>
+  <si>
+    <t>8: self-lose Methoden</t>
+  </si>
+  <si>
+    <t>8:35-75</t>
+  </si>
+  <si>
+    <t>Konstruktor; mehrere Objekte; Methodenaufruf; Gleichheit; self-lose Methoden/statische vs. dynamische Methoden</t>
+  </si>
+  <si>
+    <t>8: Punkt: Abstand bestimmen</t>
+  </si>
+  <si>
+    <t>8:75-100(5)</t>
+  </si>
+  <si>
+    <t>Namensräume; Refernezen zählen als Beispiel für statische Attribute; string; stack; Anfang binärer Suchbaum</t>
+  </si>
+  <si>
+    <t>9: Gemeinsamkeiten in Klassen fassen</t>
+  </si>
+  <si>
+    <t>8:100-Ende; 9:1-32</t>
+  </si>
+  <si>
+    <t>Binäre Suchbaum rekursives Einfügen (insbes.: wo State speichern?). Vererbung. Liskov Substituion.</t>
+  </si>
+  <si>
+    <t>9: vernaschaulichung isinstnace</t>
+  </si>
+  <si>
+    <t>9:1:34-9:92</t>
+  </si>
+  <si>
+    <t>Vererbung praktisch in Python; getter/setter; property;</t>
+  </si>
+  <si>
+    <t>9: Ende</t>
+  </si>
+  <si>
+    <t>9:92-Ende; 10:1-24</t>
+  </si>
+  <si>
+    <t>Verberbung wie strukturieren und nutzen. Excpetions bis geschachtelte try-Blöcke</t>
+  </si>
+  <si>
+    <t>10: try in try</t>
+  </si>
+  <si>
+    <t>10 bis Ende; 11</t>
+  </si>
+  <si>
+    <t>try komplett; 10 erster Teil bis vor closures</t>
+  </si>
+  <si>
+    <t>11: Zugriff auf globale Variabeln</t>
+  </si>
+  <si>
+    <t>11 bis vor generatoren</t>
+  </si>
+  <si>
+    <t>closures, lambda-Ausdrücke, Generatoren</t>
+  </si>
+  <si>
+    <t>11: Werte auf Aufforderung</t>
+  </si>
+  <si>
+    <t>11: bis ende. 12:1-18</t>
+  </si>
+  <si>
+    <t>Generatoren. Verfachverebrung, einfache Beispiele.</t>
+  </si>
+  <si>
+    <t>12: Beispiel Uhr und Kalender</t>
+  </si>
+  <si>
+    <t>12:18-56. Linearisierung. C3-Algorithmus, Bis Beispiel 2 einschließlich (mit viel Tafel-anschrieb)</t>
+  </si>
+  <si>
+    <t>12: Beobachtung: Teilsequenz</t>
+  </si>
+  <si>
+    <t>12:56-Ende. C3 Wiederholung; MRO; dependency injection</t>
+  </si>
+  <si>
+    <t>13: Code reuse</t>
+  </si>
+  <si>
+    <t>14: Virtualenvwrapper</t>
+  </si>
+  <si>
+    <t>13:komplett; 14:1-11</t>
+  </si>
+  <si>
+    <t>14: Vorgehen: Basics</t>
+  </si>
+  <si>
+    <t>14: 11-Ende; 15:1-29. bis zu Typen und Klassen</t>
+  </si>
+  <si>
+    <t>15: Zuweisung inkompatibler Typen</t>
+  </si>
+  <si>
+    <t>15:-Ende: 16:1-20. (Variablendeklaration mit Typen)</t>
+  </si>
+  <si>
+    <t>16: Klassen als Datentypen</t>
+  </si>
+  <si>
+    <t>16: bis Ende.</t>
+  </si>
+  <si>
+    <t>16: Funktionen</t>
+  </si>
+  <si>
+    <t>17: 1-37 (boxing/unboxing)</t>
+  </si>
+  <si>
+    <t>17: Zugriff auf Felder</t>
+  </si>
+  <si>
+    <t>17:37-71 (bis abstrakte Methoden)</t>
+  </si>
+  <si>
+    <t>17: interface vs. Levak</t>
+  </si>
+  <si>
+    <t>18: Ende</t>
+  </si>
+  <si>
+    <t>Blattnummer</t>
+  </si>
+  <si>
+    <t>Bearbeitet in Woche</t>
+  </si>
+  <si>
+    <t>Termine</t>
+  </si>
+  <si>
+    <t>Wer?</t>
+  </si>
+  <si>
+    <t>Bezug auf Vorlesungen</t>
+  </si>
+  <si>
+    <t>Bezug auf Vorlesungen; Themen (einschliesslich)</t>
+  </si>
+  <si>
+    <t>Sonderthemen</t>
+  </si>
+  <si>
+    <t>Themen fertig</t>
+  </si>
+  <si>
+    <t>Entwurf fertig</t>
+  </si>
+  <si>
+    <t>Review fertig</t>
+  </si>
+  <si>
+    <t>Endfassung fertig</t>
+  </si>
+  <si>
+    <t>Ausgabe</t>
+  </si>
+  <si>
+    <t>Fertig</t>
+  </si>
+  <si>
+    <t>Vorlesungen</t>
+  </si>
+  <si>
+    <t>Entwurf</t>
+  </si>
+  <si>
+    <t>Review 1</t>
+  </si>
+  <si>
+    <t>Review 2 (WIMi)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Erreichte Vorlesung</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Anmelden, Markup</t>
+  </si>
+  <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Terminal, Programme ausführen</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>PUE ok</t>
+  </si>
+  <si>
+    <t>PUE leidlich ok</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
+  </si>
+  <si>
+    <t>Vorlesung fertig</t>
+  </si>
+  <si>
+    <t>Entwurf (wIMi)</t>
+  </si>
+  <si>
+    <t>Review 2</t>
+  </si>
+  <si>
+    <t>Korrekturen fertig</t>
+  </si>
+  <si>
+    <t>Donald Parruca</t>
+  </si>
+  <si>
+    <t>Alexander Setzer</t>
+  </si>
+  <si>
+    <t>Michael Feldmann</t>
+  </si>
+  <si>
+    <t>Jonas Harbig</t>
+  </si>
+  <si>
+    <t>Jost Rossel</t>
+  </si>
+  <si>
+    <t>Moritz Thiele</t>
+  </si>
+  <si>
+    <t>Thomas Kellner</t>
+  </si>
+  <si>
+    <t>Paul Börding</t>
+  </si>
+  <si>
+    <t>Patrick Steffens</t>
+  </si>
+  <si>
+    <t>#PUE entwerfen</t>
+  </si>
+  <si>
+    <t>#PUE review</t>
+  </si>
+  <si>
+    <t>#HUE entwerfen</t>
+  </si>
+  <si>
+    <t>#HUE review</t>
+  </si>
+  <si>
+    <t>ZUE vorbereiten</t>
+  </si>
+  <si>
+    <t>ZUE abhalten</t>
+  </si>
+  <si>
+    <t>Tut vorbereiten</t>
+  </si>
+  <si>
+    <t>Tut abhalten (inkl. korrigieren!)</t>
+  </si>
+  <si>
+    <t>Korrigieren, ein Tutorium</t>
+  </si>
+  <si>
+    <t>Fixer Aufwand (Meeting etc.)</t>
+  </si>
+  <si>
+    <t>Aufwand (in Stunden)</t>
+  </si>
+  <si>
+    <t>Wie oft im Semester?</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Wieviele Betroffen?</t>
+  </si>
+  <si>
+    <t>Gewichte</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>SHK</t>
+  </si>
+  <si>
+    <t>SHK (1/2)</t>
+  </si>
+  <si>
+    <t>Gesamtgewicht</t>
+  </si>
+  <si>
+    <t>1/Gesamtgewicht</t>
+  </si>
+  <si>
+    <t>Gesamtaufwand (h)</t>
+  </si>
+  <si>
+    <t>Tutoren</t>
+  </si>
+  <si>
+    <t>Kürzel</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Anzahl:</t>
+  </si>
+  <si>
+    <t>Erreichte Leistung</t>
+  </si>
+  <si>
+    <t>Soll Leistung</t>
+  </si>
+  <si>
+    <t>Mo 14-16</t>
+  </si>
+  <si>
+    <t>Di 11-13</t>
+  </si>
+  <si>
+    <t>Di 16-18</t>
+  </si>
+  <si>
+    <t>Mi 11-13</t>
+  </si>
+  <si>
+    <t>Mi 16-18</t>
+  </si>
+  <si>
+    <t>Do 9-11</t>
+  </si>
+  <si>
+    <t>Do 14-16</t>
+  </si>
+  <si>
+    <t>Fr 9-11</t>
+  </si>
+  <si>
+    <t>D3.301</t>
+  </si>
+  <si>
+    <t>E1.111</t>
+  </si>
+  <si>
+    <t>E3.303</t>
+  </si>
+  <si>
+    <t>PUE</t>
+  </si>
+  <si>
+    <t>HUE</t>
+  </si>
+  <si>
+    <t>Oktober</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Dezember</t>
+  </si>
+  <si>
+    <t>Januar</t>
+  </si>
+  <si>
+    <t>Februar</t>
+  </si>
+  <si>
+    <t>Themen fertig(1)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(4)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(14)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(3)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(13)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(3)</t>
+  </si>
+  <si>
+    <t>Ausgabe(7)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(2)</t>
+  </si>
+  <si>
+    <t>Ausgabe(6)</t>
+  </si>
+  <si>
+    <t>Themen fertig(10)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(11)</t>
+  </si>
+  <si>
+    <t>Ausgabe(14)</t>
+  </si>
+  <si>
+    <t>Themen fertig(9)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(10)</t>
+  </si>
+  <si>
+    <t>Ausgabe(13)</t>
+  </si>
+  <si>
+    <t>Ausgabe(3)</t>
+  </si>
+  <si>
+    <t>Review fertig(8)</t>
+  </si>
+  <si>
+    <t>Ausgabe(2)</t>
+  </si>
+  <si>
+    <t>Review fertig(7)</t>
+  </si>
+  <si>
+    <t>Themen fertig(6)</t>
+  </si>
+  <si>
+    <t>Themen fertig(5)</t>
+  </si>
+  <si>
+    <t>Review fertig(4)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(9)</t>
+  </si>
+  <si>
+    <t>Review fertig(3)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(8)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(8)</t>
+  </si>
+  <si>
+    <t>Themen fertig(13)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(7)</t>
+  </si>
+  <si>
+    <t>Themen fertig(12)</t>
+  </si>
+  <si>
+    <t>Themen fertig(2)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(5)</t>
+  </si>
+  <si>
+    <t>Review fertig(11)</t>
+  </si>
+  <si>
+    <t>Review fertig(10)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(4)</t>
+  </si>
+  <si>
+    <t>Ausgabe(8)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(12)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(1)</t>
+  </si>
+  <si>
+    <t>Ausgabe(4)</t>
+  </si>
+  <si>
+    <t>Review fertig(9)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(11)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(10)</t>
+  </si>
+  <si>
+    <t>Themen fertig(7)</t>
+  </si>
+  <si>
+    <t>Review fertig(5)</t>
+  </si>
+  <si>
+    <t>Ausgabe(11)</t>
+  </si>
+  <si>
+    <t>Ausgabe(10)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(9)</t>
+  </si>
+  <si>
+    <t>Themen fertig(14)</t>
+  </si>
+  <si>
+    <t>Themen fertig(3)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(6)</t>
+  </si>
+  <si>
+    <t>Review fertig(12)</t>
+  </si>
+  <si>
+    <t>Review fertig(1)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(5)</t>
+  </si>
+  <si>
+    <t>Ausgabe(9)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(13)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(2)</t>
+  </si>
+  <si>
+    <t>Ausgabe(5)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(12)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(1)</t>
+  </si>
+  <si>
+    <t>Themen fertig(8)</t>
+  </si>
+  <si>
+    <t>Review fertig(6)</t>
+  </si>
+  <si>
+    <t>Ausgabe(12)</t>
+  </si>
+  <si>
+    <t>Ausgabe(1)</t>
+  </si>
+  <si>
+    <t>Themen fertig(4)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(7)</t>
+  </si>
+  <si>
+    <t>Review fertig(13)</t>
+  </si>
+  <si>
+    <t>Review fertig(2)</t>
+  </si>
+  <si>
+    <t>Endfassung fertig(6)</t>
+  </si>
+  <si>
+    <t>Themen fertig(11)</t>
+  </si>
+  <si>
+    <t>Entwurf fertig(14)</t>
+  </si>
+  <si>
+    <t>Review fertig(14)</t>
   </si>
 </sst>
 </file>
@@ -783,7 +778,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -812,16 +807,16 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1133,7 +1128,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1166,7 +1161,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1174,7 +1169,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1326,7 +1321,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1382,15 +1377,16 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="9">
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1400,10 +1396,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C6500"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
@@ -1413,10 +1410,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
@@ -1426,10 +1424,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1439,10 +1438,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C6500"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
@@ -1452,10 +1452,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
@@ -1465,10 +1466,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1478,10 +1480,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -1491,170 +1494,15 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1730,7 +1578,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="G13 I31"/>
+      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="C13 I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1744,6 +1592,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="0"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -2663,7 +2512,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2679,7 +2528,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="G13 D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="C13 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2889,9 +2738,11 @@
         <f aca="false">VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>2:1-19</v>
       </c>
-      <c r="R4" s="0" t="e">
+      <c r="R4" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S4" s="0" t="n">
         <f aca="false">MAX(M4:O4)</f>
@@ -2959,9 +2810,11 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:1-49</v>
       </c>
-      <c r="R5" s="0" t="e">
+      <c r="R5" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">MAX(M5:O5)</f>
@@ -3026,9 +2879,11 @@
         <f aca="false">VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:49-Ende; 5:1-12</v>
       </c>
-      <c r="R6" s="0" t="e">
+      <c r="R6" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S6" s="0" t="n">
         <f aca="false">MAX(M6:O6)</f>
@@ -3093,9 +2948,11 @@
         <f aca="false">VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>6:1-6:39</v>
       </c>
-      <c r="R7" s="0" t="e">
+      <c r="R7" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S7" s="0" t="n">
         <f aca="false">MAX(M7:O7)</f>
@@ -3230,9 +3087,11 @@
         <f aca="false">VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>8:35-75</v>
       </c>
-      <c r="R9" s="0" t="e">
+      <c r="R9" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S9" s="0" t="n">
         <f aca="false">MAX(M9:O9)</f>
@@ -3367,9 +3226,11 @@
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>10 bis Ende; 11</v>
       </c>
-      <c r="R11" s="0" t="e">
+      <c r="R11" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S11" s="0" t="n">
         <f aca="false">MAX(M11:N11)</f>
@@ -3504,9 +3365,11 @@
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>14: Virtualenvwrapper</v>
       </c>
-      <c r="R13" s="0" t="e">
+      <c r="R13" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">MAX(M13:O13)</f>
@@ -3757,7 +3620,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3773,7 +3636,7 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="1" sqref="G13 F13"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="1" sqref="C13 F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3991,9 +3854,11 @@
         <f aca="false">VLOOKUP(N4,vorlesung!$A$4:$H$33,8,0)</f>
         <v>2:20-Ende; 3 komplett</v>
       </c>
-      <c r="R4" s="0" t="e">
+      <c r="R4" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O4,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U4" s="0" t="n">
         <f aca="false">MAX(M4:O4)&lt;=MAX(PUE!M4:O4)</f>
@@ -4059,9 +3924,11 @@
         <f aca="false">VLOOKUP(N5,vorlesung!$A$4:$H$33,8,0)</f>
         <v>4:1-49</v>
       </c>
-      <c r="R5" s="0" t="e">
+      <c r="R5" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O5,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">MAX(M5:O5)&lt;=MAX(PUE!M5:O5)</f>
@@ -4127,9 +3994,11 @@
         <f aca="false">VLOOKUP(N6,vorlesung!$A$4:$H$33,8,0)</f>
         <v>5:12-Ende</v>
       </c>
-      <c r="R6" s="0" t="e">
+      <c r="R6" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O6,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">MAX(M6:O6)&lt;=MAX(PUE!M6:O6)</f>
@@ -4195,9 +4064,11 @@
         <f aca="false">VLOOKUP(N7,vorlesung!$A$4:$H$33,8,0)</f>
         <v>6:39-6:53</v>
       </c>
-      <c r="R7" s="0" t="e">
+      <c r="R7" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O7,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U7" s="0" t="n">
         <f aca="false">MAX(M7:O7)&lt;=MAX(PUE!M7:O7)</f>
@@ -4263,9 +4134,11 @@
         <f aca="false">VLOOKUP(N8,vorlesung!$A$4:$H$33,8,0)</f>
         <v>7:11-7:60</v>
       </c>
-      <c r="R8" s="0" t="e">
+      <c r="R8" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O8,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U8" s="0" t="n">
         <f aca="false">MAX(M8:O8)&lt;=MAX(PUE!M8:O8)</f>
@@ -4331,9 +4204,11 @@
         <f aca="false">VLOOKUP(N9,vorlesung!$A$4:$H$33,8,0)</f>
         <v>8:35-75</v>
       </c>
-      <c r="R9" s="0" t="e">
+      <c r="R9" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O9,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U9" s="0" t="n">
         <f aca="false">MAX(M9:O9)&lt;=MAX(PUE!M9:O9)</f>
@@ -4470,9 +4345,11 @@
         <f aca="false">VLOOKUP(N11,vorlesung!$A$4:$H$33,8,0)</f>
         <v>10 bis Ende; 11</v>
       </c>
-      <c r="R11" s="0" t="e">
+      <c r="R11" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O11,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U11" s="0" t="n">
         <f aca="false">MAX(M11:O11)&lt;=MAX(PUE!M11:N11)</f>
@@ -4609,9 +4486,11 @@
         <f aca="false">VLOOKUP(N13,vorlesung!$A$4:$H$33,8,0)</f>
         <v>14: Virtualenvwrapper</v>
       </c>
-      <c r="R13" s="0" t="e">
+      <c r="R13" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O13,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U13" s="0" t="n">
         <f aca="false">MAX(M13:O13)&lt;=MAX(PUE!M13:O13)</f>
@@ -4748,9 +4627,11 @@
         <f aca="false">VLOOKUP(N15,vorlesung!$A$4:$H$33,8,0)</f>
         <v>17: Zugriff auf Felder</v>
       </c>
-      <c r="R15" s="0" t="e">
+      <c r="R15" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(O15,vorlesung!$A$4:$H$33,8,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="U15" s="0" t="n">
         <f aca="false">MAX(M15:O15)&lt;=MAX(PUE!M15:N15)</f>
@@ -4791,7 +4672,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4807,7 +4688,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5004,6 +4885,7 @@
       <c r="A13" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="G13" s="11"/>
       <c r="I13" s="11"/>
@@ -5021,7 +4903,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5037,7 +4919,7 @@
   <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="G13 B21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="C13 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6185,7 +6067,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6201,7 +6083,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="G13 I4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="C13 I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6387,10 +6269,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6403,7 +6285,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="1" sqref="G13 F43"/>
+      <selection pane="topLeft" activeCell="F43" activeCellId="1" sqref="C13 F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7837,7 +7719,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Set grading of HÜ13 to done
</commit_message>
<xml_diff>
--- a/meetings/Termine.xlsx
+++ b/meetings/Termine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vorlesung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1384,7 +1384,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="9">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1502,162 +1502,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1729,15 +1573,15 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="J14:J15 I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.11481481481482"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.11481481481482"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2508,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2679,13 +2523,13 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="J14:J15 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3758,7 +3602,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3773,13 +3617,13 @@
   </sheetPr>
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="1" sqref="J14:J15 F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4792,7 +4636,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4807,13 +4651,13 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5016,7 +4860,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>12</v>
       </c>
@@ -5034,11 +4878,12 @@
       </c>
       <c r="D15" s="11"/>
       <c r="G15" s="11"/>
+      <c r="J15" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5053,13 +4898,13 @@
   </sheetPr>
   <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="J14:J15 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6202,7 +6047,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6217,13 +6062,13 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="J14:J15 I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,10 +6249,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6419,13 +6264,13 @@
   </sheetPr>
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F43" activeCellId="1" sqref="J14:J15 F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7854,7 +7699,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>